<commit_message>
Updated samples and gear
</commit_message>
<xml_diff>
--- a/Sample_and_gear_types_AeN.xlsx
+++ b/Sample_and_gear_types_AeN.xlsx
@@ -8,11 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample_type" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Groups" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sample_type" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_Toc511305932" vbProcedure="false">Sample_type!$G$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_Toc511305933" vbProcedure="false">Sample_type!$G$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_Toc511305932" vbProcedure="false">Sample_type!$G$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_Toc511305933" vbProcedure="false">Sample_type!$G$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,6 +25,42 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="AN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Lena Seuthe:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Jeg forstår ikke helt denne kategorien</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -216,12 +253,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="154">
   <si>
     <t xml:space="preserve">Sample Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Types</t>
   </si>
   <si>
     <t xml:space="preserve">Water</t>
@@ -237,6 +271,421 @@
   </si>
   <si>
     <t xml:space="preserve">Zooplankton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleo/Geology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nekton/ Fish?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phytoplankton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecotox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs to be moved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gear Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bucket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go-Flo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niskin bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice corer 9 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice corer 12 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice corer 14 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice corer 18 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice corer 22 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrobios mini CTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship CTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship water intake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beam trawl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campelen trawl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemini core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Van Veen grab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handnet 20 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multinet 64 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multinet 90µm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Multinet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">180 µm</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MIK-net 1500 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niskin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swim-net 200 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP2 64 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP2 180 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP3 1000 µm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Box corer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment trap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Van veen grab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demersal trawl?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krill trawl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelagic trawl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tucker trawl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baited trap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ammonium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacterial production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trace elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different fish species weight, length, abundance, stomach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurp gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biogenic silica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jelly fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromoform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microzooplankton taxonomy, abundance, biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suction pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small mesozooplankton taxonomy, abunande, biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pore water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deltaO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozooplankton taxonomy, abundance, biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lipids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIC/AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton abundance, weight, taxonomy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOC, TON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dissolved oxygen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton stable isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment grain size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow cytometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA protists/bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxa lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton lipid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benthic foraminifera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density/Abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktic foraminifera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC/TDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice algal taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecotoxicology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment oxygen demand </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diatoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice fauna taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluorescence excitation spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable isotope values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBIs and coccoliths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grazing on bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diet composition as genetic sequence data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sedimentology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meiofauna taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPLC Pigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phaeopigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mRNA /bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic carbon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment geochemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phytoplankton taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mycosporine-like aminoacids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinocysts, ancient DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scavenger taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magnetic susceptibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zooplankton physiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particulate absorption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithological description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zooplankton taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC/PON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists culturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists large volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists small volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA protists/bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment traps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM coccolithophores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viral concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viral production and decay</t>
   </si>
   <si>
     <r>
@@ -284,367 +733,28 @@
     <t xml:space="preserve">Other</t>
   </si>
   <si>
-    <t xml:space="preserve">Microbes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phytoplankton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecotox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammonium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron</t>
-  </si>
-  <si>
     <t xml:space="preserve">CTD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxa lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microzooplankton taxonomy, abundance, biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stable isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacterial production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trace elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Density/Abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small mesozooplankton taxonomy, abunande, biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pore water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lipids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozooplankton taxonomy, abundance, biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen profiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biogenic silica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment oxygen demand </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton abundance, weight, taxonomy?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOC, TON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Different fish species weight, length, abundance, stomach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow cytometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bromoform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stable isotope values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton stable isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment grain size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jelly fish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genetics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diet composition as genetic sequence data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton lipid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benthic foraminifera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handnet 20 µm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deltaO18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorophyll a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planktic foraminifera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice algal taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIC/AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phaeopigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice fauna taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved oxygen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic carbon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diatoms</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozooplankton taxonomy</t>
   </si>
   <si>
-    <t xml:space="preserve">DNA protists/bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBIs and coccoliths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meiofauna taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC/TDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sedimentology</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mesozooplankton taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecotoxicology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dating</t>
   </si>
   <si>
     <t xml:space="preserve">Microplankton taxonomy</t>
   </si>
   <si>
-    <t xml:space="preserve">Fluorescence excitation spectrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phytoplankton taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPLC Pigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment geochemistry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scavenger taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinocysts, ancient DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zooplankton physiology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mRNA /bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">magnetic susceptibility </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zooplankton taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mycosporine-like aminoacids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithological description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XRF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Particulate absorption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POC/PON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists culturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists large volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists small volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA protists/bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salinity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEM coccolithophores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viral concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viral production and decay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grazing on bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment traps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gear Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice corer 22 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydrobios mini CTD</t>
   </si>
   <si>
     <t xml:space="preserve">Bottom trawl</t>
   </si>
   <si>
-    <t xml:space="preserve">Sediment trap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krill trawl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baited trap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bucket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice corer 12 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ship CTD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam trawl</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microplastic net</t>
   </si>
   <si>
-    <t xml:space="preserve">Van veen grab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pelagic trawl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go-Flo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice corer 14 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ship water intake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campelen trawl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIK-net 1500 µm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Box corer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tucker trawl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife</t>
-  </si>
-  <si>
     <t xml:space="preserve">Limnos water sampler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice corer 18 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gemini core</t>
   </si>
   <si>
     <r>
@@ -677,37 +787,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Demersal trawl?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurp gun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niskin bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice corer 9 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Van Veen grab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multinet 90µm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pelagic trawl?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spoon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multinet 64 µm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suction pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swim-net 200 µm</t>
   </si>
   <si>
     <r>
@@ -745,15 +825,6 @@
   <si>
     <t xml:space="preserve">WP2 500 µm</t>
   </si>
-  <si>
-    <t xml:space="preserve">WP2 64 µm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WP3 1000 µm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niskin</t>
-  </si>
 </sst>
 </file>
 
@@ -763,7 +834,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -787,18 +858,69 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -845,30 +967,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -878,35 +978,77 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9999FF"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FF66FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FFCCFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBEBE00"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
-        <bgColor rgb="FF33CCCC"/>
+        <bgColor rgb="FF99FFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD0FFEF"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF66"/>
-        <bgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -915,9 +1057,72 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -953,28 +1158,160 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,63 +1319,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1059,7 +1444,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1072,7 +1457,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFEB9C"/>
       <rgbColor rgb="FFD0FFEF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -1087,18 +1472,18 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFF66"/>
-      <rgbColor rgb="FFFFEB9C"/>
+      <rgbColor rgb="FF99FFFF"/>
+      <rgbColor rgb="FF99FF99"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF66FFFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFBEBE00"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFFC000"/>
-      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -1120,42 +1505,1443 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AP39"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="27.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="21.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="3" width="15.4591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="25.7040816326531"/>
+    <col collapsed="false" hidden="false" max="29" min="21" style="5" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="36" min="34" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="6" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="7" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="8" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="3" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="21" customFormat="true" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="20"/>
+    </row>
+    <row r="2" s="24" customFormat="true" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ2" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP2" s="35"/>
+    </row>
+    <row r="3" s="38" customFormat="true" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="D3" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="37"/>
+      <c r="K3" s="40"/>
+      <c r="O3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="41"/>
+      <c r="AN3" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36"/>
+      <c r="B4" s="42"/>
+      <c r="D4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="40"/>
+      <c r="O4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" s="38" customFormat="true" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36"/>
+      <c r="B5" s="42"/>
+      <c r="D5" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="K5" s="40"/>
+      <c r="O5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="40"/>
+      <c r="Y5" s="40"/>
+      <c r="Z5" s="40"/>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="37"/>
+      <c r="AG5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="41"/>
+      <c r="AN5" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="36"/>
+      <c r="B6" s="42"/>
+      <c r="D6" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="40"/>
+      <c r="O6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="40"/>
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="40"/>
+      <c r="AC6" s="40"/>
+      <c r="AD6" s="37"/>
+      <c r="AG6" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="41"/>
+      <c r="AN6" s="38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36"/>
+      <c r="B7" s="42"/>
+      <c r="D7" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="40"/>
+      <c r="O7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="40"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="37"/>
+      <c r="AE7" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG7" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36"/>
+      <c r="B8" s="42"/>
+      <c r="D8" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="40"/>
+      <c r="O8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="40"/>
+      <c r="Y8" s="40"/>
+      <c r="Z8" s="40"/>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="40"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="37"/>
+      <c r="AE8" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG8" s="37"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="36"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="40"/>
+      <c r="O9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG9" s="37"/>
+      <c r="AK9" s="37"/>
+      <c r="AL9" s="37"/>
+      <c r="AM9" s="41"/>
+      <c r="AN9" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="36"/>
+      <c r="B10" s="42"/>
+      <c r="D10" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="40"/>
+      <c r="O10" s="37"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="45"/>
+      <c r="X10" s="45"/>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="45"/>
+      <c r="AA10" s="45"/>
+      <c r="AB10" s="45"/>
+      <c r="AC10" s="45"/>
+      <c r="AD10" s="44"/>
+      <c r="AE10" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG10" s="37"/>
+      <c r="AK10" s="37"/>
+      <c r="AL10" s="37"/>
+      <c r="AM10" s="41"/>
+    </row>
+    <row r="11" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="36"/>
+      <c r="B11" s="42"/>
+      <c r="D11" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="40"/>
+      <c r="O11" s="37"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="44"/>
+      <c r="AE11" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG11" s="37"/>
+      <c r="AK11" s="37"/>
+      <c r="AL11" s="37"/>
+      <c r="AM11" s="41"/>
+      <c r="AN11" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36"/>
+      <c r="B12" s="42"/>
+      <c r="D12" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="40"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="S12" s="37"/>
+      <c r="T12" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="45"/>
+      <c r="AB12" s="45"/>
+      <c r="AC12" s="45"/>
+      <c r="AD12" s="44"/>
+      <c r="AE12" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG12" s="37"/>
+      <c r="AK12" s="37"/>
+      <c r="AL12" s="37"/>
+      <c r="AM12" s="41"/>
+      <c r="AN12" s="38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36"/>
+      <c r="B13" s="42"/>
+      <c r="D13" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="40"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="S13" s="37"/>
+      <c r="T13" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
+      <c r="Z13" s="40"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="40"/>
+      <c r="AC13" s="40"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG13" s="37"/>
+      <c r="AK13" s="37"/>
+      <c r="AL13" s="37"/>
+      <c r="AM13" s="41"/>
+      <c r="AN13" s="38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" s="38" customFormat="true" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36"/>
+      <c r="B14" s="42"/>
+      <c r="D14" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="40"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="37"/>
+      <c r="T14" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="40"/>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="40"/>
+      <c r="AC14" s="40"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG14" s="37"/>
+      <c r="AK14" s="37"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="41"/>
+      <c r="AN14" s="38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="36"/>
+      <c r="B15" s="42"/>
+      <c r="D15" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="40"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="S15" s="37"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="37"/>
+      <c r="AE15" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG15" s="37"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="37"/>
+      <c r="AM15" s="41"/>
+      <c r="AN15" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="36"/>
+      <c r="B16" s="42"/>
+      <c r="D16" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="40"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="S16" s="37"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
+      <c r="W16" s="40"/>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="40"/>
+      <c r="Z16" s="40"/>
+      <c r="AA16" s="40"/>
+      <c r="AB16" s="40"/>
+      <c r="AC16" s="40"/>
+      <c r="AD16" s="37"/>
+      <c r="AE16" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG16" s="37"/>
+      <c r="AK16" s="37"/>
+      <c r="AL16" s="37"/>
+      <c r="AM16" s="41"/>
+    </row>
+    <row r="17" s="38" customFormat="true" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="36"/>
+      <c r="B17" s="42"/>
+      <c r="D17" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="40"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="S17" s="37"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="40"/>
+      <c r="Z17" s="40"/>
+      <c r="AA17" s="40"/>
+      <c r="AB17" s="40"/>
+      <c r="AC17" s="40"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG17" s="37"/>
+      <c r="AK17" s="37"/>
+      <c r="AL17" s="37"/>
+      <c r="AM17" s="41"/>
+      <c r="AN17" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="36"/>
+      <c r="B18" s="42"/>
+      <c r="D18" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="40"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="S18" s="37"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="40"/>
+      <c r="AC18" s="40"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG18" s="37"/>
+      <c r="AK18" s="37"/>
+      <c r="AL18" s="37"/>
+      <c r="AM18" s="41"/>
+    </row>
+    <row r="19" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36"/>
+      <c r="B19" s="42"/>
+      <c r="D19" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="40"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="S19" s="37"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="40"/>
+      <c r="AA19" s="40"/>
+      <c r="AB19" s="40"/>
+      <c r="AC19" s="40"/>
+      <c r="AD19" s="37"/>
+      <c r="AE19" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG19" s="37"/>
+      <c r="AK19" s="37"/>
+      <c r="AL19" s="37"/>
+      <c r="AM19" s="41"/>
+    </row>
+    <row r="20" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36"/>
+      <c r="B20" s="42"/>
+      <c r="D20" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="40"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="S20" s="37"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="40"/>
+      <c r="AA20" s="40"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="37"/>
+      <c r="AE20" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG20" s="37"/>
+      <c r="AK20" s="37"/>
+      <c r="AL20" s="37"/>
+      <c r="AM20" s="41"/>
+      <c r="AN20" s="38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="36"/>
+      <c r="B21" s="42"/>
+      <c r="D21" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="40"/>
+      <c r="O21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="40"/>
+      <c r="AA21" s="40"/>
+      <c r="AB21" s="40"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG21" s="37"/>
+      <c r="AK21" s="37"/>
+      <c r="AL21" s="37"/>
+      <c r="AM21" s="41"/>
+      <c r="AN21" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="36"/>
+      <c r="B22" s="42"/>
+      <c r="D22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="40"/>
+      <c r="O22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="40"/>
+      <c r="X22" s="40"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="40"/>
+      <c r="AA22" s="40"/>
+      <c r="AB22" s="40"/>
+      <c r="AC22" s="40"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG22" s="37"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="37"/>
+      <c r="AM22" s="41"/>
+      <c r="AN22" s="38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" s="38" customFormat="true" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="36"/>
+      <c r="B23" s="42"/>
+      <c r="D23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="40"/>
+      <c r="O23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="40"/>
+      <c r="AA23" s="40"/>
+      <c r="AB23" s="40"/>
+      <c r="AC23" s="40"/>
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG23" s="37"/>
+      <c r="AK23" s="37"/>
+      <c r="AL23" s="37"/>
+      <c r="AM23" s="41"/>
+      <c r="AN23" s="38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="36"/>
+      <c r="B24" s="42"/>
+      <c r="D24" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="40"/>
+      <c r="O24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="40"/>
+      <c r="W24" s="40"/>
+      <c r="X24" s="40"/>
+      <c r="Y24" s="40"/>
+      <c r="Z24" s="40"/>
+      <c r="AA24" s="40"/>
+      <c r="AB24" s="40"/>
+      <c r="AC24" s="40"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG24" s="37"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="41"/>
+    </row>
+    <row r="25" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="36"/>
+      <c r="B25" s="42"/>
+      <c r="D25" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="40"/>
+      <c r="O25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="40"/>
+      <c r="X25" s="40"/>
+      <c r="Y25" s="40"/>
+      <c r="Z25" s="40"/>
+      <c r="AA25" s="40"/>
+      <c r="AB25" s="40"/>
+      <c r="AC25" s="40"/>
+      <c r="AD25" s="37"/>
+      <c r="AG25" s="37"/>
+      <c r="AK25" s="37"/>
+      <c r="AL25" s="37"/>
+      <c r="AM25" s="41"/>
+    </row>
+    <row r="26" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="36"/>
+      <c r="B26" s="42"/>
+      <c r="D26" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="40"/>
+      <c r="O26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="40"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="40"/>
+      <c r="Z26" s="40"/>
+      <c r="AA26" s="40"/>
+      <c r="AB26" s="40"/>
+      <c r="AC26" s="40"/>
+      <c r="AD26" s="37"/>
+      <c r="AG26" s="37"/>
+      <c r="AK26" s="37"/>
+      <c r="AL26" s="37"/>
+      <c r="AM26" s="41"/>
+    </row>
+    <row r="27" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="D27" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="40"/>
+      <c r="O27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="40"/>
+      <c r="Z27" s="40"/>
+      <c r="AA27" s="40"/>
+      <c r="AB27" s="40"/>
+      <c r="AC27" s="40"/>
+      <c r="AD27" s="37"/>
+      <c r="AG27" s="37"/>
+      <c r="AK27" s="37"/>
+      <c r="AL27" s="37"/>
+      <c r="AM27" s="41"/>
+    </row>
+    <row r="28" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="D28" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="40"/>
+      <c r="O28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="40"/>
+      <c r="W28" s="40"/>
+      <c r="X28" s="40"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="40"/>
+      <c r="AA28" s="40"/>
+      <c r="AB28" s="40"/>
+      <c r="AC28" s="40"/>
+      <c r="AD28" s="37"/>
+      <c r="AG28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
+      <c r="AM28" s="41"/>
+    </row>
+    <row r="29" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="36"/>
+      <c r="B29" s="42"/>
+      <c r="D29" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="40"/>
+      <c r="O29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="40"/>
+      <c r="AA29" s="40"/>
+      <c r="AB29" s="40"/>
+      <c r="AC29" s="40"/>
+      <c r="AD29" s="37"/>
+      <c r="AG29" s="37"/>
+      <c r="AK29" s="37"/>
+      <c r="AL29" s="37"/>
+      <c r="AM29" s="41"/>
+    </row>
+    <row r="30" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="36"/>
+      <c r="B30" s="42"/>
+      <c r="D30" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="40"/>
+      <c r="O30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
+      <c r="Z30" s="40"/>
+      <c r="AA30" s="40"/>
+      <c r="AB30" s="40"/>
+      <c r="AC30" s="40"/>
+      <c r="AD30" s="37"/>
+      <c r="AG30" s="37"/>
+      <c r="AK30" s="37"/>
+      <c r="AL30" s="37"/>
+      <c r="AM30" s="41"/>
+    </row>
+    <row r="31" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="36"/>
+      <c r="B31" s="42"/>
+      <c r="D31" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="40"/>
+      <c r="O31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="40"/>
+      <c r="AA31" s="40"/>
+      <c r="AB31" s="40"/>
+      <c r="AC31" s="40"/>
+      <c r="AD31" s="37"/>
+      <c r="AG31" s="37"/>
+      <c r="AK31" s="37"/>
+      <c r="AL31" s="37"/>
+      <c r="AM31" s="41"/>
+    </row>
+    <row r="32" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="36"/>
+      <c r="B32" s="42"/>
+      <c r="D32" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="40"/>
+      <c r="O32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="40"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="40"/>
+      <c r="Z32" s="40"/>
+      <c r="AA32" s="40"/>
+      <c r="AB32" s="40"/>
+      <c r="AC32" s="40"/>
+      <c r="AD32" s="37"/>
+      <c r="AG32" s="37"/>
+      <c r="AK32" s="37"/>
+      <c r="AL32" s="37"/>
+      <c r="AM32" s="41"/>
+    </row>
+    <row r="33" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="36"/>
+      <c r="B33" s="42"/>
+      <c r="D33" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="40"/>
+      <c r="O33" s="37"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="40"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="40"/>
+      <c r="AA33" s="40"/>
+      <c r="AB33" s="40"/>
+      <c r="AC33" s="40"/>
+      <c r="AD33" s="37"/>
+      <c r="AG33" s="37"/>
+      <c r="AK33" s="37"/>
+      <c r="AL33" s="37"/>
+      <c r="AM33" s="41"/>
+    </row>
+    <row r="34" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="36"/>
+      <c r="B34" s="42"/>
+      <c r="D34" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="40"/>
+      <c r="O34" s="37"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="40"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="40"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+      <c r="AC34" s="40"/>
+      <c r="AD34" s="37"/>
+      <c r="AG34" s="37"/>
+      <c r="AK34" s="37"/>
+      <c r="AL34" s="37"/>
+      <c r="AM34" s="41"/>
+    </row>
+    <row r="35" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="36"/>
+      <c r="B35" s="42"/>
+      <c r="D35" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="40"/>
+      <c r="O35" s="37"/>
+      <c r="S35" s="37"/>
+      <c r="T35" s="40"/>
+      <c r="U35" s="40"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="40"/>
+      <c r="AA35" s="40"/>
+      <c r="AB35" s="40"/>
+      <c r="AC35" s="40"/>
+      <c r="AD35" s="37"/>
+      <c r="AG35" s="37"/>
+      <c r="AK35" s="37"/>
+      <c r="AL35" s="37"/>
+      <c r="AM35" s="41"/>
+    </row>
+    <row r="36" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="36"/>
+      <c r="B36" s="42"/>
+      <c r="D36" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="40"/>
+      <c r="O36" s="37"/>
+      <c r="S36" s="37"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="40"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
+      <c r="Z36" s="40"/>
+      <c r="AA36" s="40"/>
+      <c r="AB36" s="40"/>
+      <c r="AC36" s="40"/>
+      <c r="AD36" s="37"/>
+      <c r="AG36" s="37"/>
+      <c r="AK36" s="37"/>
+      <c r="AL36" s="37"/>
+      <c r="AM36" s="41"/>
+    </row>
+    <row r="37" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="36"/>
+      <c r="B37" s="42"/>
+      <c r="D37" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="40"/>
+      <c r="O37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="40"/>
+      <c r="U37" s="40"/>
+      <c r="V37" s="40"/>
+      <c r="W37" s="40"/>
+      <c r="X37" s="40"/>
+      <c r="Y37" s="40"/>
+      <c r="Z37" s="40"/>
+      <c r="AA37" s="40"/>
+      <c r="AB37" s="40"/>
+      <c r="AC37" s="40"/>
+      <c r="AD37" s="37"/>
+      <c r="AG37" s="37"/>
+      <c r="AK37" s="37"/>
+      <c r="AL37" s="37"/>
+      <c r="AM37" s="41"/>
+    </row>
+    <row r="38" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="36"/>
+      <c r="B38" s="42"/>
+      <c r="D38" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="40"/>
+      <c r="O38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="40"/>
+      <c r="U38" s="40"/>
+      <c r="V38" s="40"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="40"/>
+      <c r="Y38" s="40"/>
+      <c r="Z38" s="40"/>
+      <c r="AA38" s="40"/>
+      <c r="AB38" s="40"/>
+      <c r="AC38" s="40"/>
+      <c r="AD38" s="37"/>
+      <c r="AG38" s="37"/>
+      <c r="AK38" s="37"/>
+      <c r="AL38" s="37"/>
+      <c r="AM38" s="41"/>
+    </row>
+    <row r="39" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="36"/>
+      <c r="B39" s="42"/>
+      <c r="D39" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="40"/>
+      <c r="O39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="40"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="40"/>
+      <c r="AA39" s="40"/>
+      <c r="AB39" s="40"/>
+      <c r="AC39" s="40"/>
+      <c r="AD39" s="37"/>
+      <c r="AG39" s="37"/>
+      <c r="AK39" s="37"/>
+      <c r="AL39" s="37"/>
+      <c r="AM39" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:AC1"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="A3:A43"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="1:56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="E44" activeCellId="0" sqref="E44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="46" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="46" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="46" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="46" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="46" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="46" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="46" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
@@ -2172,67 +3958,67 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="6" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="51" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
+      <c r="G2" s="49" t="s">
+        <v>138</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
+      <c r="H2" s="49" t="s">
+        <v>139</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="50" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
+      <c r="A3" s="48"/>
+      <c r="B3" s="52" t="s">
+        <v>49</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
+      <c r="C3" s="53" t="s">
+        <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
+      <c r="D3" s="46" t="s">
+        <v>141</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
+      <c r="E3" s="53" t="s">
+        <v>83</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>17</v>
+      <c r="F3" s="54" t="s">
+        <v>63</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>18</v>
+      <c r="G3" s="55" t="s">
+        <v>64</v>
       </c>
       <c r="H3" s="0"/>
-      <c r="I3" s="11" t="s">
-        <v>19</v>
+      <c r="I3" s="56" t="s">
+        <v>70</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
@@ -3251,28 +5037,28 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
+      <c r="A4" s="48"/>
+      <c r="B4" s="46" t="s">
+        <v>52</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
+      <c r="C4" s="53" t="s">
+        <v>53</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>24</v>
+      <c r="E4" s="53" t="s">
+        <v>88</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>25</v>
+      <c r="F4" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>69</v>
       </c>
       <c r="H4" s="0"/>
-      <c r="I4" s="11" t="s">
-        <v>26</v>
+      <c r="I4" s="56" t="s">
+        <v>74</v>
       </c>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
@@ -4291,24 +6077,24 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7" t="s">
-        <v>27</v>
+      <c r="A5" s="48"/>
+      <c r="B5" s="52" t="s">
+        <v>55</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>28</v>
+      <c r="C5" s="53" t="s">
+        <v>56</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
+      <c r="D5" s="46" t="s">
+        <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>30</v>
+      <c r="E5" s="53" t="s">
+        <v>92</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>31</v>
+      <c r="F5" s="54" t="s">
+        <v>72</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>32</v>
+      <c r="G5" s="55" t="s">
+        <v>73</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
@@ -5329,26 +7115,26 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7" t="s">
-        <v>33</v>
+      <c r="A6" s="48"/>
+      <c r="B6" s="52" t="s">
+        <v>59</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
-        <v>34</v>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53" t="s">
+        <v>96</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>35</v>
+      <c r="F6" s="54" t="s">
+        <v>76</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>36</v>
+      <c r="G6" s="55" t="s">
+        <v>77</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>37</v>
+      <c r="H6" s="54" t="s">
+        <v>57</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>38</v>
+      <c r="I6" s="46" t="s">
+        <v>81</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
@@ -6366,27 +8152,27 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7" t="s">
-        <v>39</v>
+    <row r="7" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48"/>
+      <c r="B7" s="52" t="s">
+        <v>62</v>
       </c>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
-      <c r="E7" s="8" t="s">
-        <v>40</v>
+      <c r="E7" s="53" t="s">
+        <v>100</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>41</v>
+      <c r="F7" s="54" t="s">
+        <v>79</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>42</v>
+      <c r="G7" s="54" t="s">
+        <v>80</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>43</v>
+      <c r="H7" s="54" t="s">
+        <v>60</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>44</v>
+      <c r="I7" s="56" t="s">
+        <v>86</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
@@ -7405,26 +9191,26 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
+      <c r="A8" s="48"/>
+      <c r="B8" s="46" t="s">
+        <v>67</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
-      <c r="E8" s="8" t="s">
-        <v>46</v>
+      <c r="E8" s="53" t="s">
+        <v>103</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>47</v>
+      <c r="F8" s="54" t="s">
+        <v>84</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>48</v>
+      <c r="G8" s="57" t="s">
+        <v>85</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>49</v>
+      <c r="H8" s="54" t="s">
+        <v>65</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>50</v>
+      <c r="I8" s="46" t="s">
+        <v>30</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -8443,24 +10229,24 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1" t="s">
-        <v>51</v>
+      <c r="A9" s="48"/>
+      <c r="B9" s="46" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
-      <c r="E9" s="8" t="s">
-        <v>52</v>
+      <c r="E9" s="53" t="s">
+        <v>107</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>53</v>
+      <c r="F9" s="54" t="s">
+        <v>89</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>54</v>
+      <c r="G9" s="57" t="s">
+        <v>90</v>
       </c>
       <c r="H9" s="0"/>
-      <c r="I9" s="1" t="s">
-        <v>55</v>
+      <c r="I9" s="46" t="s">
+        <v>94</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
@@ -9479,24 +11265,24 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
+      <c r="A10" s="48"/>
+      <c r="B10" s="46" t="s">
+        <v>75</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
-      <c r="E10" s="8" t="s">
-        <v>57</v>
+      <c r="E10" s="53" t="s">
+        <v>110</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>58</v>
+      <c r="F10" s="58" t="s">
+        <v>93</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>19</v>
+      <c r="G10" s="57" t="s">
+        <v>70</v>
       </c>
       <c r="H10" s="0"/>
-      <c r="I10" s="1" t="s">
-        <v>59</v>
+      <c r="I10" s="46" t="s">
+        <v>98</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -10515,22 +12301,22 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
+      <c r="A11" s="48"/>
+      <c r="B11" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
-      <c r="E11" s="8" t="s">
-        <v>61</v>
+      <c r="E11" s="53" t="s">
+        <v>113</v>
       </c>
       <c r="F11" s="0"/>
-      <c r="G11" s="12" t="s">
-        <v>62</v>
+      <c r="G11" s="57" t="s">
+        <v>97</v>
       </c>
       <c r="H11" s="0"/>
-      <c r="I11" s="1" t="s">
-        <v>63</v>
+      <c r="I11" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -11549,20 +13335,20 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
+      <c r="A12" s="48"/>
+      <c r="B12" s="46" t="s">
+        <v>82</v>
       </c>
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="0"/>
-      <c r="G12" s="12" t="s">
-        <v>65</v>
+      <c r="G12" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="H12" s="0"/>
-      <c r="I12" s="1" t="s">
-        <v>66</v>
+      <c r="I12" s="46" t="s">
+        <v>105</v>
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -12581,20 +14367,20 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>67</v>
+      <c r="A13" s="48"/>
+      <c r="B13" s="46" t="s">
+        <v>91</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="0"/>
-      <c r="G13" s="12" t="s">
-        <v>68</v>
+      <c r="G13" s="57" t="s">
+        <v>104</v>
       </c>
       <c r="H13" s="0"/>
-      <c r="I13" s="1" t="s">
-        <v>69</v>
+      <c r="I13" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -13613,20 +15399,20 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
-        <v>70</v>
+      <c r="A14" s="48"/>
+      <c r="B14" s="46" t="s">
+        <v>95</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="53"/>
       <c r="F14" s="0"/>
-      <c r="G14" s="12" t="s">
-        <v>71</v>
+      <c r="G14" s="57" t="s">
+        <v>108</v>
       </c>
       <c r="H14" s="0"/>
-      <c r="I14" s="1" t="s">
-        <v>72</v>
+      <c r="I14" s="46" t="s">
+        <v>144</v>
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -14645,20 +16431,20 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
-        <v>73</v>
+      <c r="A15" s="48"/>
+      <c r="B15" s="46" t="s">
+        <v>99</v>
       </c>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="0"/>
-      <c r="G15" s="12" t="s">
-        <v>74</v>
+      <c r="G15" s="57" t="s">
+        <v>111</v>
       </c>
       <c r="H15" s="0"/>
-      <c r="I15" s="1" t="s">
-        <v>75</v>
+      <c r="I15" s="46" t="s">
+        <v>115</v>
       </c>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -15677,18 +17463,18 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
-        <v>76</v>
+      <c r="A16" s="48"/>
+      <c r="B16" s="46" t="s">
+        <v>106</v>
       </c>
       <c r="C16" s="0"/>
       <c r="D16" s="0"/>
-      <c r="E16" s="8"/>
-      <c r="G16" s="12" t="s">
-        <v>77</v>
+      <c r="E16" s="53"/>
+      <c r="G16" s="57" t="s">
+        <v>114</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>78</v>
+      <c r="I16" s="46" t="s">
+        <v>118</v>
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -16707,20 +18493,20 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7" t="s">
-        <v>79</v>
+      <c r="A17" s="48"/>
+      <c r="B17" s="52" t="s">
+        <v>109</v>
       </c>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="0"/>
-      <c r="G17" s="12" t="s">
-        <v>80</v>
+      <c r="G17" s="57" t="s">
+        <v>117</v>
       </c>
       <c r="H17" s="0"/>
-      <c r="I17" s="1" t="s">
-        <v>81</v>
+      <c r="I17" s="46" t="s">
+        <v>120</v>
       </c>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -17739,20 +19525,20 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
+      <c r="A18" s="48"/>
+      <c r="B18" s="46" t="s">
+        <v>112</v>
       </c>
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="0"/>
-      <c r="G18" s="12" t="s">
-        <v>83</v>
+      <c r="G18" s="57" t="s">
+        <v>119</v>
       </c>
       <c r="H18" s="0"/>
-      <c r="I18" s="1" t="s">
-        <v>84</v>
+      <c r="I18" s="46" t="s">
+        <v>123</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -18771,16 +20557,16 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7" t="s">
-        <v>85</v>
+      <c r="A19" s="48"/>
+      <c r="B19" s="52" t="s">
+        <v>116</v>
       </c>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
-      <c r="G19" s="12" t="s">
-        <v>86</v>
+      <c r="G19" s="57" t="s">
+        <v>122</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -19801,16 +21587,16 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
+      <c r="A20" s="48"/>
+      <c r="B20" s="46" t="s">
+        <v>56</v>
       </c>
       <c r="C20" s="0"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
-      <c r="G20" s="12" t="s">
-        <v>87</v>
+      <c r="G20" s="57" t="s">
+        <v>124</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -20831,15 +22617,15 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1" t="s">
-        <v>88</v>
+      <c r="A21" s="48"/>
+      <c r="B21" s="46" t="s">
+        <v>121</v>
       </c>
       <c r="C21" s="0"/>
       <c r="D21" s="0"/>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -21859,15 +23645,15 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
+      <c r="A22" s="48"/>
+      <c r="B22" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="C22" s="0"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
       <c r="F22" s="0"/>
-      <c r="G22" s="12"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
@@ -22887,15 +24673,15 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="1" t="s">
-        <v>89</v>
+      <c r="A23" s="48"/>
+      <c r="B23" s="46" t="s">
+        <v>125</v>
       </c>
       <c r="C23" s="0"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
-      <c r="G23" s="12"/>
+      <c r="G23" s="57"/>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
@@ -23915,15 +25701,15 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="1" t="s">
-        <v>90</v>
+      <c r="A24" s="48"/>
+      <c r="B24" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="57"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
@@ -24943,15 +26729,15 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="1" t="s">
-        <v>91</v>
+      <c r="A25" s="48"/>
+      <c r="B25" s="46" t="s">
+        <v>128</v>
       </c>
       <c r="C25" s="0"/>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
-      <c r="G25" s="12"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
@@ -25971,9 +27757,9 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="1" t="s">
-        <v>92</v>
+      <c r="A26" s="48"/>
+      <c r="B26" s="46" t="s">
+        <v>129</v>
       </c>
       <c r="C26" s="0"/>
       <c r="D26" s="0"/>
@@ -26999,9 +28785,9 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="1" t="s">
-        <v>93</v>
+      <c r="A27" s="48"/>
+      <c r="B27" s="46" t="s">
+        <v>130</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" s="0"/>
@@ -28027,9 +29813,9 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="1" t="s">
-        <v>94</v>
+      <c r="A28" s="48"/>
+      <c r="B28" s="46" t="s">
+        <v>131</v>
       </c>
       <c r="C28" s="0"/>
       <c r="D28" s="0"/>
@@ -29055,9 +30841,9 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="14" t="s">
-        <v>95</v>
+      <c r="A29" s="48"/>
+      <c r="B29" s="59" t="s">
+        <v>132</v>
       </c>
       <c r="C29" s="0"/>
       <c r="D29" s="0"/>
@@ -30083,9 +31869,9 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="1" t="s">
-        <v>96</v>
+      <c r="A30" s="48"/>
+      <c r="B30" s="46" t="s">
+        <v>134</v>
       </c>
       <c r="C30" s="0"/>
       <c r="D30" s="0"/>
@@ -31111,9 +32897,9 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1" t="s">
-        <v>97</v>
+      <c r="A31" s="48"/>
+      <c r="B31" s="46" t="s">
+        <v>135</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="0"/>
@@ -32139,9 +33925,9 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1" t="s">
-        <v>21</v>
+      <c r="A32" s="48"/>
+      <c r="B32" s="46" t="s">
+        <v>53</v>
       </c>
       <c r="C32" s="0"/>
       <c r="D32" s="0"/>
@@ -33167,9 +34953,9 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1" t="s">
-        <v>98</v>
+      <c r="A33" s="48"/>
+      <c r="B33" s="46" t="s">
+        <v>136</v>
       </c>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
@@ -34195,9 +35981,9 @@
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
-      <c r="B34" s="1" t="s">
-        <v>99</v>
+      <c r="A34" s="48"/>
+      <c r="B34" s="46" t="s">
+        <v>137</v>
       </c>
       <c r="C34" s="0"/>
       <c r="D34" s="0"/>
@@ -35223,9 +37009,9 @@
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1" t="s">
-        <v>87</v>
+      <c r="A35" s="48"/>
+      <c r="B35" s="46" t="s">
+        <v>124</v>
       </c>
       <c r="C35" s="0"/>
       <c r="D35" s="0"/>
@@ -36251,9 +38037,9 @@
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-      <c r="B36" s="14" t="s">
-        <v>100</v>
+      <c r="A36" s="48"/>
+      <c r="B36" s="59" t="s">
+        <v>127</v>
       </c>
       <c r="C36" s="0"/>
       <c r="D36" s="0"/>
@@ -37279,9 +39065,9 @@
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-      <c r="B37" s="14" t="s">
-        <v>101</v>
+      <c r="A37" s="48"/>
+      <c r="B37" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="C37" s="0"/>
       <c r="D37" s="0"/>
@@ -38307,8 +40093,8 @@
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3"/>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="48"/>
+      <c r="B38" s="59" t="s">
         <v>102</v>
       </c>
       <c r="C38" s="0"/>
@@ -39335,9 +41121,9 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3"/>
-      <c r="B39" s="14" t="s">
-        <v>103</v>
+      <c r="A39" s="48"/>
+      <c r="B39" s="59" t="s">
+        <v>133</v>
       </c>
       <c r="C39" s="0"/>
       <c r="D39" s="0"/>
@@ -40363,9 +42149,9 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3"/>
-      <c r="B40" s="14" t="s">
-        <v>21</v>
+      <c r="A40" s="48"/>
+      <c r="B40" s="59" t="s">
+        <v>53</v>
       </c>
       <c r="C40" s="0"/>
       <c r="D40" s="0"/>
@@ -41391,10 +43177,10 @@
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3"/>
+      <c r="A41" s="48"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
@@ -41405,201 +43191,201 @@
       <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
-        <v>104</v>
+      <c r="A43" s="60" t="s">
+        <v>12</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15"/>
-      <c r="B44" s="11" t="s">
-        <v>105</v>
+      <c r="A44" s="60"/>
+      <c r="B44" s="56" t="s">
+        <v>145</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>106</v>
+      <c r="C44" s="63" t="s">
+        <v>20</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>107</v>
+      <c r="D44" s="63" t="s">
+        <v>22</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>108</v>
+      <c r="E44" s="63" t="s">
+        <v>146</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>50</v>
+      <c r="F44" s="56" t="s">
+        <v>30</v>
       </c>
-      <c r="G44" s="11" t="s">
-        <v>109</v>
+      <c r="G44" s="56" t="s">
+        <v>41</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>110</v>
+      <c r="H44" s="63" t="s">
+        <v>44</v>
       </c>
-      <c r="I44" s="11" t="s">
-        <v>111</v>
+      <c r="I44" s="56" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15"/>
-      <c r="B45" s="11" t="s">
-        <v>112</v>
+      <c r="A45" s="60"/>
+      <c r="B45" s="56" t="s">
+        <v>13</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>113</v>
+      <c r="C45" s="56" t="s">
+        <v>17</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>114</v>
+      <c r="D45" s="56" t="s">
+        <v>24</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>115</v>
+      <c r="E45" s="54" t="s">
+        <v>26</v>
       </c>
-      <c r="F45" s="18" t="s">
-        <v>116</v>
+      <c r="F45" s="63" t="s">
+        <v>147</v>
       </c>
-      <c r="G45" s="11" t="s">
-        <v>117</v>
+      <c r="G45" s="56" t="s">
+        <v>42</v>
       </c>
-      <c r="H45" s="18" t="s">
-        <v>118</v>
+      <c r="H45" s="63" t="s">
+        <v>45</v>
       </c>
-      <c r="I45" s="11" t="s">
-        <v>119</v>
+      <c r="I45" s="56" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15"/>
-      <c r="B46" s="11" t="s">
-        <v>120</v>
+      <c r="A46" s="60"/>
+      <c r="B46" s="56" t="s">
+        <v>14</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>121</v>
+      <c r="C46" s="56" t="s">
+        <v>18</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>122</v>
+      <c r="D46" s="56" t="s">
+        <v>25</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>123</v>
+      <c r="E46" s="54" t="s">
+        <v>27</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>124</v>
+      <c r="F46" s="56" t="s">
+        <v>34</v>
       </c>
-      <c r="G46" s="8" t="s">
-        <v>125</v>
+      <c r="G46" s="53" t="s">
+        <v>40</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>126</v>
+      <c r="H46" s="56" t="s">
+        <v>46</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>127</v>
+      <c r="I46" s="56" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15"/>
-      <c r="B47" s="11" t="s">
-        <v>128</v>
+      <c r="A47" s="60"/>
+      <c r="B47" s="56" t="s">
+        <v>148</v>
       </c>
-      <c r="C47" s="18" t="s">
-        <v>129</v>
+      <c r="C47" s="63" t="s">
+        <v>19</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>130</v>
+      <c r="E47" s="53" t="s">
+        <v>28</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>131</v>
+      <c r="F47" s="56" t="s">
+        <v>149</v>
       </c>
       <c r="G47" s="0"/>
-      <c r="H47" s="9" t="s">
-        <v>132</v>
+      <c r="H47" s="54" t="s">
+        <v>43</v>
       </c>
-      <c r="I47" s="11" t="s">
-        <v>133</v>
+      <c r="I47" s="56" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15"/>
-      <c r="B48" s="11" t="s">
-        <v>134</v>
+      <c r="A48" s="60"/>
+      <c r="B48" s="56" t="s">
+        <v>15</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>135</v>
+      <c r="C48" s="56" t="s">
+        <v>16</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>136</v>
+      <c r="E48" s="53" t="s">
+        <v>29</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>137</v>
+      <c r="F48" s="53" t="s">
+        <v>32</v>
       </c>
       <c r="G48" s="0"/>
-      <c r="H48" s="9" t="s">
-        <v>138</v>
+      <c r="H48" s="54" t="s">
+        <v>150</v>
       </c>
-      <c r="I48" s="11" t="s">
-        <v>139</v>
+      <c r="I48" s="56" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15"/>
+      <c r="A49" s="60"/>
       <c r="E49" s="0"/>
-      <c r="F49" s="11" t="s">
-        <v>140</v>
+      <c r="F49" s="56" t="s">
+        <v>31</v>
       </c>
       <c r="G49" s="0"/>
-      <c r="I49" s="11" t="s">
-        <v>141</v>
+      <c r="I49" s="56" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="0"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="11" t="s">
-        <v>142</v>
+      <c r="E50" s="53"/>
+      <c r="F50" s="56" t="s">
+        <v>36</v>
       </c>
-      <c r="G50" s="11"/>
+      <c r="G50" s="56"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="11" t="s">
-        <v>143</v>
+      <c r="A51" s="60"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="56" t="s">
+        <v>151</v>
       </c>
-      <c r="G51" s="11"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="15"/>
-      <c r="F52" s="19" t="s">
-        <v>144</v>
+      <c r="A52" s="60"/>
+      <c r="F52" s="64" t="s">
+        <v>152</v>
       </c>
-      <c r="G52" s="11"/>
+      <c r="G52" s="56"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15"/>
+      <c r="A53" s="60"/>
       <c r="B53" s="0"/>
-      <c r="F53" s="19" t="s">
-        <v>145</v>
+      <c r="F53" s="64" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15"/>
-      <c r="F54" s="20" t="s">
-        <v>146</v>
+      <c r="A54" s="60"/>
+      <c r="F54" s="65" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="15"/>
-      <c r="F55" s="11" t="s">
-        <v>147</v>
+      <c r="A55" s="60"/>
+      <c r="F55" s="56" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15"/>
-      <c r="F56" s="8" t="s">
-        <v>148</v>
+      <c r="A56" s="60"/>
+      <c r="F56" s="53" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated sample and gear types with number for subsample
</commit_message>
<xml_diff>
--- a/Sample_and_gear_types_AeN.xlsx
+++ b/Sample_and_gear_types_AeN.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="255">
   <si>
     <t xml:space="preserve">Sample Group</t>
   </si>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">Baited trap</t>
   </si>
   <si>
-    <t xml:space="preserve">Lengtd</t>
+    <t xml:space="preserve">Length</t>
   </si>
   <si>
     <t xml:space="preserve">Long_name</t>
@@ -322,12 +322,18 @@
     <t xml:space="preserve">Bacterial prod</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Ice core section</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ice core section</t>
   </si>
   <si>
     <t xml:space="preserve">Density/Abundance</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Algal pigments</t>
+  </si>
+  <si>
     <t xml:space="preserve">Algal pigments</t>
   </si>
   <si>
@@ -370,9 +376,15 @@
     <t xml:space="preserve">Barium</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Bacterial production</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biomass</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Barcoding samples</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barcoding samples</t>
   </si>
   <si>
@@ -406,6 +418,12 @@
     <t xml:space="preserve">Biogenic silica</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Food web samples</t>
+  </si>
+  <si>
     <t xml:space="preserve">Food web samples</t>
   </si>
   <si>
@@ -433,10 +451,13 @@
     <t xml:space="preserve">Bromoform</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Iron</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iron</t>
   </si>
   <si>
-    <t xml:space="preserve">Foraminifera experiment</t>
+    <t xml:space="preserve">1,Foraminifera experiment</t>
   </si>
   <si>
     <t xml:space="preserve">Foraminifera exp</t>
@@ -460,6 +481,12 @@
     <t xml:space="preserve">C-DOM</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Microalgal culturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Microbes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Microbes</t>
   </si>
   <si>
@@ -481,235 +508,265 @@
     <t xml:space="preserve">Meiofauna taxonomy</t>
   </si>
   <si>
+    <t xml:space="preserve">1, PicoNanoEpifluorenscens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PicoNanoEpifluo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Organic carbon/nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic C/N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton stable isotope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop isotope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinocysts, ancient DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scavenger taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deltaO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, PicoNanoFlowcytometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PicoNanoFlowcyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBIs and coccoliths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurp gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIC/AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Primary production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Pore water content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pore water content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithological description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA protists/bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA protists/bact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Prokaryote DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prokaryote DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Quantitative macrofauna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti macrofauna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton gonad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop gonad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">magnetic susceptibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Respiration experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiration exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suction pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC/DON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Sediment stable isotopes, carbon and nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sed isotopes, C, N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoop physiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecotoxicology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist microscopy &lt;  um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists micros&lt;10um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktic foraminifera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoop taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluorescence excitation spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluo ex spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ,Protist microscopy &gt; 10 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pore water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grazing on bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPLC Pigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Silicate incorporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicate incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment geochemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Virus DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virus DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoplankton stomach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozop stomach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment grain size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sedimentology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mycosporine-like aminoacids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mycosporine amin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOC, TON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particulate absorption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Particulate abs</t>
+  </si>
+  <si>
     <t xml:space="preserve">PicoNanoEpifluorenscens</t>
   </si>
   <si>
-    <t xml:space="preserve">PicoNanoEpifluo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic carbon/nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic C/N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton stable isotope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop isotope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinocysts, ancient DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scavenger taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deltaO18</t>
-  </si>
-  <si>
     <t xml:space="preserve">PicoNanoFlowcytometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PicoNanoFlowcyt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBIs and coccoliths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurp gun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIC/AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pore water content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithological description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spoon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA protists/bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA protists/bact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prokaryote DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantitative macrofauna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti macrofauna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton gonad </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop gonad </t>
-  </si>
-  <si>
-    <t xml:space="preserve">magnetic susceptibility </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stable isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prokaryote RNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respiration experiments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respiration exp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop hg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen profiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suction pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC/DON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment stable isotopes, carbon and nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sed isotopes, C, N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoop physiology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecotoxicology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist microscopy &lt;  um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists micros&lt;10um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton nutrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planktic foraminifera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoop taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluorescence excitation spectrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluo ex spec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist microscopy &gt; 10 um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop nutrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pore water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grazing on bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPLC Pigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicate incorporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicate incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment geochemistry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virus DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoplankton stomach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozop stomach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment grain size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sedimentology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mycosporine-like aminoacids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mycosporine amin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOC, TON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XRF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Particulate absorption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Particulate abs</t>
   </si>
   <si>
     <t xml:space="preserve">PicoNanoImagingFlow</t>
@@ -1387,11 +1444,11 @@
       <xdr:col>58</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>355320</xdr:rowOff>
+      <xdr:rowOff>355680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
@@ -1402,8 +1459,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60300720" y="4919400"/>
-          <a:ext cx="3168360" cy="430560"/>
+          <a:off x="59340600" y="4919760"/>
+          <a:ext cx="3118680" cy="430200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1434,7 +1491,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
@@ -1445,8 +1502,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60300720" y="5300280"/>
-          <a:ext cx="3168360" cy="430560"/>
+          <a:off x="59340600" y="5300280"/>
+          <a:ext cx="3118680" cy="1360800"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1471,9 +1528,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>356400</xdr:rowOff>
+      <xdr:rowOff>356760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
@@ -1488,8 +1545,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="74666880" y="3399120"/>
-          <a:ext cx="4194720" cy="429840"/>
+          <a:off x="73476000" y="3399480"/>
+          <a:ext cx="4128120" cy="429480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1514,9 +1571,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>355680</xdr:rowOff>
+      <xdr:rowOff>356040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
@@ -1531,8 +1588,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="74666880" y="4159080"/>
-          <a:ext cx="4194720" cy="430560"/>
+          <a:off x="73476000" y="4159440"/>
+          <a:ext cx="4128120" cy="430200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1557,7 +1614,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>355680</xdr:rowOff>
     </xdr:from>
@@ -1565,7 +1622,7 @@
       <xdr:col>76</xdr:col>
       <xdr:colOff>90000</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1574,8 +1631,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="74666880" y="4539600"/>
-          <a:ext cx="4194720" cy="430200"/>
+          <a:off x="73476000" y="4539600"/>
+          <a:ext cx="4128120" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1600,15 +1657,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>355680</xdr:rowOff>
+      <xdr:rowOff>356040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
       <xdr:colOff>90000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1617,8 +1674,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="74666880" y="5680440"/>
-          <a:ext cx="4194720" cy="430560"/>
+          <a:off x="73476000" y="5680800"/>
+          <a:ext cx="4128120" cy="1360080"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1643,9 +1700,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>355680</xdr:rowOff>
+      <xdr:rowOff>356040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
@@ -1660,8 +1717,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="74666880" y="6821640"/>
-          <a:ext cx="4194720" cy="430560"/>
+          <a:off x="73476000" y="7752240"/>
+          <a:ext cx="4128120" cy="430200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1691,43 +1748,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:DR83"/>
+  <dimension ref="1:83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM15" activeCellId="0" sqref="BM15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="8" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="5" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="25" min="22" style="5" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="33" min="26" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="43" min="36" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="71" min="46" style="5" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="73" min="72" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="77" min="74" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="79" min="78" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="82" min="80" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="86" min="84" style="2" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="87" min="87" style="5" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="90" min="88" style="6" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="7" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="92" min="92" style="8" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="9" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="4" width="14.5408163265306"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="4" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="10" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="97" style="4" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="8" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="5" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="25" min="22" style="5" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="33" min="26" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="43" min="36" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="71" min="46" style="5" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="73" min="72" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="77" min="74" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="79" min="78" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="82" min="80" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="86" min="84" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="87" min="87" style="5" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="90" min="88" style="6" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="7" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="92" min="92" style="8" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="9" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="4" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="4" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="10" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="97" style="4" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2045,7 +2102,7 @@
       </c>
       <c r="CR2" s="33"/>
     </row>
-    <row r="3" s="32" customFormat="true" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
         <v>59</v>
       </c>
@@ -2326,7 +2383,936 @@
         <v>61</v>
       </c>
       <c r="CP3" s="26"/>
+      <c r="CQ3" s="0"/>
       <c r="CR3" s="33"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
+      <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
+      <c r="IX3" s="0"/>
+      <c r="IY3" s="0"/>
+      <c r="IZ3" s="0"/>
+      <c r="JA3" s="0"/>
+      <c r="JB3" s="0"/>
+      <c r="JC3" s="0"/>
+      <c r="JD3" s="0"/>
+      <c r="JE3" s="0"/>
+      <c r="JF3" s="0"/>
+      <c r="JG3" s="0"/>
+      <c r="JH3" s="0"/>
+      <c r="JI3" s="0"/>
+      <c r="JJ3" s="0"/>
+      <c r="JK3" s="0"/>
+      <c r="JL3" s="0"/>
+      <c r="JM3" s="0"/>
+      <c r="JN3" s="0"/>
+      <c r="JO3" s="0"/>
+      <c r="JP3" s="0"/>
+      <c r="JQ3" s="0"/>
+      <c r="JR3" s="0"/>
+      <c r="JS3" s="0"/>
+      <c r="JT3" s="0"/>
+      <c r="JU3" s="0"/>
+      <c r="JV3" s="0"/>
+      <c r="JW3" s="0"/>
+      <c r="JX3" s="0"/>
+      <c r="JY3" s="0"/>
+      <c r="JZ3" s="0"/>
+      <c r="KA3" s="0"/>
+      <c r="KB3" s="0"/>
+      <c r="KC3" s="0"/>
+      <c r="KD3" s="0"/>
+      <c r="KE3" s="0"/>
+      <c r="KF3" s="0"/>
+      <c r="KG3" s="0"/>
+      <c r="KH3" s="0"/>
+      <c r="KI3" s="0"/>
+      <c r="KJ3" s="0"/>
+      <c r="KK3" s="0"/>
+      <c r="KL3" s="0"/>
+      <c r="KM3" s="0"/>
+      <c r="KN3" s="0"/>
+      <c r="KO3" s="0"/>
+      <c r="KP3" s="0"/>
+      <c r="KQ3" s="0"/>
+      <c r="KR3" s="0"/>
+      <c r="KS3" s="0"/>
+      <c r="KT3" s="0"/>
+      <c r="KU3" s="0"/>
+      <c r="KV3" s="0"/>
+      <c r="KW3" s="0"/>
+      <c r="KX3" s="0"/>
+      <c r="KY3" s="0"/>
+      <c r="KZ3" s="0"/>
+      <c r="LA3" s="0"/>
+      <c r="LB3" s="0"/>
+      <c r="LC3" s="0"/>
+      <c r="LD3" s="0"/>
+      <c r="LE3" s="0"/>
+      <c r="LF3" s="0"/>
+      <c r="LG3" s="0"/>
+      <c r="LH3" s="0"/>
+      <c r="LI3" s="0"/>
+      <c r="LJ3" s="0"/>
+      <c r="LK3" s="0"/>
+      <c r="LL3" s="0"/>
+      <c r="LM3" s="0"/>
+      <c r="LN3" s="0"/>
+      <c r="LO3" s="0"/>
+      <c r="LP3" s="0"/>
+      <c r="LQ3" s="0"/>
+      <c r="LR3" s="0"/>
+      <c r="LS3" s="0"/>
+      <c r="LT3" s="0"/>
+      <c r="LU3" s="0"/>
+      <c r="LV3" s="0"/>
+      <c r="LW3" s="0"/>
+      <c r="LX3" s="0"/>
+      <c r="LY3" s="0"/>
+      <c r="LZ3" s="0"/>
+      <c r="MA3" s="0"/>
+      <c r="MB3" s="0"/>
+      <c r="MC3" s="0"/>
+      <c r="MD3" s="0"/>
+      <c r="ME3" s="0"/>
+      <c r="MF3" s="0"/>
+      <c r="MG3" s="0"/>
+      <c r="MH3" s="0"/>
+      <c r="MI3" s="0"/>
+      <c r="MJ3" s="0"/>
+      <c r="MK3" s="0"/>
+      <c r="ML3" s="0"/>
+      <c r="MM3" s="0"/>
+      <c r="MN3" s="0"/>
+      <c r="MO3" s="0"/>
+      <c r="MP3" s="0"/>
+      <c r="MQ3" s="0"/>
+      <c r="MR3" s="0"/>
+      <c r="MS3" s="0"/>
+      <c r="MT3" s="0"/>
+      <c r="MU3" s="0"/>
+      <c r="MV3" s="0"/>
+      <c r="MW3" s="0"/>
+      <c r="MX3" s="0"/>
+      <c r="MY3" s="0"/>
+      <c r="MZ3" s="0"/>
+      <c r="NA3" s="0"/>
+      <c r="NB3" s="0"/>
+      <c r="NC3" s="0"/>
+      <c r="ND3" s="0"/>
+      <c r="NE3" s="0"/>
+      <c r="NF3" s="0"/>
+      <c r="NG3" s="0"/>
+      <c r="NH3" s="0"/>
+      <c r="NI3" s="0"/>
+      <c r="NJ3" s="0"/>
+      <c r="NK3" s="0"/>
+      <c r="NL3" s="0"/>
+      <c r="NM3" s="0"/>
+      <c r="NN3" s="0"/>
+      <c r="NO3" s="0"/>
+      <c r="NP3" s="0"/>
+      <c r="NQ3" s="0"/>
+      <c r="NR3" s="0"/>
+      <c r="NS3" s="0"/>
+      <c r="NT3" s="0"/>
+      <c r="NU3" s="0"/>
+      <c r="NV3" s="0"/>
+      <c r="NW3" s="0"/>
+      <c r="NX3" s="0"/>
+      <c r="NY3" s="0"/>
+      <c r="NZ3" s="0"/>
+      <c r="OA3" s="0"/>
+      <c r="OB3" s="0"/>
+      <c r="OC3" s="0"/>
+      <c r="OD3" s="0"/>
+      <c r="OE3" s="0"/>
+      <c r="OF3" s="0"/>
+      <c r="OG3" s="0"/>
+      <c r="OH3" s="0"/>
+      <c r="OI3" s="0"/>
+      <c r="OJ3" s="0"/>
+      <c r="OK3" s="0"/>
+      <c r="OL3" s="0"/>
+      <c r="OM3" s="0"/>
+      <c r="ON3" s="0"/>
+      <c r="OO3" s="0"/>
+      <c r="OP3" s="0"/>
+      <c r="OQ3" s="0"/>
+      <c r="OR3" s="0"/>
+      <c r="OS3" s="0"/>
+      <c r="OT3" s="0"/>
+      <c r="OU3" s="0"/>
+      <c r="OV3" s="0"/>
+      <c r="OW3" s="0"/>
+      <c r="OX3" s="0"/>
+      <c r="OY3" s="0"/>
+      <c r="OZ3" s="0"/>
+      <c r="PA3" s="0"/>
+      <c r="PB3" s="0"/>
+      <c r="PC3" s="0"/>
+      <c r="PD3" s="0"/>
+      <c r="PE3" s="0"/>
+      <c r="PF3" s="0"/>
+      <c r="PG3" s="0"/>
+      <c r="PH3" s="0"/>
+      <c r="PI3" s="0"/>
+      <c r="PJ3" s="0"/>
+      <c r="PK3" s="0"/>
+      <c r="PL3" s="0"/>
+      <c r="PM3" s="0"/>
+      <c r="PN3" s="0"/>
+      <c r="PO3" s="0"/>
+      <c r="PP3" s="0"/>
+      <c r="PQ3" s="0"/>
+      <c r="PR3" s="0"/>
+      <c r="PS3" s="0"/>
+      <c r="PT3" s="0"/>
+      <c r="PU3" s="0"/>
+      <c r="PV3" s="0"/>
+      <c r="PW3" s="0"/>
+      <c r="PX3" s="0"/>
+      <c r="PY3" s="0"/>
+      <c r="PZ3" s="0"/>
+      <c r="QA3" s="0"/>
+      <c r="QB3" s="0"/>
+      <c r="QC3" s="0"/>
+      <c r="QD3" s="0"/>
+      <c r="QE3" s="0"/>
+      <c r="QF3" s="0"/>
+      <c r="QG3" s="0"/>
+      <c r="QH3" s="0"/>
+      <c r="QI3" s="0"/>
+      <c r="QJ3" s="0"/>
+      <c r="QK3" s="0"/>
+      <c r="QL3" s="0"/>
+      <c r="QM3" s="0"/>
+      <c r="QN3" s="0"/>
+      <c r="QO3" s="0"/>
+      <c r="QP3" s="0"/>
+      <c r="QQ3" s="0"/>
+      <c r="QR3" s="0"/>
+      <c r="QS3" s="0"/>
+      <c r="QT3" s="0"/>
+      <c r="QU3" s="0"/>
+      <c r="QV3" s="0"/>
+      <c r="QW3" s="0"/>
+      <c r="QX3" s="0"/>
+      <c r="QY3" s="0"/>
+      <c r="QZ3" s="0"/>
+      <c r="RA3" s="0"/>
+      <c r="RB3" s="0"/>
+      <c r="RC3" s="0"/>
+      <c r="RD3" s="0"/>
+      <c r="RE3" s="0"/>
+      <c r="RF3" s="0"/>
+      <c r="RG3" s="0"/>
+      <c r="RH3" s="0"/>
+      <c r="RI3" s="0"/>
+      <c r="RJ3" s="0"/>
+      <c r="RK3" s="0"/>
+      <c r="RL3" s="0"/>
+      <c r="RM3" s="0"/>
+      <c r="RN3" s="0"/>
+      <c r="RO3" s="0"/>
+      <c r="RP3" s="0"/>
+      <c r="RQ3" s="0"/>
+      <c r="RR3" s="0"/>
+      <c r="RS3" s="0"/>
+      <c r="RT3" s="0"/>
+      <c r="RU3" s="0"/>
+      <c r="RV3" s="0"/>
+      <c r="RW3" s="0"/>
+      <c r="RX3" s="0"/>
+      <c r="RY3" s="0"/>
+      <c r="RZ3" s="0"/>
+      <c r="SA3" s="0"/>
+      <c r="SB3" s="0"/>
+      <c r="SC3" s="0"/>
+      <c r="SD3" s="0"/>
+      <c r="SE3" s="0"/>
+      <c r="SF3" s="0"/>
+      <c r="SG3" s="0"/>
+      <c r="SH3" s="0"/>
+      <c r="SI3" s="0"/>
+      <c r="SJ3" s="0"/>
+      <c r="SK3" s="0"/>
+      <c r="SL3" s="0"/>
+      <c r="SM3" s="0"/>
+      <c r="SN3" s="0"/>
+      <c r="SO3" s="0"/>
+      <c r="SP3" s="0"/>
+      <c r="SQ3" s="0"/>
+      <c r="SR3" s="0"/>
+      <c r="SS3" s="0"/>
+      <c r="ST3" s="0"/>
+      <c r="SU3" s="0"/>
+      <c r="SV3" s="0"/>
+      <c r="SW3" s="0"/>
+      <c r="SX3" s="0"/>
+      <c r="SY3" s="0"/>
+      <c r="SZ3" s="0"/>
+      <c r="TA3" s="0"/>
+      <c r="TB3" s="0"/>
+      <c r="TC3" s="0"/>
+      <c r="TD3" s="0"/>
+      <c r="TE3" s="0"/>
+      <c r="TF3" s="0"/>
+      <c r="TG3" s="0"/>
+      <c r="TH3" s="0"/>
+      <c r="TI3" s="0"/>
+      <c r="TJ3" s="0"/>
+      <c r="TK3" s="0"/>
+      <c r="TL3" s="0"/>
+      <c r="TM3" s="0"/>
+      <c r="TN3" s="0"/>
+      <c r="TO3" s="0"/>
+      <c r="TP3" s="0"/>
+      <c r="TQ3" s="0"/>
+      <c r="TR3" s="0"/>
+      <c r="TS3" s="0"/>
+      <c r="TT3" s="0"/>
+      <c r="TU3" s="0"/>
+      <c r="TV3" s="0"/>
+      <c r="TW3" s="0"/>
+      <c r="TX3" s="0"/>
+      <c r="TY3" s="0"/>
+      <c r="TZ3" s="0"/>
+      <c r="UA3" s="0"/>
+      <c r="UB3" s="0"/>
+      <c r="UC3" s="0"/>
+      <c r="UD3" s="0"/>
+      <c r="UE3" s="0"/>
+      <c r="UF3" s="0"/>
+      <c r="UG3" s="0"/>
+      <c r="UH3" s="0"/>
+      <c r="UI3" s="0"/>
+      <c r="UJ3" s="0"/>
+      <c r="UK3" s="0"/>
+      <c r="UL3" s="0"/>
+      <c r="UM3" s="0"/>
+      <c r="UN3" s="0"/>
+      <c r="UO3" s="0"/>
+      <c r="UP3" s="0"/>
+      <c r="UQ3" s="0"/>
+      <c r="UR3" s="0"/>
+      <c r="US3" s="0"/>
+      <c r="UT3" s="0"/>
+      <c r="UU3" s="0"/>
+      <c r="UV3" s="0"/>
+      <c r="UW3" s="0"/>
+      <c r="UX3" s="0"/>
+      <c r="UY3" s="0"/>
+      <c r="UZ3" s="0"/>
+      <c r="VA3" s="0"/>
+      <c r="VB3" s="0"/>
+      <c r="VC3" s="0"/>
+      <c r="VD3" s="0"/>
+      <c r="VE3" s="0"/>
+      <c r="VF3" s="0"/>
+      <c r="VG3" s="0"/>
+      <c r="VH3" s="0"/>
+      <c r="VI3" s="0"/>
+      <c r="VJ3" s="0"/>
+      <c r="VK3" s="0"/>
+      <c r="VL3" s="0"/>
+      <c r="VM3" s="0"/>
+      <c r="VN3" s="0"/>
+      <c r="VO3" s="0"/>
+      <c r="VP3" s="0"/>
+      <c r="VQ3" s="0"/>
+      <c r="VR3" s="0"/>
+      <c r="VS3" s="0"/>
+      <c r="VT3" s="0"/>
+      <c r="VU3" s="0"/>
+      <c r="VV3" s="0"/>
+      <c r="VW3" s="0"/>
+      <c r="VX3" s="0"/>
+      <c r="VY3" s="0"/>
+      <c r="VZ3" s="0"/>
+      <c r="WA3" s="0"/>
+      <c r="WB3" s="0"/>
+      <c r="WC3" s="0"/>
+      <c r="WD3" s="0"/>
+      <c r="WE3" s="0"/>
+      <c r="WF3" s="0"/>
+      <c r="WG3" s="0"/>
+      <c r="WH3" s="0"/>
+      <c r="WI3" s="0"/>
+      <c r="WJ3" s="0"/>
+      <c r="WK3" s="0"/>
+      <c r="WL3" s="0"/>
+      <c r="WM3" s="0"/>
+      <c r="WN3" s="0"/>
+      <c r="WO3" s="0"/>
+      <c r="WP3" s="0"/>
+      <c r="WQ3" s="0"/>
+      <c r="WR3" s="0"/>
+      <c r="WS3" s="0"/>
+      <c r="WT3" s="0"/>
+      <c r="WU3" s="0"/>
+      <c r="WV3" s="0"/>
+      <c r="WW3" s="0"/>
+      <c r="WX3" s="0"/>
+      <c r="WY3" s="0"/>
+      <c r="WZ3" s="0"/>
+      <c r="XA3" s="0"/>
+      <c r="XB3" s="0"/>
+      <c r="XC3" s="0"/>
+      <c r="XD3" s="0"/>
+      <c r="XE3" s="0"/>
+      <c r="XF3" s="0"/>
+      <c r="XG3" s="0"/>
+      <c r="XH3" s="0"/>
+      <c r="XI3" s="0"/>
+      <c r="XJ3" s="0"/>
+      <c r="XK3" s="0"/>
+      <c r="XL3" s="0"/>
+      <c r="XM3" s="0"/>
+      <c r="XN3" s="0"/>
+      <c r="XO3" s="0"/>
+      <c r="XP3" s="0"/>
+      <c r="XQ3" s="0"/>
+      <c r="XR3" s="0"/>
+      <c r="XS3" s="0"/>
+      <c r="XT3" s="0"/>
+      <c r="XU3" s="0"/>
+      <c r="XV3" s="0"/>
+      <c r="XW3" s="0"/>
+      <c r="XX3" s="0"/>
+      <c r="XY3" s="0"/>
+      <c r="XZ3" s="0"/>
+      <c r="YA3" s="0"/>
+      <c r="YB3" s="0"/>
+      <c r="YC3" s="0"/>
+      <c r="YD3" s="0"/>
+      <c r="YE3" s="0"/>
+      <c r="YF3" s="0"/>
+      <c r="YG3" s="0"/>
+      <c r="YH3" s="0"/>
+      <c r="YI3" s="0"/>
+      <c r="YJ3" s="0"/>
+      <c r="YK3" s="0"/>
+      <c r="YL3" s="0"/>
+      <c r="YM3" s="0"/>
+      <c r="YN3" s="0"/>
+      <c r="YO3" s="0"/>
+      <c r="YP3" s="0"/>
+      <c r="YQ3" s="0"/>
+      <c r="YR3" s="0"/>
+      <c r="YS3" s="0"/>
+      <c r="YT3" s="0"/>
+      <c r="YU3" s="0"/>
+      <c r="YV3" s="0"/>
+      <c r="YW3" s="0"/>
+      <c r="YX3" s="0"/>
+      <c r="YY3" s="0"/>
+      <c r="YZ3" s="0"/>
+      <c r="ZA3" s="0"/>
+      <c r="ZB3" s="0"/>
+      <c r="ZC3" s="0"/>
+      <c r="ZD3" s="0"/>
+      <c r="ZE3" s="0"/>
+      <c r="ZF3" s="0"/>
+      <c r="ZG3" s="0"/>
+      <c r="ZH3" s="0"/>
+      <c r="ZI3" s="0"/>
+      <c r="ZJ3" s="0"/>
+      <c r="ZK3" s="0"/>
+      <c r="ZL3" s="0"/>
+      <c r="ZM3" s="0"/>
+      <c r="ZN3" s="0"/>
+      <c r="ZO3" s="0"/>
+      <c r="ZP3" s="0"/>
+      <c r="ZQ3" s="0"/>
+      <c r="ZR3" s="0"/>
+      <c r="ZS3" s="0"/>
+      <c r="ZT3" s="0"/>
+      <c r="ZU3" s="0"/>
+      <c r="ZV3" s="0"/>
+      <c r="ZW3" s="0"/>
+      <c r="ZX3" s="0"/>
+      <c r="ZY3" s="0"/>
+      <c r="ZZ3" s="0"/>
+      <c r="AAA3" s="0"/>
+      <c r="AAB3" s="0"/>
+      <c r="AAC3" s="0"/>
+      <c r="AAD3" s="0"/>
+      <c r="AAE3" s="0"/>
+      <c r="AAF3" s="0"/>
+      <c r="AAG3" s="0"/>
+      <c r="AAH3" s="0"/>
+      <c r="AAI3" s="0"/>
+      <c r="AAJ3" s="0"/>
+      <c r="AAK3" s="0"/>
+      <c r="AAL3" s="0"/>
+      <c r="AAM3" s="0"/>
+      <c r="AAN3" s="0"/>
+      <c r="AAO3" s="0"/>
+      <c r="AAP3" s="0"/>
+      <c r="AAQ3" s="0"/>
+      <c r="AAR3" s="0"/>
+      <c r="AAS3" s="0"/>
+      <c r="AAT3" s="0"/>
+      <c r="AAU3" s="0"/>
+      <c r="AAV3" s="0"/>
+      <c r="AAW3" s="0"/>
+      <c r="AAX3" s="0"/>
+      <c r="AAY3" s="0"/>
+      <c r="AAZ3" s="0"/>
+      <c r="ABA3" s="0"/>
+      <c r="ABB3" s="0"/>
+      <c r="ABC3" s="0"/>
+      <c r="ABD3" s="0"/>
+      <c r="ABE3" s="0"/>
+      <c r="ABF3" s="0"/>
+      <c r="ABG3" s="0"/>
+      <c r="ABH3" s="0"/>
+      <c r="ABI3" s="0"/>
+      <c r="ABJ3" s="0"/>
+      <c r="ABK3" s="0"/>
+      <c r="ABL3" s="0"/>
+      <c r="ABM3" s="0"/>
+      <c r="ABN3" s="0"/>
+      <c r="ABO3" s="0"/>
+      <c r="ABP3" s="0"/>
+      <c r="ABQ3" s="0"/>
+      <c r="ABR3" s="0"/>
+      <c r="ABS3" s="0"/>
+      <c r="ABT3" s="0"/>
+      <c r="ABU3" s="0"/>
+      <c r="ABV3" s="0"/>
+      <c r="ABW3" s="0"/>
+      <c r="ABX3" s="0"/>
+      <c r="ABY3" s="0"/>
+      <c r="ABZ3" s="0"/>
+      <c r="ACA3" s="0"/>
+      <c r="ACB3" s="0"/>
+      <c r="ACC3" s="0"/>
+      <c r="ACD3" s="0"/>
+      <c r="ACE3" s="0"/>
+      <c r="ACF3" s="0"/>
+      <c r="ACG3" s="0"/>
+      <c r="ACH3" s="0"/>
+      <c r="ACI3" s="0"/>
+      <c r="ACJ3" s="0"/>
+      <c r="ACK3" s="0"/>
+      <c r="ACL3" s="0"/>
+      <c r="ACM3" s="0"/>
+      <c r="ACN3" s="0"/>
+      <c r="ACO3" s="0"/>
+      <c r="ACP3" s="0"/>
+      <c r="ACQ3" s="0"/>
+      <c r="ACR3" s="0"/>
+      <c r="ACS3" s="0"/>
+      <c r="ACT3" s="0"/>
+      <c r="ACU3" s="0"/>
+      <c r="ACV3" s="0"/>
+      <c r="ACW3" s="0"/>
+      <c r="ACX3" s="0"/>
+      <c r="ACY3" s="0"/>
+      <c r="ACZ3" s="0"/>
+      <c r="ADA3" s="0"/>
+      <c r="ADB3" s="0"/>
+      <c r="ADC3" s="0"/>
+      <c r="ADD3" s="0"/>
+      <c r="ADE3" s="0"/>
+      <c r="ADF3" s="0"/>
+      <c r="ADG3" s="0"/>
+      <c r="ADH3" s="0"/>
+      <c r="ADI3" s="0"/>
+      <c r="ADJ3" s="0"/>
+      <c r="ADK3" s="0"/>
+      <c r="ADL3" s="0"/>
+      <c r="ADM3" s="0"/>
+      <c r="ADN3" s="0"/>
+      <c r="ADO3" s="0"/>
+      <c r="ADP3" s="0"/>
+      <c r="ADQ3" s="0"/>
+      <c r="ADR3" s="0"/>
+      <c r="ADS3" s="0"/>
+      <c r="ADT3" s="0"/>
+      <c r="ADU3" s="0"/>
+      <c r="ADV3" s="0"/>
+      <c r="ADW3" s="0"/>
+      <c r="ADX3" s="0"/>
+      <c r="ADY3" s="0"/>
+      <c r="ADZ3" s="0"/>
+      <c r="AEA3" s="0"/>
+      <c r="AEB3" s="0"/>
+      <c r="AEC3" s="0"/>
+      <c r="AED3" s="0"/>
+      <c r="AEE3" s="0"/>
+      <c r="AEF3" s="0"/>
+      <c r="AEG3" s="0"/>
+      <c r="AEH3" s="0"/>
+      <c r="AEI3" s="0"/>
+      <c r="AEJ3" s="0"/>
+      <c r="AEK3" s="0"/>
+      <c r="AEL3" s="0"/>
+      <c r="AEM3" s="0"/>
+      <c r="AEN3" s="0"/>
+      <c r="AEO3" s="0"/>
+      <c r="AEP3" s="0"/>
+      <c r="AEQ3" s="0"/>
+      <c r="AER3" s="0"/>
+      <c r="AES3" s="0"/>
+      <c r="AET3" s="0"/>
+      <c r="AEU3" s="0"/>
+      <c r="AEV3" s="0"/>
+      <c r="AEW3" s="0"/>
+      <c r="AEX3" s="0"/>
+      <c r="AEY3" s="0"/>
+      <c r="AEZ3" s="0"/>
+      <c r="AFA3" s="0"/>
+      <c r="AFB3" s="0"/>
+      <c r="AFC3" s="0"/>
+      <c r="AFD3" s="0"/>
+      <c r="AFE3" s="0"/>
+      <c r="AFF3" s="0"/>
+      <c r="AFG3" s="0"/>
+      <c r="AFH3" s="0"/>
+      <c r="AFI3" s="0"/>
+      <c r="AFJ3" s="0"/>
+      <c r="AFK3" s="0"/>
+      <c r="AFL3" s="0"/>
+      <c r="AFM3" s="0"/>
+      <c r="AFN3" s="0"/>
+      <c r="AFO3" s="0"/>
+      <c r="AFP3" s="0"/>
+      <c r="AFQ3" s="0"/>
+      <c r="AFR3" s="0"/>
+      <c r="AFS3" s="0"/>
+      <c r="AFT3" s="0"/>
+      <c r="AFU3" s="0"/>
+      <c r="AFV3" s="0"/>
+      <c r="AFW3" s="0"/>
+      <c r="AFX3" s="0"/>
+      <c r="AFY3" s="0"/>
+      <c r="AFZ3" s="0"/>
+      <c r="AGA3" s="0"/>
+      <c r="AGB3" s="0"/>
+      <c r="AGC3" s="0"/>
+      <c r="AGD3" s="0"/>
+      <c r="AGE3" s="0"/>
+      <c r="AGF3" s="0"/>
+      <c r="AGG3" s="0"/>
+      <c r="AGH3" s="0"/>
+      <c r="AGI3" s="0"/>
+      <c r="AGJ3" s="0"/>
+      <c r="AGK3" s="0"/>
+      <c r="AGL3" s="0"/>
+      <c r="AGM3" s="0"/>
+      <c r="AGN3" s="0"/>
+      <c r="AGO3" s="0"/>
+      <c r="AGP3" s="0"/>
+      <c r="AGQ3" s="0"/>
+      <c r="AGR3" s="0"/>
+      <c r="AGS3" s="0"/>
+      <c r="AGT3" s="0"/>
+      <c r="AGU3" s="0"/>
+      <c r="AGV3" s="0"/>
+      <c r="AGW3" s="0"/>
+      <c r="AGX3" s="0"/>
+      <c r="AGY3" s="0"/>
+      <c r="AGZ3" s="0"/>
+      <c r="AHA3" s="0"/>
+      <c r="AHB3" s="0"/>
+      <c r="AHC3" s="0"/>
+      <c r="AHD3" s="0"/>
+      <c r="AHE3" s="0"/>
+      <c r="AHF3" s="0"/>
+      <c r="AHG3" s="0"/>
+      <c r="AHH3" s="0"/>
+      <c r="AHI3" s="0"/>
+      <c r="AHJ3" s="0"/>
+      <c r="AHK3" s="0"/>
+      <c r="AHL3" s="0"/>
+      <c r="AHM3" s="0"/>
+      <c r="AHN3" s="0"/>
+      <c r="AHO3" s="0"/>
+      <c r="AHP3" s="0"/>
+      <c r="AHQ3" s="0"/>
+      <c r="AHR3" s="0"/>
+      <c r="AHS3" s="0"/>
+      <c r="AHT3" s="0"/>
+      <c r="AHU3" s="0"/>
+      <c r="AHV3" s="0"/>
+      <c r="AHW3" s="0"/>
+      <c r="AHX3" s="0"/>
+      <c r="AHY3" s="0"/>
+      <c r="AHZ3" s="0"/>
+      <c r="AIA3" s="0"/>
+      <c r="AIB3" s="0"/>
+      <c r="AIC3" s="0"/>
+      <c r="AID3" s="0"/>
+      <c r="AIE3" s="0"/>
+      <c r="AIF3" s="0"/>
+      <c r="AIG3" s="0"/>
+      <c r="AIH3" s="0"/>
+      <c r="AII3" s="0"/>
+      <c r="AIJ3" s="0"/>
+      <c r="AIK3" s="0"/>
+      <c r="AIL3" s="0"/>
+      <c r="AIM3" s="0"/>
+      <c r="AIN3" s="0"/>
+      <c r="AIO3" s="0"/>
+      <c r="AIP3" s="0"/>
+      <c r="AIQ3" s="0"/>
+      <c r="AIR3" s="0"/>
+      <c r="AIS3" s="0"/>
+      <c r="AIT3" s="0"/>
+      <c r="AIU3" s="0"/>
+      <c r="AIV3" s="0"/>
+      <c r="AIW3" s="0"/>
+      <c r="AIX3" s="0"/>
+      <c r="AIY3" s="0"/>
+      <c r="AIZ3" s="0"/>
+      <c r="AJA3" s="0"/>
+      <c r="AJB3" s="0"/>
+      <c r="AJC3" s="0"/>
+      <c r="AJD3" s="0"/>
+      <c r="AJE3" s="0"/>
+      <c r="AJF3" s="0"/>
+      <c r="AJG3" s="0"/>
+      <c r="AJH3" s="0"/>
+      <c r="AJI3" s="0"/>
+      <c r="AJJ3" s="0"/>
+      <c r="AJK3" s="0"/>
+      <c r="AJL3" s="0"/>
+      <c r="AJM3" s="0"/>
+      <c r="AJN3" s="0"/>
+      <c r="AJO3" s="0"/>
+      <c r="AJP3" s="0"/>
+      <c r="AJQ3" s="0"/>
+      <c r="AJR3" s="0"/>
+      <c r="AJS3" s="0"/>
+      <c r="AJT3" s="0"/>
+      <c r="AJU3" s="0"/>
+      <c r="AJV3" s="0"/>
+      <c r="AJW3" s="0"/>
+      <c r="AJX3" s="0"/>
+      <c r="AJY3" s="0"/>
+      <c r="AJZ3" s="0"/>
+      <c r="AKA3" s="0"/>
+      <c r="AKB3" s="0"/>
+      <c r="AKC3" s="0"/>
+      <c r="AKD3" s="0"/>
+      <c r="AKE3" s="0"/>
+      <c r="AKF3" s="0"/>
+      <c r="AKG3" s="0"/>
+      <c r="AKH3" s="0"/>
+      <c r="AKI3" s="0"/>
+      <c r="AKJ3" s="0"/>
+      <c r="AKK3" s="0"/>
+      <c r="AKL3" s="0"/>
+      <c r="AKM3" s="0"/>
+      <c r="AKN3" s="0"/>
+      <c r="AKO3" s="0"/>
+      <c r="AKP3" s="0"/>
+      <c r="AKQ3" s="0"/>
+      <c r="AKR3" s="0"/>
+      <c r="AKS3" s="0"/>
+      <c r="AKT3" s="0"/>
+      <c r="AKU3" s="0"/>
+      <c r="AKV3" s="0"/>
+      <c r="AKW3" s="0"/>
+      <c r="AKX3" s="0"/>
+      <c r="AKY3" s="0"/>
+      <c r="AKZ3" s="0"/>
+      <c r="ALA3" s="0"/>
+      <c r="ALB3" s="0"/>
+      <c r="ALC3" s="0"/>
+      <c r="ALD3" s="0"/>
+      <c r="ALE3" s="0"/>
+      <c r="ALF3" s="0"/>
+      <c r="ALG3" s="0"/>
+      <c r="ALH3" s="0"/>
+      <c r="ALI3" s="0"/>
+      <c r="ALJ3" s="0"/>
+      <c r="ALK3" s="0"/>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="52" customFormat="true" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
@@ -2588,31 +3574,31 @@
         <v>88</v>
       </c>
       <c r="G5" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="I5" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="K5" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="M5" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="N5" s="56" t="s">
-        <v>88</v>
-      </c>
       <c r="O5" s="56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P5" s="40"/>
       <c r="Q5" s="40"/>
@@ -2633,34 +3619,34 @@
       <c r="AF5" s="38"/>
       <c r="AG5" s="38"/>
       <c r="AH5" s="43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI5" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AJ5" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK5" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL5" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="AK5" s="57" t="s">
+      <c r="AM5" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="AL5" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM5" s="42" t="s">
-        <v>89</v>
-      </c>
       <c r="AN5" s="45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AO5" s="45" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AP5" s="45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ5" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AR5" s="43"/>
       <c r="AS5" s="42"/>
@@ -2693,34 +3679,34 @@
       <c r="BD5" s="42"/>
       <c r="BE5" s="42"/>
       <c r="BF5" s="47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BG5" s="47" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="BH5" s="47"/>
       <c r="BI5" s="47"/>
       <c r="BJ5" s="46" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BK5" s="47" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BL5" s="42"/>
       <c r="BM5" s="42"/>
       <c r="BN5" s="42"/>
       <c r="BO5" s="42"/>
       <c r="BP5" s="46" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BQ5" s="42" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="BR5" s="42" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BS5" s="42" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="BT5" s="43"/>
       <c r="BU5" s="42"/>
@@ -2729,47 +3715,47 @@
       <c r="BX5" s="45"/>
       <c r="BY5" s="38"/>
       <c r="BZ5" s="48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CA5" s="49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CB5" s="49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CC5" s="49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CD5" s="49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CE5" s="50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CF5" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="CG5" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="CH5" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="CI5" s="49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="CJ5" s="53" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="CK5" s="54" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="CL5" s="54"/>
       <c r="CM5" s="54"/>
       <c r="CN5" s="53"/>
       <c r="CO5" s="42"/>
       <c r="CP5" s="38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="CQ5" s="38"/>
       <c r="CR5" s="58"/>
@@ -2805,13 +3791,13 @@
       <c r="B6" s="53"/>
       <c r="C6" s="54"/>
       <c r="D6" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="G6" s="60" t="s">
         <v>87</v>
@@ -2843,58 +3829,58 @@
       <c r="AF6" s="38"/>
       <c r="AG6" s="38"/>
       <c r="AH6" s="43" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AI6" s="42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AJ6" s="57" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="AK6" s="57" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AL6" s="42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AM6" s="42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AN6" s="38"/>
       <c r="AO6" s="38"/>
       <c r="AP6" s="38" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AQ6" s="42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="AR6" s="43"/>
       <c r="AS6" s="42"/>
       <c r="AT6" s="42"/>
       <c r="AU6" s="42"/>
       <c r="AV6" s="40" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AW6" s="40" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AX6" s="40" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AY6" s="40" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AZ6" s="40" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="BA6" s="40" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="BB6" s="40" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="BC6" s="40" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="BD6" s="42"/>
       <c r="BE6" s="42"/>
@@ -2909,16 +3895,16 @@
       <c r="BN6" s="42"/>
       <c r="BO6" s="42"/>
       <c r="BP6" s="46" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="BQ6" s="42" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="BR6" s="42" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="BS6" s="42" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="BT6" s="43"/>
       <c r="BU6" s="42"/>
@@ -2927,40 +3913,40 @@
       <c r="BX6" s="45"/>
       <c r="BY6" s="38"/>
       <c r="BZ6" s="48" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CA6" s="49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CB6" s="49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CC6" s="49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CD6" s="49" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CE6" s="50" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="49" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="CG6" s="49" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="CH6" s="49" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="CI6" s="49" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="CJ6" s="53" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="CK6" s="54" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="CL6" s="54"/>
       <c r="CM6" s="54"/>
@@ -3001,16 +3987,16 @@
       <c r="B7" s="53"/>
       <c r="C7" s="54"/>
       <c r="D7" s="38" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G7" s="60" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H7" s="45"/>
       <c r="I7" s="45"/>
@@ -3041,10 +4027,10 @@
       <c r="AH7" s="43"/>
       <c r="AI7" s="42"/>
       <c r="AJ7" s="57" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="AK7" s="57" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="AL7" s="45"/>
       <c r="AM7" s="45"/>
@@ -3057,28 +4043,28 @@
       <c r="AT7" s="42"/>
       <c r="AU7" s="42"/>
       <c r="AV7" s="40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="AW7" s="40" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="AX7" s="40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="AY7" s="40" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="AZ7" s="40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="BA7" s="40" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="BB7" s="40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="BC7" s="40" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="BD7" s="42"/>
       <c r="BE7" s="42"/>
@@ -3093,21 +4079,21 @@
       <c r="BN7" s="42"/>
       <c r="BO7" s="42"/>
       <c r="BP7" s="46" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="BQ7" s="45" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="BR7" s="45" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="BS7" s="42" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="BT7" s="43"/>
       <c r="BU7" s="42"/>
       <c r="BV7" s="38" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="BW7" s="38"/>
       <c r="BX7" s="38"/>
@@ -3129,7 +4115,7 @@
       <c r="CN7" s="62"/>
       <c r="CO7" s="42"/>
       <c r="CP7" s="38" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="CQ7" s="38"/>
       <c r="CR7" s="58"/>
@@ -3165,16 +4151,16 @@
       <c r="B8" s="53"/>
       <c r="C8" s="54"/>
       <c r="D8" s="38" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G8" s="65" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
@@ -3205,10 +4191,10 @@
       <c r="AH8" s="43"/>
       <c r="AI8" s="42"/>
       <c r="AJ8" s="57" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="AK8" s="57" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="AL8" s="45"/>
       <c r="AM8" s="45"/>
@@ -3221,28 +4207,28 @@
       <c r="AT8" s="42"/>
       <c r="AU8" s="42"/>
       <c r="AV8" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="AW8" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="AX8" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="AY8" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="AZ8" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="BA8" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="BB8" s="40" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="BC8" s="40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="BD8" s="42"/>
       <c r="BE8" s="42"/>
@@ -3259,15 +4245,15 @@
       <c r="BP8" s="42"/>
       <c r="BQ8" s="42"/>
       <c r="BR8" s="42" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="BS8" s="42" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="BT8" s="43"/>
       <c r="BU8" s="42"/>
       <c r="BV8" s="38" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="BW8" s="38"/>
       <c r="BX8" s="38"/>
@@ -3289,7 +4275,7 @@
       <c r="CN8" s="43"/>
       <c r="CO8" s="42"/>
       <c r="CP8" s="38" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="CQ8" s="38"/>
       <c r="CR8" s="58"/>
@@ -3325,16 +4311,16 @@
       <c r="B9" s="53"/>
       <c r="C9" s="54"/>
       <c r="D9" s="38" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
@@ -3365,10 +4351,10 @@
       <c r="AH9" s="43"/>
       <c r="AI9" s="42"/>
       <c r="AJ9" s="57" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="AK9" s="57" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="AL9" s="45"/>
       <c r="AM9" s="45"/>
@@ -3381,28 +4367,28 @@
       <c r="AT9" s="42"/>
       <c r="AU9" s="42"/>
       <c r="AV9" s="40" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="AW9" s="40" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="AX9" s="40" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="AY9" s="40" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="AZ9" s="40" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="BA9" s="40" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="BB9" s="40" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="BC9" s="40" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="BD9" s="42"/>
       <c r="BE9" s="42"/>
@@ -3419,15 +4405,15 @@
       <c r="BP9" s="42"/>
       <c r="BQ9" s="42"/>
       <c r="BR9" s="42" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="BS9" s="42" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="BT9" s="43"/>
       <c r="BU9" s="42"/>
       <c r="BV9" s="38" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="BW9" s="38"/>
       <c r="BX9" s="38"/>
@@ -3449,7 +4435,7 @@
       <c r="CN9" s="43"/>
       <c r="CO9" s="42"/>
       <c r="CP9" s="38" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="CQ9" s="38"/>
       <c r="CR9" s="58"/>
@@ -3485,16 +4471,16 @@
       <c r="B10" s="53"/>
       <c r="C10" s="54"/>
       <c r="D10" s="42" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="G10" s="60" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
@@ -3525,10 +4511,10 @@
       <c r="AH10" s="43"/>
       <c r="AI10" s="42"/>
       <c r="AJ10" s="57" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="AK10" s="57" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="AL10" s="45"/>
       <c r="AM10" s="45"/>
@@ -3579,15 +4565,15 @@
       <c r="BP10" s="42"/>
       <c r="BQ10" s="42"/>
       <c r="BR10" s="42" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="BS10" s="42" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="BT10" s="43"/>
       <c r="BU10" s="42"/>
       <c r="BV10" s="38" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="BW10" s="38"/>
       <c r="BX10" s="38"/>
@@ -3609,7 +4595,7 @@
       <c r="CN10" s="43"/>
       <c r="CO10" s="42"/>
       <c r="CP10" s="38" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="CQ10" s="38"/>
       <c r="CR10" s="58"/>
@@ -3645,16 +4631,16 @@
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
       <c r="D11" s="38" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="G11" s="65" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
@@ -3685,10 +4671,10 @@
       <c r="AH11" s="43"/>
       <c r="AI11" s="42"/>
       <c r="AJ11" s="57" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="AK11" s="57" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="AL11" s="45"/>
       <c r="AM11" s="45"/>
@@ -3701,28 +4687,28 @@
       <c r="AT11" s="42"/>
       <c r="AU11" s="42"/>
       <c r="AV11" s="40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AW11" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AX11" s="40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AY11" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AZ11" s="40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BA11" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="BB11" s="40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BC11" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="BD11" s="42"/>
       <c r="BE11" s="42"/>
@@ -3743,7 +4729,7 @@
       <c r="BT11" s="43"/>
       <c r="BU11" s="42"/>
       <c r="BV11" s="38" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="BW11" s="38"/>
       <c r="BX11" s="38"/>
@@ -3765,7 +4751,7 @@
       <c r="CN11" s="43"/>
       <c r="CO11" s="42"/>
       <c r="CP11" s="38" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="CQ11" s="38"/>
       <c r="CR11" s="58"/>
@@ -3801,16 +4787,16 @@
       <c r="B12" s="53"/>
       <c r="C12" s="54"/>
       <c r="D12" s="38" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G12" s="60" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
@@ -3841,10 +4827,10 @@
       <c r="AH12" s="43"/>
       <c r="AI12" s="42"/>
       <c r="AJ12" s="57" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="AK12" s="57" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="AL12" s="45"/>
       <c r="AM12" s="45"/>
@@ -3857,28 +4843,28 @@
       <c r="AT12" s="42"/>
       <c r="AU12" s="42"/>
       <c r="AV12" s="40" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AW12" s="40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="AX12" s="40" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AY12" s="40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="AZ12" s="40" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="BA12" s="40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="BB12" s="40" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="BC12" s="40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="BD12" s="42"/>
       <c r="BE12" s="42"/>
@@ -3899,7 +4885,7 @@
       <c r="BT12" s="43"/>
       <c r="BU12" s="42"/>
       <c r="BV12" s="38" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="BW12" s="38"/>
       <c r="BX12" s="38"/>
@@ -3921,7 +4907,7 @@
       <c r="CN12" s="43"/>
       <c r="CO12" s="42"/>
       <c r="CP12" s="38" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="CQ12" s="38"/>
       <c r="CR12" s="58"/>
@@ -3957,16 +4943,16 @@
       <c r="B13" s="53"/>
       <c r="C13" s="54"/>
       <c r="D13" s="38" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
@@ -3997,10 +4983,10 @@
       <c r="AH13" s="53"/>
       <c r="AI13" s="54"/>
       <c r="AJ13" s="57" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="AK13" s="57" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="AL13" s="45"/>
       <c r="AM13" s="45"/>
@@ -4013,28 +4999,28 @@
       <c r="AT13" s="42"/>
       <c r="AU13" s="42"/>
       <c r="AV13" s="40" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="AW13" s="40" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="AX13" s="40" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="AY13" s="40" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="AZ13" s="40" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="BA13" s="40" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="BB13" s="40" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="BC13" s="40" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="BD13" s="42"/>
       <c r="BE13" s="42"/>
@@ -4055,7 +5041,7 @@
       <c r="BT13" s="43"/>
       <c r="BU13" s="42"/>
       <c r="BV13" s="38" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="BW13" s="38"/>
       <c r="BX13" s="38"/>
@@ -4077,7 +5063,7 @@
       <c r="CN13" s="43"/>
       <c r="CO13" s="42"/>
       <c r="CP13" s="38" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="CQ13" s="38"/>
       <c r="CR13" s="58"/>
@@ -4113,16 +5099,16 @@
       <c r="B14" s="53"/>
       <c r="C14" s="54"/>
       <c r="D14" s="38" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="F14" s="59" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="G14" s="60" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
@@ -4153,10 +5139,10 @@
       <c r="AH14" s="53"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="57" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="AK14" s="57" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="AL14" s="45"/>
       <c r="AM14" s="45"/>
@@ -4169,35 +5155,35 @@
       <c r="AT14" s="42"/>
       <c r="AU14" s="42"/>
       <c r="AV14" s="40" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="AW14" s="40" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="AX14" s="40" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="AY14" s="40" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="AZ14" s="40" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="BA14" s="40" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="BB14" s="40" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="BC14" s="40" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="BD14" s="42"/>
       <c r="BE14" s="42"/>
       <c r="BF14" s="42"/>
       <c r="BG14" s="42"/>
       <c r="BH14" s="42" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="BI14" s="42"/>
       <c r="BJ14" s="42"/>
@@ -4213,7 +5199,7 @@
       <c r="BT14" s="43"/>
       <c r="BU14" s="42"/>
       <c r="BV14" s="38" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="BW14" s="38"/>
       <c r="BX14" s="38"/>
@@ -4235,7 +5221,7 @@
       <c r="CN14" s="43"/>
       <c r="CO14" s="42"/>
       <c r="CP14" s="38" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="CQ14" s="38"/>
       <c r="CR14" s="58"/>
@@ -4266,21 +5252,21 @@
       <c r="DQ14" s="51"/>
       <c r="DR14" s="51"/>
     </row>
-    <row r="15" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="103.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35"/>
       <c r="B15" s="53"/>
       <c r="C15" s="54"/>
       <c r="D15" s="38" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="F15" s="59" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
@@ -4311,10 +5297,10 @@
       <c r="AH15" s="53"/>
       <c r="AI15" s="54"/>
       <c r="AJ15" s="57" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="AK15" s="57" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="AL15" s="45"/>
       <c r="AM15" s="45"/>
@@ -4327,35 +5313,35 @@
       <c r="AT15" s="42"/>
       <c r="AU15" s="42"/>
       <c r="AV15" s="40" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="AW15" s="40" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="AX15" s="40" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="AY15" s="40" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="AZ15" s="40" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="BA15" s="40" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="BB15" s="40" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="BC15" s="40" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="BD15" s="42"/>
       <c r="BE15" s="42"/>
       <c r="BF15" s="42"/>
       <c r="BG15" s="42"/>
       <c r="BH15" s="42" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="BI15" s="42"/>
       <c r="BJ15" s="42"/>
@@ -4371,7 +5357,7 @@
       <c r="BT15" s="43"/>
       <c r="BU15" s="42"/>
       <c r="BV15" s="38" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="BW15" s="38"/>
       <c r="BX15" s="38"/>
@@ -4393,7 +5379,7 @@
       <c r="CN15" s="43"/>
       <c r="CO15" s="42"/>
       <c r="CP15" s="38" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="CQ15" s="38"/>
       <c r="CR15" s="58"/>
@@ -4429,16 +5415,16 @@
       <c r="B16" s="53"/>
       <c r="C16" s="54"/>
       <c r="D16" s="38" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
@@ -4481,28 +5467,28 @@
       <c r="AT16" s="42"/>
       <c r="AU16" s="42"/>
       <c r="AV16" s="40" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="AW16" s="40" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="AX16" s="40" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="AY16" s="40" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="AZ16" s="40" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="BA16" s="40" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="BB16" s="40" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="BC16" s="40" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="BD16" s="42"/>
       <c r="BE16" s="42"/>
@@ -4523,7 +5509,7 @@
       <c r="BT16" s="43"/>
       <c r="BU16" s="42"/>
       <c r="BV16" s="38" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="BW16" s="38"/>
       <c r="BX16" s="38"/>
@@ -4545,7 +5531,7 @@
       <c r="CN16" s="43"/>
       <c r="CO16" s="42"/>
       <c r="CP16" s="38" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="CQ16" s="38"/>
       <c r="CR16" s="58"/>
@@ -4581,13 +5567,13 @@
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
       <c r="D17" s="38" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="F17" s="59" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="G17" s="65" t="s">
         <v>83</v>
@@ -4633,28 +5619,28 @@
       <c r="AT17" s="42"/>
       <c r="AU17" s="42"/>
       <c r="AV17" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="AW17" s="40" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="AX17" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="AY17" s="40" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="AZ17" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="BA17" s="40" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="BB17" s="40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="BC17" s="40" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="BD17" s="42"/>
       <c r="BE17" s="42"/>
@@ -4675,7 +5661,7 @@
       <c r="BT17" s="43"/>
       <c r="BU17" s="42"/>
       <c r="BV17" s="38" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="BW17" s="38"/>
       <c r="BX17" s="38"/>
@@ -4731,16 +5717,16 @@
       <c r="B18" s="53"/>
       <c r="C18" s="54"/>
       <c r="D18" s="38" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="F18" s="59" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="G18" s="60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H18" s="38"/>
       <c r="I18" s="38"/>
@@ -4783,28 +5769,28 @@
       <c r="AT18" s="42"/>
       <c r="AU18" s="42"/>
       <c r="AV18" s="40" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="AW18" s="40" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="AX18" s="40" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="AY18" s="40" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="AZ18" s="40" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="BA18" s="40" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="BB18" s="40" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="BC18" s="40" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="BD18" s="42"/>
       <c r="BE18" s="42"/>
@@ -4825,7 +5811,7 @@
       <c r="BT18" s="43"/>
       <c r="BU18" s="42"/>
       <c r="BV18" s="38" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="BW18" s="38"/>
       <c r="BX18" s="38"/>
@@ -4881,16 +5867,16 @@
       <c r="B19" s="53"/>
       <c r="C19" s="54"/>
       <c r="D19" s="38" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G19" s="60" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
@@ -4933,28 +5919,28 @@
       <c r="AT19" s="42"/>
       <c r="AU19" s="42"/>
       <c r="AV19" s="40" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="AW19" s="40" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="AX19" s="40" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="AY19" s="40" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="AZ19" s="40" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="BA19" s="40" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="BB19" s="40" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="BC19" s="40" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="BD19" s="42"/>
       <c r="BE19" s="42"/>
@@ -4975,7 +5961,7 @@
       <c r="BT19" s="43"/>
       <c r="BU19" s="42"/>
       <c r="BV19" s="38" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="BW19" s="38"/>
       <c r="BX19" s="38"/>
@@ -5031,16 +6017,16 @@
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
       <c r="D20" s="38" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="G20" s="60" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
@@ -5083,28 +6069,28 @@
       <c r="AT20" s="42"/>
       <c r="AU20" s="42"/>
       <c r="AV20" s="40" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="AW20" s="40" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="AX20" s="40" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="AY20" s="40" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="AZ20" s="40" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="BA20" s="40" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="BB20" s="40" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="BC20" s="40" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="BD20" s="42"/>
       <c r="BE20" s="42"/>
@@ -5125,7 +6111,7 @@
       <c r="BT20" s="43"/>
       <c r="BU20" s="42"/>
       <c r="BV20" s="38" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="BW20" s="38"/>
       <c r="BX20" s="38"/>
@@ -5181,10 +6167,10 @@
       <c r="B21" s="53"/>
       <c r="C21" s="54"/>
       <c r="D21" s="38" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F21" s="53"/>
       <c r="G21" s="54"/>
@@ -5232,25 +6218,25 @@
         <v>70</v>
       </c>
       <c r="AW21" s="49" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="AX21" s="49" t="s">
         <v>70</v>
       </c>
       <c r="AY21" s="49" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="AZ21" s="49" t="s">
         <v>70</v>
       </c>
       <c r="BA21" s="49" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="BB21" s="49" t="s">
         <v>70</v>
       </c>
       <c r="BC21" s="49" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="BD21" s="42"/>
       <c r="BE21" s="42"/>
@@ -5271,7 +6257,7 @@
       <c r="BT21" s="43"/>
       <c r="BU21" s="42"/>
       <c r="BV21" s="38" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="BW21" s="38"/>
       <c r="BX21" s="38"/>
@@ -5327,10 +6313,10 @@
       <c r="B22" s="53"/>
       <c r="C22" s="54"/>
       <c r="D22" s="38" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="54"/>
@@ -5401,7 +6387,7 @@
       <c r="BT22" s="43"/>
       <c r="BU22" s="42"/>
       <c r="BV22" s="38" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="BW22" s="38"/>
       <c r="BX22" s="38"/>
@@ -5457,10 +6443,10 @@
       <c r="B23" s="53"/>
       <c r="C23" s="54"/>
       <c r="D23" s="38" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="54"/>
@@ -5531,7 +6517,7 @@
       <c r="BT23" s="43"/>
       <c r="BU23" s="42"/>
       <c r="BV23" s="38" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="BW23" s="38"/>
       <c r="BX23" s="38"/>
@@ -5587,10 +6573,10 @@
       <c r="B24" s="53"/>
       <c r="C24" s="54"/>
       <c r="D24" s="38" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="54"/>
@@ -5661,7 +6647,7 @@
       <c r="BT24" s="43"/>
       <c r="BU24" s="42"/>
       <c r="BV24" s="38" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="BW24" s="38"/>
       <c r="BX24" s="38"/>
@@ -5717,10 +6703,10 @@
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
       <c r="D25" s="38" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="54"/>
@@ -5845,10 +6831,10 @@
       <c r="B26" s="53"/>
       <c r="C26" s="54"/>
       <c r="D26" s="38" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="F26" s="53"/>
       <c r="G26" s="54"/>
@@ -5973,10 +6959,10 @@
       <c r="B27" s="53"/>
       <c r="C27" s="54"/>
       <c r="D27" s="42" t="s">
-        <v>141</v>
+        <v>235</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="F27" s="53"/>
       <c r="G27" s="54"/>
@@ -6101,10 +7087,10 @@
       <c r="B28" s="53"/>
       <c r="C28" s="54"/>
       <c r="D28" s="42" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="F28" s="53"/>
       <c r="G28" s="54"/>
@@ -6229,10 +7215,10 @@
       <c r="B29" s="53"/>
       <c r="C29" s="54"/>
       <c r="D29" s="42" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="54"/>
@@ -6357,10 +7343,10 @@
       <c r="B30" s="53"/>
       <c r="C30" s="54"/>
       <c r="D30" s="38" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="F30" s="53"/>
       <c r="G30" s="54"/>
@@ -6613,10 +7599,10 @@
       <c r="B32" s="53"/>
       <c r="C32" s="54"/>
       <c r="D32" s="38" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="54"/>
@@ -6741,10 +7727,10 @@
       <c r="B33" s="53"/>
       <c r="C33" s="54"/>
       <c r="D33" s="38" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="F33" s="53"/>
       <c r="G33" s="54"/>
@@ -6869,10 +7855,10 @@
       <c r="B34" s="53"/>
       <c r="C34" s="54"/>
       <c r="D34" s="38" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F34" s="53"/>
       <c r="G34" s="54"/>
@@ -6997,10 +7983,10 @@
       <c r="B35" s="53"/>
       <c r="C35" s="54"/>
       <c r="D35" s="38" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="F35" s="53"/>
       <c r="G35" s="54"/>
@@ -7125,10 +8111,10 @@
       <c r="B36" s="53"/>
       <c r="C36" s="54"/>
       <c r="D36" s="38" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="E36" s="38" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="F36" s="53"/>
       <c r="G36" s="54"/>
@@ -7253,10 +8239,10 @@
       <c r="B37" s="53"/>
       <c r="C37" s="54"/>
       <c r="D37" s="42" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="F37" s="53"/>
       <c r="G37" s="54"/>
@@ -7381,10 +8367,10 @@
       <c r="B38" s="53"/>
       <c r="C38" s="54"/>
       <c r="D38" s="42" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="F38" s="53"/>
       <c r="G38" s="54"/>
@@ -7509,10 +8495,10 @@
       <c r="B39" s="53"/>
       <c r="C39" s="54"/>
       <c r="D39" s="42" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="F39" s="53"/>
       <c r="G39" s="54"/>
@@ -7637,10 +8623,10 @@
       <c r="B40" s="53"/>
       <c r="C40" s="54"/>
       <c r="D40" s="38" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="F40" s="53"/>
       <c r="G40" s="54"/>
@@ -7765,10 +8751,10 @@
       <c r="B41" s="43"/>
       <c r="C41" s="42"/>
       <c r="D41" s="38" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="F41" s="53"/>
       <c r="G41" s="54"/>
@@ -7893,10 +8879,10 @@
       <c r="B42" s="43"/>
       <c r="C42" s="42"/>
       <c r="D42" s="38" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="F42" s="53"/>
       <c r="G42" s="54"/>
@@ -8021,10 +9007,10 @@
       <c r="B43" s="43"/>
       <c r="C43" s="42"/>
       <c r="D43" s="38" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F43" s="53"/>
       <c r="G43" s="54"/>
@@ -8149,10 +9135,10 @@
       <c r="B44" s="43"/>
       <c r="C44" s="42"/>
       <c r="D44" s="38" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="F44" s="43"/>
       <c r="G44" s="42"/>
@@ -8276,10 +9262,10 @@
       <c r="B45" s="43"/>
       <c r="C45" s="42"/>
       <c r="D45" s="38" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F45" s="43"/>
       <c r="G45" s="42"/>
@@ -8403,10 +9389,10 @@
       <c r="B46" s="43"/>
       <c r="C46" s="42"/>
       <c r="D46" s="38" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="42"/>
@@ -8530,10 +9516,10 @@
       <c r="B47" s="43"/>
       <c r="C47" s="42"/>
       <c r="D47" s="38" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="42"/>

</xml_diff>

<commit_message>
Updated the Zooplankton samples and subsamples
</commit_message>
<xml_diff>
--- a/Sample_and_gear_types_AeN.xlsx
+++ b/Sample_and_gear_types_AeN.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="261">
   <si>
     <t xml:space="preserve">Sample Group</t>
   </si>
@@ -520,6 +520,9 @@
     <t xml:space="preserve">Organic C/N</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton carbohydrat</t>
+  </si>
+  <si>
     <t xml:space="preserve">Macrozooplankton stable isotope</t>
   </si>
   <si>
@@ -547,6 +550,9 @@
     <t xml:space="preserve">pH</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton energetics</t>
+  </si>
+  <si>
     <t xml:space="preserve">HBIs and coccoliths</t>
   </si>
   <si>
@@ -568,6 +574,9 @@
     <t xml:space="preserve">Pore water content</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton fatty acid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lithological description</t>
   </si>
   <si>
@@ -592,63 +601,69 @@
     <t xml:space="preserve">Quanti macrofauna</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrozooplankton gonad </t>
+    <t xml:space="preserve">Macrozooplankton genetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop genetics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">magnetic susceptibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Respiration experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiration exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton gonad </t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop gonad </t>
   </si>
   <si>
-    <t xml:space="preserve">magnetic susceptibility </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stable isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Prokaryote RNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prokaryote RNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Respiration experiments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respiration exp</t>
+    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suction pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC/DON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Sediment stable isotopes, carbon and nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sed isotopes, C, N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton hg</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop hg</t>
   </si>
   <si>
-    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen profiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suction pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC/DON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Protist DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Sediment stable isotopes, carbon and nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sed isotopes, C, N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton length</t>
-  </si>
-  <si>
     <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
   </si>
   <si>
@@ -664,10 +679,7 @@
     <t xml:space="preserve">Protists micros&lt;10um</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrozooplankton nutrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop length</t>
+    <t xml:space="preserve">1, Macrozooplankton stable isotope</t>
   </si>
   <si>
     <t xml:space="preserve">Planktic foraminifera</t>
@@ -685,6 +697,9 @@
     <t xml:space="preserve">1 ,Protist microscopy &gt; 10 um</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton nutrition</t>
+  </si>
+  <si>
     <t xml:space="preserve">Macrozoop nutrition</t>
   </si>
   <si>
@@ -697,6 +712,9 @@
     <t xml:space="preserve">1, Protist PCR</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton organic pollutio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
@@ -709,6 +727,9 @@
     <t xml:space="preserve">Silicate incorp</t>
   </si>
   <si>
+    <t xml:space="preserve">1, Macrozooplankton protein</t>
+  </si>
+  <si>
     <t xml:space="preserve">Macrozoop protein</t>
   </si>
   <si>
@@ -724,16 +745,13 @@
     <t xml:space="preserve">Virus DNA</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrozoplankton stomach</t>
+    <t xml:space="preserve">1, Macrozoplankton stomach</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozop stomach</t>
   </si>
   <si>
     <t xml:space="preserve">Sediment grain size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop tax</t>
   </si>
   <si>
     <t xml:space="preserve">Sedimentology</t>
@@ -1444,11 +1462,11 @@
       <xdr:col>58</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>355680</xdr:rowOff>
+      <xdr:rowOff>356040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
@@ -1459,8 +1477,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59340600" y="4919760"/>
-          <a:ext cx="3118680" cy="430200"/>
+          <a:off x="58588200" y="4920120"/>
+          <a:ext cx="3061080" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1491,9 +1509,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1502,8 +1520,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="59340600" y="5300280"/>
-          <a:ext cx="3118680" cy="1360800"/>
+          <a:off x="58588200" y="5300280"/>
+          <a:ext cx="3061080" cy="1347840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1528,13 +1546,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>356760</xdr:rowOff>
+      <xdr:rowOff>357120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
@@ -1545,8 +1563,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73476000" y="3399480"/>
-          <a:ext cx="4128120" cy="429480"/>
+          <a:off x="72457200" y="3399840"/>
+          <a:ext cx="4051440" cy="429120"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1571,13 +1589,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>356040</xdr:rowOff>
+      <xdr:rowOff>356400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
@@ -1588,8 +1606,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73476000" y="4159440"/>
-          <a:ext cx="4128120" cy="430200"/>
+          <a:off x="72457200" y="4159800"/>
+          <a:ext cx="4051440" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1614,15 +1632,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>355680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1631,8 +1649,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73476000" y="4539600"/>
-          <a:ext cx="4128120" cy="429840"/>
+          <a:off x="72457200" y="4539600"/>
+          <a:ext cx="4051440" cy="429480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1657,15 +1675,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>356040</xdr:rowOff>
+      <xdr:rowOff>356400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1674,8 +1692,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73476000" y="5680800"/>
-          <a:ext cx="4128120" cy="1360080"/>
+          <a:off x="72457200" y="5681160"/>
+          <a:ext cx="4051440" cy="1346760"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1700,15 +1718,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>356040</xdr:rowOff>
+      <xdr:rowOff>349920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1717,8 +1735,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73476000" y="7752240"/>
-          <a:ext cx="4128120" cy="430200"/>
+          <a:off x="72457200" y="7740000"/>
+          <a:ext cx="4051440" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1750,41 +1768,43 @@
   </sheetPr>
   <dimension ref="1:83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BM15" activeCellId="0" sqref="BM15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="8" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="5" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="25" min="22" style="5" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="33" min="26" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="43" min="36" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="71" min="46" style="5" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="73" min="72" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="77" min="74" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="79" min="78" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="82" min="80" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="86" min="84" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="87" min="87" style="5" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="90" min="88" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="7" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="92" min="92" style="8" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="9" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="94" min="94" style="4" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="10" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="97" style="4" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="8" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="25" min="22" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="33" min="26" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="43" min="36" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="47" min="46" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="5" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="71" min="49" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="73" min="72" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="77" min="74" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="79" min="78" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="82" min="80" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="86" min="84" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="87" min="87" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="90" min="88" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="92" min="92" style="8" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="9" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="94" min="94" style="4" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="10" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="97" style="4" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="23" customFormat="true" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3576,25 +3596,25 @@
       <c r="G5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="I5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="K5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="M5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="56" t="s">
         <v>88</v>
       </c>
       <c r="O5" s="56" t="s">
@@ -4526,28 +4546,28 @@
       <c r="AS10" s="42"/>
       <c r="AT10" s="42"/>
       <c r="AU10" s="42"/>
-      <c r="AV10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="AW10" s="40" t="s">
+      <c r="AV10" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="AW10" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="AX10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY10" s="40" t="s">
+      <c r="AX10" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="AY10" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="AZ10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="BA10" s="40" t="s">
+      <c r="AZ10" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="BA10" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="BB10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="BC10" s="40" t="s">
+      <c r="BB10" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="BC10" s="56" t="s">
         <v>80</v>
       </c>
       <c r="BD10" s="42"/>
@@ -4565,15 +4585,15 @@
       <c r="BP10" s="42"/>
       <c r="BQ10" s="42"/>
       <c r="BR10" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="BS10" s="42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BT10" s="43"/>
       <c r="BU10" s="42"/>
       <c r="BV10" s="38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BW10" s="38"/>
       <c r="BX10" s="38"/>
@@ -4595,7 +4615,7 @@
       <c r="CN10" s="43"/>
       <c r="CO10" s="42"/>
       <c r="CP10" s="38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="CQ10" s="38"/>
       <c r="CR10" s="58"/>
@@ -4631,16 +4651,16 @@
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
       <c r="D11" s="38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G11" s="65" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
@@ -4671,10 +4691,10 @@
       <c r="AH11" s="43"/>
       <c r="AI11" s="42"/>
       <c r="AJ11" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AK11" s="57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AL11" s="45"/>
       <c r="AM11" s="45"/>
@@ -4686,28 +4706,28 @@
       <c r="AS11" s="42"/>
       <c r="AT11" s="42"/>
       <c r="AU11" s="42"/>
-      <c r="AV11" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW11" s="40" t="s">
+      <c r="AV11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="AW11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="AX11" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY11" s="40" t="s">
+      <c r="AX11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="AY11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="AZ11" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="BA11" s="40" t="s">
+      <c r="AZ11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="BA11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="BB11" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="BC11" s="40" t="s">
+      <c r="BB11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="BC11" s="56" t="s">
         <v>101</v>
       </c>
       <c r="BD11" s="42"/>
@@ -4729,7 +4749,7 @@
       <c r="BT11" s="43"/>
       <c r="BU11" s="42"/>
       <c r="BV11" s="38" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="BW11" s="38"/>
       <c r="BX11" s="38"/>
@@ -4751,7 +4771,7 @@
       <c r="CN11" s="43"/>
       <c r="CO11" s="42"/>
       <c r="CP11" s="38" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="CQ11" s="38"/>
       <c r="CR11" s="58"/>
@@ -4787,16 +4807,16 @@
       <c r="B12" s="53"/>
       <c r="C12" s="54"/>
       <c r="D12" s="38" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G12" s="60" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
@@ -4827,10 +4847,10 @@
       <c r="AH12" s="43"/>
       <c r="AI12" s="42"/>
       <c r="AJ12" s="57" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AK12" s="57" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AL12" s="45"/>
       <c r="AM12" s="45"/>
@@ -4842,28 +4862,28 @@
       <c r="AS12" s="42"/>
       <c r="AT12" s="42"/>
       <c r="AU12" s="42"/>
-      <c r="AV12" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="AW12" s="40" t="s">
+      <c r="AV12" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW12" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="AX12" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY12" s="40" t="s">
+      <c r="AX12" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="AY12" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="AZ12" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA12" s="40" t="s">
+      <c r="AZ12" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="BA12" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="BB12" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="BC12" s="40" t="s">
+      <c r="BB12" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="BC12" s="56" t="s">
         <v>115</v>
       </c>
       <c r="BD12" s="42"/>
@@ -4885,7 +4905,7 @@
       <c r="BT12" s="43"/>
       <c r="BU12" s="42"/>
       <c r="BV12" s="38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="BW12" s="38"/>
       <c r="BX12" s="38"/>
@@ -4907,7 +4927,7 @@
       <c r="CN12" s="43"/>
       <c r="CO12" s="42"/>
       <c r="CP12" s="38" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="CQ12" s="38"/>
       <c r="CR12" s="58"/>
@@ -4943,16 +4963,16 @@
       <c r="B13" s="53"/>
       <c r="C13" s="54"/>
       <c r="D13" s="38" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
@@ -4983,10 +5003,10 @@
       <c r="AH13" s="53"/>
       <c r="AI13" s="54"/>
       <c r="AJ13" s="57" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AK13" s="57" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AL13" s="45"/>
       <c r="AM13" s="45"/>
@@ -4999,28 +5019,28 @@
       <c r="AT13" s="42"/>
       <c r="AU13" s="42"/>
       <c r="AV13" s="40" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AW13" s="40" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AX13" s="40" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AY13" s="40" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AZ13" s="40" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BA13" s="40" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BB13" s="40" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BC13" s="40" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BD13" s="42"/>
       <c r="BE13" s="42"/>
@@ -5041,7 +5061,7 @@
       <c r="BT13" s="43"/>
       <c r="BU13" s="42"/>
       <c r="BV13" s="38" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BW13" s="38"/>
       <c r="BX13" s="38"/>
@@ -5063,7 +5083,7 @@
       <c r="CN13" s="43"/>
       <c r="CO13" s="42"/>
       <c r="CP13" s="38" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="CQ13" s="38"/>
       <c r="CR13" s="58"/>
@@ -5099,16 +5119,16 @@
       <c r="B14" s="53"/>
       <c r="C14" s="54"/>
       <c r="D14" s="38" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F14" s="59" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G14" s="60" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
@@ -5139,10 +5159,10 @@
       <c r="AH14" s="53"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="57" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AK14" s="57" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AL14" s="45"/>
       <c r="AM14" s="45"/>
@@ -5154,36 +5174,36 @@
       <c r="AS14" s="42"/>
       <c r="AT14" s="42"/>
       <c r="AU14" s="42"/>
-      <c r="AV14" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW14" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="AX14" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="AY14" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="AZ14" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA14" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="BB14" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="BC14" s="40" t="s">
-        <v>187</v>
+      <c r="AV14" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW14" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX14" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AY14" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ14" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="BA14" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="BB14" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="BC14" s="56" t="s">
+        <v>191</v>
       </c>
       <c r="BD14" s="42"/>
       <c r="BE14" s="42"/>
       <c r="BF14" s="42"/>
       <c r="BG14" s="42"/>
       <c r="BH14" s="42" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="BI14" s="42"/>
       <c r="BJ14" s="42"/>
@@ -5199,7 +5219,7 @@
       <c r="BT14" s="43"/>
       <c r="BU14" s="42"/>
       <c r="BV14" s="38" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="BW14" s="38"/>
       <c r="BX14" s="38"/>
@@ -5221,7 +5241,7 @@
       <c r="CN14" s="43"/>
       <c r="CO14" s="42"/>
       <c r="CP14" s="38" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="CQ14" s="38"/>
       <c r="CR14" s="58"/>
@@ -5252,21 +5272,21 @@
       <c r="DQ14" s="51"/>
       <c r="DR14" s="51"/>
     </row>
-    <row r="15" customFormat="false" ht="103.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35"/>
       <c r="B15" s="53"/>
       <c r="C15" s="54"/>
       <c r="D15" s="38" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F15" s="59" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
@@ -5297,10 +5317,10 @@
       <c r="AH15" s="53"/>
       <c r="AI15" s="54"/>
       <c r="AJ15" s="57" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="AK15" s="57" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="AL15" s="45"/>
       <c r="AM15" s="45"/>
@@ -5312,36 +5332,36 @@
       <c r="AS15" s="42"/>
       <c r="AT15" s="42"/>
       <c r="AU15" s="42"/>
-      <c r="AV15" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="AW15" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX15" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="AY15" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="AZ15" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="BA15" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB15" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="BC15" s="40" t="s">
-        <v>155</v>
+      <c r="AV15" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AW15" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX15" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY15" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="AZ15" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="BA15" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="BB15" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="BC15" s="56" t="s">
+        <v>201</v>
       </c>
       <c r="BD15" s="42"/>
       <c r="BE15" s="42"/>
       <c r="BF15" s="42"/>
       <c r="BG15" s="42"/>
       <c r="BH15" s="42" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="BI15" s="42"/>
       <c r="BJ15" s="42"/>
@@ -5357,7 +5377,7 @@
       <c r="BT15" s="43"/>
       <c r="BU15" s="42"/>
       <c r="BV15" s="38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BW15" s="38"/>
       <c r="BX15" s="38"/>
@@ -5379,7 +5399,7 @@
       <c r="CN15" s="43"/>
       <c r="CO15" s="42"/>
       <c r="CP15" s="38" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="CQ15" s="38"/>
       <c r="CR15" s="58"/>
@@ -5415,16 +5435,16 @@
       <c r="B16" s="53"/>
       <c r="C16" s="54"/>
       <c r="D16" s="38" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="G16" s="65" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
@@ -5466,29 +5486,29 @@
       <c r="AS16" s="42"/>
       <c r="AT16" s="42"/>
       <c r="AU16" s="42"/>
-      <c r="AV16" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="AW16" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="AX16" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="AY16" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="AZ16" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="BA16" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="BB16" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="BC16" s="40" t="s">
-        <v>203</v>
+      <c r="AV16" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW16" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX16" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="AY16" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="AZ16" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="BA16" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB16" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="BC16" s="56" t="s">
+        <v>156</v>
       </c>
       <c r="BD16" s="42"/>
       <c r="BE16" s="42"/>
@@ -5509,7 +5529,7 @@
       <c r="BT16" s="43"/>
       <c r="BU16" s="42"/>
       <c r="BV16" s="38" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="BW16" s="38"/>
       <c r="BX16" s="38"/>
@@ -5531,7 +5551,7 @@
       <c r="CN16" s="43"/>
       <c r="CO16" s="42"/>
       <c r="CP16" s="38" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="CQ16" s="38"/>
       <c r="CR16" s="58"/>
@@ -5567,13 +5587,13 @@
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
       <c r="D17" s="38" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F17" s="59" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G17" s="65" t="s">
         <v>83</v>
@@ -5618,29 +5638,29 @@
       <c r="AS17" s="42"/>
       <c r="AT17" s="42"/>
       <c r="AU17" s="42"/>
-      <c r="AV17" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="AW17" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX17" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="AY17" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="AZ17" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="BA17" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="BB17" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="BC17" s="40" t="s">
-        <v>209</v>
+      <c r="AV17" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW17" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="AX17" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="AY17" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="AZ17" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="BA17" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="BB17" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="BC17" s="56" t="s">
+        <v>214</v>
       </c>
       <c r="BD17" s="42"/>
       <c r="BE17" s="42"/>
@@ -5661,7 +5681,7 @@
       <c r="BT17" s="43"/>
       <c r="BU17" s="42"/>
       <c r="BV17" s="38" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="BW17" s="38"/>
       <c r="BX17" s="38"/>
@@ -5717,13 +5737,13 @@
       <c r="B18" s="53"/>
       <c r="C18" s="54"/>
       <c r="D18" s="38" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F18" s="59" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="G18" s="60" t="s">
         <v>103</v>
@@ -5768,28 +5788,28 @@
       <c r="AS18" s="42"/>
       <c r="AT18" s="42"/>
       <c r="AU18" s="42"/>
-      <c r="AV18" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="AW18" s="40" t="s">
+      <c r="AV18" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="AW18" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="AX18" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="AY18" s="40" t="s">
+      <c r="AX18" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY18" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="AZ18" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="BA18" s="40" t="s">
+      <c r="AZ18" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="BA18" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="BB18" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC18" s="40" t="s">
+      <c r="BB18" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC18" s="56" t="s">
         <v>147</v>
       </c>
       <c r="BD18" s="42"/>
@@ -5811,7 +5831,7 @@
       <c r="BT18" s="43"/>
       <c r="BU18" s="42"/>
       <c r="BV18" s="38" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="BW18" s="38"/>
       <c r="BX18" s="38"/>
@@ -5867,16 +5887,16 @@
       <c r="B19" s="53"/>
       <c r="C19" s="54"/>
       <c r="D19" s="38" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="G19" s="60" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
@@ -5918,29 +5938,29 @@
       <c r="AS19" s="42"/>
       <c r="AT19" s="42"/>
       <c r="AU19" s="42"/>
-      <c r="AV19" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW19" s="40" t="s">
-        <v>217</v>
-      </c>
-      <c r="AX19" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="AY19" s="40" t="s">
-        <v>217</v>
-      </c>
-      <c r="AZ19" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA19" s="40" t="s">
-        <v>217</v>
-      </c>
-      <c r="BB19" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC19" s="40" t="s">
-        <v>217</v>
+      <c r="AV19" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="AW19" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="AX19" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="AY19" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ19" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="BA19" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="BB19" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC19" s="56" t="s">
+        <v>224</v>
       </c>
       <c r="BD19" s="42"/>
       <c r="BE19" s="42"/>
@@ -5961,7 +5981,7 @@
       <c r="BT19" s="43"/>
       <c r="BU19" s="42"/>
       <c r="BV19" s="38" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="BW19" s="38"/>
       <c r="BX19" s="38"/>
@@ -6017,16 +6037,16 @@
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
       <c r="D20" s="38" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="G20" s="60" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
@@ -6068,29 +6088,29 @@
       <c r="AS20" s="42"/>
       <c r="AT20" s="42"/>
       <c r="AU20" s="42"/>
-      <c r="AV20" s="40" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW20" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX20" s="40" t="s">
-        <v>222</v>
-      </c>
-      <c r="AY20" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="AZ20" s="40" t="s">
-        <v>222</v>
-      </c>
-      <c r="BA20" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="BB20" s="40" t="s">
-        <v>222</v>
-      </c>
-      <c r="BC20" s="40" t="s">
-        <v>223</v>
+      <c r="AV20" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="AW20" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="AX20" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY20" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="AZ20" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="BA20" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="BB20" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="BC20" s="56" t="s">
+        <v>230</v>
       </c>
       <c r="BD20" s="42"/>
       <c r="BE20" s="42"/>
@@ -6111,7 +6131,7 @@
       <c r="BT20" s="43"/>
       <c r="BU20" s="42"/>
       <c r="BV20" s="38" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="BW20" s="38"/>
       <c r="BX20" s="38"/>
@@ -6214,30 +6234,14 @@
       <c r="AS21" s="42"/>
       <c r="AT21" s="42"/>
       <c r="AU21" s="42"/>
-      <c r="AV21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW21" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="AX21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="AY21" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="AZ21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA21" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="BB21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="BC21" s="49" t="s">
-        <v>225</v>
-      </c>
+      <c r="AV21" s="0"/>
+      <c r="AW21" s="0"/>
+      <c r="AX21" s="49"/>
+      <c r="AY21" s="49"/>
+      <c r="AZ21" s="49"/>
+      <c r="BA21" s="49"/>
+      <c r="BB21" s="49"/>
+      <c r="BC21" s="49"/>
       <c r="BD21" s="42"/>
       <c r="BE21" s="42"/>
       <c r="BF21" s="42"/>
@@ -6257,7 +6261,7 @@
       <c r="BT21" s="43"/>
       <c r="BU21" s="42"/>
       <c r="BV21" s="38" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="BW21" s="38"/>
       <c r="BX21" s="38"/>
@@ -6313,10 +6317,10 @@
       <c r="B22" s="53"/>
       <c r="C22" s="54"/>
       <c r="D22" s="38" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="54"/>
@@ -6360,8 +6364,8 @@
       <c r="AS22" s="42"/>
       <c r="AT22" s="42"/>
       <c r="AU22" s="42"/>
-      <c r="AV22" s="42"/>
-      <c r="AW22" s="42"/>
+      <c r="AV22" s="49"/>
+      <c r="AW22" s="0"/>
       <c r="AX22" s="42"/>
       <c r="AY22" s="42"/>
       <c r="AZ22" s="42"/>
@@ -6387,7 +6391,7 @@
       <c r="BT22" s="43"/>
       <c r="BU22" s="42"/>
       <c r="BV22" s="38" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BW22" s="38"/>
       <c r="BX22" s="38"/>
@@ -6443,10 +6447,10 @@
       <c r="B23" s="53"/>
       <c r="C23" s="54"/>
       <c r="D23" s="38" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="54"/>
@@ -6517,7 +6521,7 @@
       <c r="BT23" s="43"/>
       <c r="BU23" s="42"/>
       <c r="BV23" s="38" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="BW23" s="38"/>
       <c r="BX23" s="38"/>
@@ -6573,10 +6577,10 @@
       <c r="B24" s="53"/>
       <c r="C24" s="54"/>
       <c r="D24" s="38" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="54"/>
@@ -6647,7 +6651,7 @@
       <c r="BT24" s="43"/>
       <c r="BU24" s="42"/>
       <c r="BV24" s="38" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="BW24" s="38"/>
       <c r="BX24" s="38"/>
@@ -6703,10 +6707,10 @@
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
       <c r="D25" s="38" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="54"/>
@@ -6831,10 +6835,10 @@
       <c r="B26" s="53"/>
       <c r="C26" s="54"/>
       <c r="D26" s="38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F26" s="53"/>
       <c r="G26" s="54"/>
@@ -6959,7 +6963,7 @@
       <c r="B27" s="53"/>
       <c r="C27" s="54"/>
       <c r="D27" s="42" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>151</v>
@@ -7087,10 +7091,10 @@
       <c r="B28" s="53"/>
       <c r="C28" s="54"/>
       <c r="D28" s="42" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F28" s="53"/>
       <c r="G28" s="54"/>
@@ -7215,10 +7219,10 @@
       <c r="B29" s="53"/>
       <c r="C29" s="54"/>
       <c r="D29" s="42" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="54"/>
@@ -7343,10 +7347,10 @@
       <c r="B30" s="53"/>
       <c r="C30" s="54"/>
       <c r="D30" s="38" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F30" s="53"/>
       <c r="G30" s="54"/>
@@ -7599,10 +7603,10 @@
       <c r="B32" s="53"/>
       <c r="C32" s="54"/>
       <c r="D32" s="38" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="54"/>
@@ -7727,10 +7731,10 @@
       <c r="B33" s="53"/>
       <c r="C33" s="54"/>
       <c r="D33" s="38" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F33" s="53"/>
       <c r="G33" s="54"/>
@@ -7983,10 +7987,10 @@
       <c r="B35" s="53"/>
       <c r="C35" s="54"/>
       <c r="D35" s="38" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F35" s="53"/>
       <c r="G35" s="54"/>
@@ -8111,10 +8115,10 @@
       <c r="B36" s="53"/>
       <c r="C36" s="54"/>
       <c r="D36" s="38" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E36" s="38" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F36" s="53"/>
       <c r="G36" s="54"/>
@@ -8239,10 +8243,10 @@
       <c r="B37" s="53"/>
       <c r="C37" s="54"/>
       <c r="D37" s="42" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F37" s="53"/>
       <c r="G37" s="54"/>
@@ -8367,10 +8371,10 @@
       <c r="B38" s="53"/>
       <c r="C38" s="54"/>
       <c r="D38" s="42" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F38" s="53"/>
       <c r="G38" s="54"/>
@@ -8495,10 +8499,10 @@
       <c r="B39" s="53"/>
       <c r="C39" s="54"/>
       <c r="D39" s="42" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="F39" s="53"/>
       <c r="G39" s="54"/>
@@ -8623,10 +8627,10 @@
       <c r="B40" s="53"/>
       <c r="C40" s="54"/>
       <c r="D40" s="38" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="F40" s="53"/>
       <c r="G40" s="54"/>
@@ -8751,10 +8755,10 @@
       <c r="B41" s="43"/>
       <c r="C41" s="42"/>
       <c r="D41" s="38" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F41" s="53"/>
       <c r="G41" s="54"/>
@@ -8879,10 +8883,10 @@
       <c r="B42" s="43"/>
       <c r="C42" s="42"/>
       <c r="D42" s="38" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F42" s="53"/>
       <c r="G42" s="54"/>
@@ -9007,10 +9011,10 @@
       <c r="B43" s="43"/>
       <c r="C43" s="42"/>
       <c r="D43" s="38" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="F43" s="53"/>
       <c r="G43" s="54"/>
@@ -9135,10 +9139,10 @@
       <c r="B44" s="43"/>
       <c r="C44" s="42"/>
       <c r="D44" s="38" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F44" s="43"/>
       <c r="G44" s="42"/>
@@ -9262,10 +9266,10 @@
       <c r="B45" s="43"/>
       <c r="C45" s="42"/>
       <c r="D45" s="38" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="F45" s="43"/>
       <c r="G45" s="42"/>
@@ -9389,10 +9393,10 @@
       <c r="B46" s="43"/>
       <c r="C46" s="42"/>
       <c r="D46" s="38" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="42"/>
@@ -9516,10 +9520,10 @@
       <c r="B47" s="43"/>
       <c r="C47" s="42"/>
       <c r="D47" s="38" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="42"/>
@@ -9885,7 +9889,7 @@
       <c r="DQ49" s="51"/>
       <c r="DR49" s="51"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -9894,6 +9898,8 @@
       <c r="U50" s="5"/>
       <c r="AI50" s="5"/>
       <c r="AS50" s="5"/>
+      <c r="AV50" s="42"/>
+      <c r="AW50" s="42"/>
       <c r="BU50" s="5"/>
       <c r="CA50" s="5"/>
       <c r="CF50" s="5"/>
@@ -10625,11 +10631,11 @@
     <mergeCell ref="A4:A44"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B83 D1:D3 F1:F5 H1:H83 J1:J83 L1:L83 N1:N83 P1:P83 R1:R83 T1:T83 V1:V83 X1:X83 Z1:Z83 AB1:AB83 AD1:AD83 AF1:AF83 AH1:AH83 AJ1:AJ83 AL1:AL83 AN1:AN83 AP1:AP83 AR1:AR83 AT1:AT83 AV1:AV83 AX1:AX83 AZ1:AZ83 BB1:BB83 BD1:BD83 BF1:BF3 BH1:BH3 BJ1:BJ3 BL1:BL83 BN1:BN83 BP1:BP3 BR1:BR83 BT1:BT83 BV1:BV83 BX1:BX83 BZ1:BZ83 CB1:CB83 CD1:CD83 CF1:CF83 CH1:CH83 CJ1:CJ83 CL1:CL83 CN1:CN83 CP1:AMJ83 E4:P5 AI4:AL4 CA4:CF6 AI5:AJ6 BH5:BH83 E6:E47 G6:H20 BF6:BF83 BJ6:BJ83 BP8:BP83 F21:F83 D50:D83" type="none">
+    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B83 D1:D3 F1:F5 H1:H83 J1:J83 L1:L83 N1:N83 P1:P83 R1:R83 T1:T83 V1:V83 X1:X83 Z1:Z83 AB1:AB83 AD1:AD83 AF1:AF83 AH1:AH83 AJ1:AJ83 AL1:AL83 AN1:AN83 AP1:AP83 AR1:AR83 AT1:AT83 AV1:AV20 AX1:AX83 AZ1:AZ83 BB1:BB83 BD1:BD83 BF1:BF3 BH1:BH3 BJ1:BJ3 BL1:BL83 BN1:BN83 BP1:BP3 BR1:BR83 BT1:BT83 BV1:BV83 BX1:BX83 BZ1:BZ83 CB1:CB83 CD1:CD83 CF1:CF83 CH1:CH83 CJ1:CJ83 CL1:CL83 CN1:CN83 CP1:AMJ83 E4:P5 AI4:AL4 CA4:CF6 AI5:AJ6 BH5:BH83 E6:E47 G6:H20 BF6:BF83 BJ6:BJ83 BP8:BP83 F21:F83 AV22:AV83 D50:D83" type="none">
       <formula1>20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C83 E1:E3 G1:G3 I1:I3 K1:K3 M1:M3 O1:O3 Q1:Q83 S1:S83 U1:U83 W1:W83 Y1:Y83 AA1:AA83 AC1:AC83 AE1:AE83 AG1:AG83 AI1:AI3 AK1:AK3 AM1:AM83 AO1:AO83 AQ1:AQ83 AS1:AS83 AU1:AU83 AW1:AW83 AY1:AY83 BA1:BA83 BC1:BC83 BE1:BE83 BG1:BG83 BI1:BI83 BK1:BK83 BM1:BM83 BO1:BO83 BQ1:BQ83 BS1:BS83 BU1:BU83 BW1:BW83 BY1:BY83 CA1:CA3 CC1:CC3 CE1:CE3 CG1:CG83 CI1:CI83 CK1:CK83 CM1:CM83 CO1:CO83 AK5:AK83 I6:I83 K6:K83 M6:M83 O6:O83 AI7:AI83 CA7:CA83 CC7:CC83 CE7:CE83 G21:G83 E50:E83" type="textLength">
+    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C83 E1:E3 G1:G3 I1:I3 K1:K3 M1:M3 O1:O3 Q1:Q83 S1:S83 U1:U83 W1:W83 Y1:Y83 AA1:AA83 AC1:AC83 AE1:AE83 AG1:AG83 AI1:AI3 AK1:AK3 AM1:AM83 AO1:AO83 AQ1:AQ83 AS1:AS83 AU1:AU83 AW1:AW20 AY1:AY83 BA1:BA83 BC1:BC83 BE1:BE83 BG1:BG83 BI1:BI83 BK1:BK83 BM1:BM83 BO1:BO83 BQ1:BQ83 BS1:BS83 BU1:BU83 BW1:BW83 BY1:BY83 CA1:CA3 CC1:CC3 CE1:CE3 CG1:CG83 CI1:CI83 CK1:CK83 CM1:CM83 CO1:CO83 AK5:AK83 I6:I83 K6:K83 M6:M83 O6:O83 AI7:AI83 CA7:CA83 CC7:CC83 CE7:CE83 G21:G83 AW23:AW83 E50:E83" type="textLength">
       <formula1>20</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Added some more subsamples
</commit_message>
<xml_diff>
--- a/Sample_and_gear_types_AeN.xlsx
+++ b/Sample_and_gear_types_AeN.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="257">
   <si>
     <t xml:space="preserve">Sample Group</t>
   </si>
@@ -295,183 +295,189 @@
     <t xml:space="preserve">Gelationous zooplankton abundance</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrozooplankton carbohydrat</t>
+    <t xml:space="preserve">Macrozooplankton ecotox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop ecotox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC/PON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists microscopy &gt; 10 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists micros&gt;10um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists microscopy &gt; 20 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists micros&gt;20um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacterial production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacterial prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Ice core section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice core section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density/Abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Algal pigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algal pigments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozooplankton abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozoop abun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microzooplankton abundance, lugol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microzoop abun,lugol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozooplankton biomass, live</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozoop mass, live</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton carbohydrat</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop carhyd</t>
   </si>
   <si>
-    <t xml:space="preserve">POC/PON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists microscopy &gt; 10 um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists micros&gt;10um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists microscopy &gt; 20 um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists micros&gt;20um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacterial production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacterial prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Ice core section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice core section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Density/Abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Algal pigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algal pigments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paleo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozooplankton abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozoop abun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microzooplankton abundance, lugol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microzoop abun,lugol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozooplankton biomass, live</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozoop mass, live</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton energetics</t>
+    <t xml:space="preserve">Protist community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protist PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice algal taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Bacterial production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Barcoding samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barcoding samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gelationous zooplankton taxonomy, ethanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gel zoop tax, EtOH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozooplankton biomass, weighed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozoop mass, wei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton energetics</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop energ</t>
   </si>
   <si>
-    <t xml:space="preserve">Protist community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist PCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice algal taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Bacterial production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Barcoding samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barcoding samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gelationous zooplankton taxonomy, ethanol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gel zoop tax, EtOH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozooplankton biomass, weighed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozoop mass, wei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton fatty acid</t>
+    <t xml:space="preserve">Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chl a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microalgal culturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biogenic silica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Chlorophyll a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Food web samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food web samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gelationous zooplankton taxonomy, formaldehyde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gel zoop tax, form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozooplankton genetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesozoop genetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton fatty acid</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop fatty acid</t>
   </si>
   <si>
-    <t xml:space="preserve">Chlorophyll a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chl a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microalgal culturing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biogenic silica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Chlorophyll a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Food web samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food web samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gelationous zooplankton taxonomy, formaldehyde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gel zoop tax, form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozooplankton genetics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesozoop genetics</t>
+    <t xml:space="preserve">Benthic foraminifera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromoform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,Foraminifera experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foraminifera exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozooplankton abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrozoop abun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton hg</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozooplankton hg</t>
   </si>
   <si>
-    <t xml:space="preserve">Benthic foraminifera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bromoform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Iron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,Foraminifera experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foraminifera exp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton abundance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozoop abun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton organic pollutio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dating</t>
   </si>
   <si>
@@ -496,63 +502,60 @@
     <t xml:space="preserve">Macrozoop biomass</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrozooplankton protein</t>
+    <t xml:space="preserve">1, Macrozooplankton organic pollutio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diatoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meiofauna taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, PicoNanoEpifluorenscens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PicoNanoEpifluo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Organic carbon/nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic C/N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton protein</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop org pol</t>
   </si>
   <si>
-    <t xml:space="preserve">Diatoms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meiofauna taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, PicoNanoEpifluorenscens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PicoNanoEpifluo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Organic carbon/nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic C/N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Macrozooplankton carbohydrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrozooplankton stable isotope</t>
+    <t xml:space="preserve">Dinocysts, ancient DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scavenger taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deltaO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, PicoNanoFlowcytometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PicoNanoFlowcyt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Macrozooplankton stable isotope</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop isotope</t>
   </si>
   <si>
-    <t xml:space="preserve">Dinocysts, ancient DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scavenger taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deltaO18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, PicoNanoFlowcytometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PicoNanoFlowcyt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Macrozooplankton energetics</t>
-  </si>
-  <si>
     <t xml:space="preserve">HBIs and coccoliths</t>
   </si>
   <si>
@@ -574,9 +577,6 @@
     <t xml:space="preserve">Pore water content</t>
   </si>
   <si>
-    <t xml:space="preserve">1, Macrozooplankton fatty acid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lithological description</t>
   </si>
   <si>
@@ -601,31 +601,55 @@
     <t xml:space="preserve">Quanti macrofauna</t>
   </si>
   <si>
+    <t xml:space="preserve">magnetic susceptibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable isotopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prokaryote RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Respiration experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiration exp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Macrozooplankton genetics</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop genetics </t>
   </si>
   <si>
-    <t xml:space="preserve">magnetic susceptibility </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stable isotopes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Prokaryote RNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prokaryote RNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Respiration experiments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respiration exp</t>
+    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suction pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC/DON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protist DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Sediment stable isotopes, carbon and nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sed isotopes, C, N</t>
   </si>
   <si>
     <t xml:space="preserve">1, Macrozooplankton gonad </t>
@@ -634,54 +658,24 @@
     <t xml:space="preserve">Macrozoop gonad </t>
   </si>
   <si>
-    <t xml:space="preserve">Pteropod shell condition, shell density and size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen profiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suction pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC/DON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Protist DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protist DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Sediment stable isotopes, carbon and nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sed isotopes, C, N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Macrozooplankton hg</t>
+    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoop physiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecotoxicology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist microscopy &lt;  um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protists micros&lt;10um</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop hg</t>
   </si>
   <si>
-    <t xml:space="preserve">Planktonic foraminifera species abundance and species composition, state of shell dissolution and shell thickness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoop physiology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecotoxicology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Protist microscopy &lt;  um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protists micros&lt;10um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Macrozooplankton stable isotope</t>
-  </si>
-  <si>
     <t xml:space="preserve">Planktic foraminifera</t>
   </si>
   <si>
@@ -697,24 +691,21 @@
     <t xml:space="preserve">1 ,Protist microscopy &gt; 10 um</t>
   </si>
   <si>
+    <t xml:space="preserve">Pore water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grazing on bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Protist PCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">1, Macrozooplankton nutrition</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop nutrition</t>
   </si>
   <si>
-    <t xml:space="preserve">Pore water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grazing on bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Protist PCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Macrozooplankton organic pollutio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
@@ -727,31 +718,28 @@
     <t xml:space="preserve">Silicate incorp</t>
   </si>
   <si>
-    <t xml:space="preserve">1, Macrozooplankton protein</t>
+    <t xml:space="preserve">Sediment geochemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Virus DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virus DNA</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozoop protein</t>
   </si>
   <si>
-    <t xml:space="preserve">Sediment geochemistry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, Virus DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virus DNA</t>
+    <t xml:space="preserve">Sediment grain size</t>
   </si>
   <si>
     <t xml:space="preserve">1, Macrozoplankton stomach</t>
   </si>
   <si>
     <t xml:space="preserve">Macrozop stomach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment grain size</t>
   </si>
   <si>
     <t xml:space="preserve">Sedimentology</t>
@@ -1347,6 +1335,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1372,10 +1364,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1511,7 +1499,7 @@
       <xdr:col>61</xdr:col>
       <xdr:colOff>89280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,7 +1509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="58588200" y="5300280"/>
-          <a:ext cx="3061080" cy="1347840"/>
+          <a:ext cx="3061080" cy="1357560"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1546,7 +1534,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>357120</xdr:rowOff>
     </xdr:from>
@@ -1563,8 +1551,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="72457200" y="3399840"/>
-          <a:ext cx="4051440" cy="429120"/>
+          <a:off x="73298880" y="3399840"/>
+          <a:ext cx="4051800" cy="429120"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1589,7 +1577,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>356400</xdr:rowOff>
     </xdr:from>
@@ -1606,8 +1594,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="72457200" y="4159800"/>
-          <a:ext cx="4051440" cy="429840"/>
+          <a:off x="73298880" y="4159800"/>
+          <a:ext cx="4051800" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1632,7 +1620,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>355680</xdr:rowOff>
     </xdr:from>
@@ -1649,8 +1637,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="72457200" y="4539600"/>
-          <a:ext cx="4051440" cy="429480"/>
+          <a:off x="73298880" y="4539600"/>
+          <a:ext cx="4051800" cy="429480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1675,7 +1663,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>356400</xdr:rowOff>
     </xdr:from>
@@ -1683,7 +1671,7 @@
       <xdr:col>76</xdr:col>
       <xdr:colOff>89640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1692,8 +1680,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="72457200" y="5681160"/>
-          <a:ext cx="4051440" cy="1346760"/>
+          <a:off x="73298880" y="5681160"/>
+          <a:ext cx="4051800" cy="1356120"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1718,15 +1706,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>72</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>349920</xdr:rowOff>
+      <xdr:rowOff>356400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
       <xdr:colOff>89640</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1735,8 +1723,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="72457200" y="7740000"/>
-          <a:ext cx="4051440" cy="429840"/>
+          <a:off x="73298880" y="7749360"/>
+          <a:ext cx="4051800" cy="429840"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1768,8 +1756,8 @@
   </sheetPr>
   <dimension ref="1:83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BI1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BQ14" activeCellId="0" sqref="BQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1789,7 +1777,9 @@
     <col collapsed="false" hidden="false" max="45" min="44" style="2" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="47" min="46" style="5" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="48" min="48" style="5" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="71" min="49" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="69" min="49" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="70" min="70" style="5" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="5" width="20.5612244897959"/>
     <col collapsed="false" hidden="false" max="73" min="72" style="2" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="77" min="74" style="4" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="79" min="78" style="2" width="14.0408163265306"/>
@@ -3494,10 +3484,10 @@
       <c r="BQ4" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="BR4" s="42" t="s">
+      <c r="BR4" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="BS4" s="42" t="s">
+      <c r="BS4" s="0" t="s">
         <v>80</v>
       </c>
       <c r="BT4" s="43"/>
@@ -3722,10 +3712,10 @@
       <c r="BQ5" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="BR5" s="42" t="s">
+      <c r="BR5" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="BS5" s="42" t="s">
+      <c r="BS5" s="58" t="s">
         <v>101</v>
       </c>
       <c r="BT5" s="43"/>
@@ -3778,7 +3768,7 @@
         <v>104</v>
       </c>
       <c r="CQ5" s="38"/>
-      <c r="CR5" s="58"/>
+      <c r="CR5" s="59"/>
       <c r="CS5" s="51"/>
       <c r="CT5" s="51"/>
       <c r="CU5" s="51"/>
@@ -3816,10 +3806,10 @@
       <c r="E6" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="61" t="s">
         <v>87</v>
       </c>
       <c r="H6" s="38"/>
@@ -3833,7 +3823,7 @@
       <c r="P6" s="42"/>
       <c r="Q6" s="42"/>
       <c r="R6" s="42"/>
-      <c r="S6" s="61"/>
+      <c r="S6" s="62"/>
       <c r="T6" s="42"/>
       <c r="U6" s="42"/>
       <c r="V6" s="42"/>
@@ -3920,10 +3910,10 @@
       <c r="BQ6" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="BR6" s="42" t="s">
+      <c r="BR6" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="BS6" s="42" t="s">
+      <c r="BS6" s="58" t="s">
         <v>115</v>
       </c>
       <c r="BT6" s="43"/>
@@ -3974,7 +3964,7 @@
       <c r="CO6" s="42"/>
       <c r="CP6" s="38"/>
       <c r="CQ6" s="38"/>
-      <c r="CR6" s="58"/>
+      <c r="CR6" s="59"/>
       <c r="CS6" s="51"/>
       <c r="CT6" s="51"/>
       <c r="CU6" s="51"/>
@@ -4012,10 +4002,10 @@
       <c r="E7" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="61" t="s">
         <v>117</v>
       </c>
       <c r="H7" s="45"/>
@@ -4029,7 +4019,7 @@
       <c r="P7" s="42"/>
       <c r="Q7" s="42"/>
       <c r="R7" s="42"/>
-      <c r="S7" s="61"/>
+      <c r="S7" s="62"/>
       <c r="T7" s="42"/>
       <c r="U7" s="42"/>
       <c r="V7" s="42"/>
@@ -4104,16 +4094,16 @@
       <c r="BQ7" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="BR7" s="45" t="s">
+      <c r="BR7" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="BS7" s="42" t="s">
-        <v>127</v>
+      <c r="BS7" s="58" t="s">
+        <v>128</v>
       </c>
       <c r="BT7" s="43"/>
       <c r="BU7" s="42"/>
       <c r="BV7" s="38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BW7" s="38"/>
       <c r="BX7" s="38"/>
@@ -4123,22 +4113,22 @@
       <c r="CB7" s="38"/>
       <c r="CC7" s="38"/>
       <c r="CD7" s="38"/>
-      <c r="CE7" s="61"/>
+      <c r="CE7" s="62"/>
       <c r="CF7" s="42"/>
       <c r="CG7" s="42"/>
       <c r="CH7" s="42"/>
       <c r="CI7" s="42"/>
-      <c r="CJ7" s="62"/>
-      <c r="CK7" s="63"/>
-      <c r="CL7" s="63"/>
-      <c r="CM7" s="63"/>
-      <c r="CN7" s="62"/>
+      <c r="CJ7" s="63"/>
+      <c r="CK7" s="64"/>
+      <c r="CL7" s="64"/>
+      <c r="CM7" s="64"/>
+      <c r="CN7" s="63"/>
       <c r="CO7" s="42"/>
       <c r="CP7" s="38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="CQ7" s="38"/>
-      <c r="CR7" s="58"/>
+      <c r="CR7" s="59"/>
       <c r="CS7" s="51"/>
       <c r="CT7" s="51"/>
       <c r="CU7" s="51"/>
@@ -4171,16 +4161,16 @@
       <c r="B8" s="53"/>
       <c r="C8" s="54"/>
       <c r="D8" s="38" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="F8" s="65" t="s">
         <v>132</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>133</v>
       </c>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
@@ -4193,7 +4183,7 @@
       <c r="P8" s="42"/>
       <c r="Q8" s="42"/>
       <c r="R8" s="42"/>
-      <c r="S8" s="61"/>
+      <c r="S8" s="62"/>
       <c r="T8" s="42"/>
       <c r="U8" s="42"/>
       <c r="V8" s="42"/>
@@ -4211,10 +4201,10 @@
       <c r="AH8" s="43"/>
       <c r="AI8" s="42"/>
       <c r="AJ8" s="57" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AK8" s="57" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AL8" s="45"/>
       <c r="AM8" s="45"/>
@@ -4227,28 +4217,28 @@
       <c r="AT8" s="42"/>
       <c r="AU8" s="42"/>
       <c r="AV8" s="40" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AW8" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX8" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="AX8" s="40" t="s">
-        <v>135</v>
-      </c>
       <c r="AY8" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ8" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="AZ8" s="40" t="s">
-        <v>135</v>
-      </c>
       <c r="BA8" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB8" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="BB8" s="40" t="s">
-        <v>135</v>
-      </c>
       <c r="BC8" s="40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BD8" s="42"/>
       <c r="BE8" s="42"/>
@@ -4264,16 +4254,16 @@
       <c r="BO8" s="42"/>
       <c r="BP8" s="42"/>
       <c r="BQ8" s="42"/>
-      <c r="BR8" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="BS8" s="42" t="s">
-        <v>115</v>
+      <c r="BR8" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="BS8" s="58" t="s">
+        <v>139</v>
       </c>
       <c r="BT8" s="43"/>
       <c r="BU8" s="42"/>
       <c r="BV8" s="38" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BW8" s="38"/>
       <c r="BX8" s="38"/>
@@ -4283,7 +4273,7 @@
       <c r="CB8" s="38"/>
       <c r="CC8" s="38"/>
       <c r="CD8" s="38"/>
-      <c r="CE8" s="61"/>
+      <c r="CE8" s="62"/>
       <c r="CF8" s="42"/>
       <c r="CG8" s="42"/>
       <c r="CH8" s="42"/>
@@ -4295,10 +4285,10 @@
       <c r="CN8" s="43"/>
       <c r="CO8" s="42"/>
       <c r="CP8" s="38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="CQ8" s="38"/>
-      <c r="CR8" s="58"/>
+      <c r="CR8" s="59"/>
       <c r="CS8" s="51"/>
       <c r="CT8" s="51"/>
       <c r="CU8" s="51"/>
@@ -4331,15 +4321,15 @@
       <c r="B9" s="53"/>
       <c r="C9" s="54"/>
       <c r="D9" s="38" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="F9" s="59" t="s">
-        <v>141</v>
-      </c>
-      <c r="G9" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="61" t="s">
         <v>118</v>
       </c>
       <c r="H9" s="38"/>
@@ -4353,7 +4343,7 @@
       <c r="P9" s="42"/>
       <c r="Q9" s="42"/>
       <c r="R9" s="42"/>
-      <c r="S9" s="61"/>
+      <c r="S9" s="62"/>
       <c r="T9" s="42"/>
       <c r="U9" s="42"/>
       <c r="V9" s="42"/>
@@ -4371,10 +4361,10 @@
       <c r="AH9" s="43"/>
       <c r="AI9" s="42"/>
       <c r="AJ9" s="57" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AK9" s="57" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AL9" s="45"/>
       <c r="AM9" s="45"/>
@@ -4387,28 +4377,28 @@
       <c r="AT9" s="42"/>
       <c r="AU9" s="42"/>
       <c r="AV9" s="40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AW9" s="40" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AX9" s="40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AY9" s="40" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AZ9" s="40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="BA9" s="40" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="BB9" s="40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="BC9" s="40" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="BD9" s="42"/>
       <c r="BE9" s="42"/>
@@ -4424,16 +4414,16 @@
       <c r="BO9" s="42"/>
       <c r="BP9" s="42"/>
       <c r="BQ9" s="42"/>
-      <c r="BR9" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="BS9" s="42" t="s">
-        <v>147</v>
+      <c r="BR9" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="BS9" s="58" t="s">
+        <v>128</v>
       </c>
       <c r="BT9" s="43"/>
       <c r="BU9" s="42"/>
       <c r="BV9" s="38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="BW9" s="38"/>
       <c r="BX9" s="38"/>
@@ -4443,7 +4433,7 @@
       <c r="CB9" s="38"/>
       <c r="CC9" s="38"/>
       <c r="CD9" s="38"/>
-      <c r="CE9" s="61"/>
+      <c r="CE9" s="62"/>
       <c r="CF9" s="42"/>
       <c r="CG9" s="42"/>
       <c r="CH9" s="42"/>
@@ -4455,10 +4445,10 @@
       <c r="CN9" s="43"/>
       <c r="CO9" s="42"/>
       <c r="CP9" s="38" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="CQ9" s="38"/>
-      <c r="CR9" s="58"/>
+      <c r="CR9" s="59"/>
       <c r="CS9" s="51"/>
       <c r="CT9" s="51"/>
       <c r="CU9" s="51"/>
@@ -4496,11 +4486,11 @@
       <c r="E10" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="60" t="s">
+      <c r="F10" s="60" t="s">
         <v>151</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
@@ -4513,7 +4503,7 @@
       <c r="P10" s="42"/>
       <c r="Q10" s="42"/>
       <c r="R10" s="42"/>
-      <c r="S10" s="61"/>
+      <c r="S10" s="62"/>
       <c r="T10" s="42"/>
       <c r="U10" s="42"/>
       <c r="V10" s="42"/>
@@ -4531,10 +4521,10 @@
       <c r="AH10" s="43"/>
       <c r="AI10" s="42"/>
       <c r="AJ10" s="57" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK10" s="57" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL10" s="45"/>
       <c r="AM10" s="45"/>
@@ -4546,28 +4536,28 @@
       <c r="AS10" s="42"/>
       <c r="AT10" s="42"/>
       <c r="AU10" s="42"/>
-      <c r="AV10" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW10" s="56" t="s">
+      <c r="AV10" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW10" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="AX10" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="AY10" s="56" t="s">
+      <c r="AX10" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY10" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="AZ10" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA10" s="56" t="s">
+      <c r="AZ10" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA10" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="BB10" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC10" s="56" t="s">
+      <c r="BB10" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC10" s="40" t="s">
         <v>80</v>
       </c>
       <c r="BD10" s="42"/>
@@ -4584,10 +4574,10 @@
       <c r="BO10" s="42"/>
       <c r="BP10" s="42"/>
       <c r="BQ10" s="42"/>
-      <c r="BR10" s="42" t="s">
+      <c r="BR10" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="BS10" s="42" t="s">
+      <c r="BS10" s="58" t="s">
         <v>156</v>
       </c>
       <c r="BT10" s="43"/>
@@ -4603,7 +4593,7 @@
       <c r="CB10" s="38"/>
       <c r="CC10" s="38"/>
       <c r="CD10" s="38"/>
-      <c r="CE10" s="61"/>
+      <c r="CE10" s="62"/>
       <c r="CF10" s="42"/>
       <c r="CG10" s="42"/>
       <c r="CH10" s="42"/>
@@ -4618,7 +4608,7 @@
         <v>158</v>
       </c>
       <c r="CQ10" s="38"/>
-      <c r="CR10" s="58"/>
+      <c r="CR10" s="59"/>
       <c r="CS10" s="51"/>
       <c r="CT10" s="51"/>
       <c r="CU10" s="51"/>
@@ -4656,10 +4646,10 @@
       <c r="E11" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="58" t="s">
         <v>161</v>
       </c>
       <c r="H11" s="38"/>
@@ -4673,7 +4663,7 @@
       <c r="P11" s="42"/>
       <c r="Q11" s="42"/>
       <c r="R11" s="42"/>
-      <c r="S11" s="61"/>
+      <c r="S11" s="62"/>
       <c r="T11" s="42"/>
       <c r="U11" s="42"/>
       <c r="V11" s="42"/>
@@ -4707,25 +4697,25 @@
       <c r="AT11" s="42"/>
       <c r="AU11" s="42"/>
       <c r="AV11" s="56" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="AW11" s="56" t="s">
         <v>101</v>
       </c>
       <c r="AX11" s="56" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="AY11" s="56" t="s">
         <v>101</v>
       </c>
       <c r="AZ11" s="56" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="BA11" s="56" t="s">
         <v>101</v>
       </c>
       <c r="BB11" s="56" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="BC11" s="56" t="s">
         <v>101</v>
@@ -4744,12 +4734,16 @@
       <c r="BO11" s="42"/>
       <c r="BP11" s="42"/>
       <c r="BQ11" s="42"/>
-      <c r="BR11" s="42"/>
-      <c r="BS11" s="42"/>
+      <c r="BR11" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="BS11" s="58" t="s">
+        <v>165</v>
+      </c>
       <c r="BT11" s="43"/>
       <c r="BU11" s="42"/>
       <c r="BV11" s="38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="BW11" s="38"/>
       <c r="BX11" s="38"/>
@@ -4759,7 +4753,7 @@
       <c r="CB11" s="38"/>
       <c r="CC11" s="38"/>
       <c r="CD11" s="38"/>
-      <c r="CE11" s="61"/>
+      <c r="CE11" s="62"/>
       <c r="CF11" s="42"/>
       <c r="CG11" s="42"/>
       <c r="CH11" s="42"/>
@@ -4771,10 +4765,10 @@
       <c r="CN11" s="43"/>
       <c r="CO11" s="42"/>
       <c r="CP11" s="38" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CQ11" s="38"/>
-      <c r="CR11" s="58"/>
+      <c r="CR11" s="59"/>
       <c r="CS11" s="51"/>
       <c r="CT11" s="51"/>
       <c r="CU11" s="51"/>
@@ -4807,16 +4801,16 @@
       <c r="B12" s="53"/>
       <c r="C12" s="54"/>
       <c r="D12" s="38" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="F12" s="60" t="s">
         <v>169</v>
+      </c>
+      <c r="G12" s="61" t="s">
+        <v>170</v>
       </c>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
@@ -4829,7 +4823,7 @@
       <c r="P12" s="42"/>
       <c r="Q12" s="42"/>
       <c r="R12" s="42"/>
-      <c r="S12" s="61"/>
+      <c r="S12" s="62"/>
       <c r="T12" s="42"/>
       <c r="U12" s="42"/>
       <c r="V12" s="42"/>
@@ -4847,10 +4841,10 @@
       <c r="AH12" s="43"/>
       <c r="AI12" s="42"/>
       <c r="AJ12" s="57" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AK12" s="57" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AL12" s="45"/>
       <c r="AM12" s="45"/>
@@ -4863,25 +4857,25 @@
       <c r="AT12" s="42"/>
       <c r="AU12" s="42"/>
       <c r="AV12" s="56" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="AW12" s="56" t="s">
         <v>115</v>
       </c>
       <c r="AX12" s="56" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="AY12" s="56" t="s">
         <v>115</v>
       </c>
       <c r="AZ12" s="56" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="BA12" s="56" t="s">
         <v>115</v>
       </c>
       <c r="BB12" s="56" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="BC12" s="56" t="s">
         <v>115</v>
@@ -4915,7 +4909,7 @@
       <c r="CB12" s="38"/>
       <c r="CC12" s="38"/>
       <c r="CD12" s="38"/>
-      <c r="CE12" s="61"/>
+      <c r="CE12" s="62"/>
       <c r="CF12" s="42"/>
       <c r="CG12" s="42"/>
       <c r="CH12" s="42"/>
@@ -4930,7 +4924,7 @@
         <v>174</v>
       </c>
       <c r="CQ12" s="38"/>
-      <c r="CR12" s="58"/>
+      <c r="CR12" s="59"/>
       <c r="CS12" s="43"/>
       <c r="CT12" s="51"/>
       <c r="CU12" s="51"/>
@@ -4968,10 +4962,10 @@
       <c r="E13" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="G13" s="60" t="s">
+      <c r="G13" s="61" t="s">
         <v>178</v>
       </c>
       <c r="H13" s="38"/>
@@ -4985,7 +4979,7 @@
       <c r="P13" s="42"/>
       <c r="Q13" s="42"/>
       <c r="R13" s="42"/>
-      <c r="S13" s="61"/>
+      <c r="S13" s="62"/>
       <c r="T13" s="42"/>
       <c r="U13" s="42"/>
       <c r="V13" s="42"/>
@@ -5018,29 +5012,29 @@
       <c r="AS13" s="42"/>
       <c r="AT13" s="42"/>
       <c r="AU13" s="42"/>
-      <c r="AV13" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="AW13" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="AX13" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="AY13" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="AZ13" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="BA13" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="BB13" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="BC13" s="40" t="s">
-        <v>182</v>
+      <c r="AV13" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW13" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX13" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY13" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ13" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="BA13" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="BB13" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC13" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="BD13" s="42"/>
       <c r="BE13" s="42"/>
@@ -5061,7 +5055,7 @@
       <c r="BT13" s="43"/>
       <c r="BU13" s="42"/>
       <c r="BV13" s="38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="BW13" s="38"/>
       <c r="BX13" s="38"/>
@@ -5071,7 +5065,7 @@
       <c r="CB13" s="38"/>
       <c r="CC13" s="38"/>
       <c r="CD13" s="38"/>
-      <c r="CE13" s="61"/>
+      <c r="CE13" s="62"/>
       <c r="CF13" s="42"/>
       <c r="CG13" s="42"/>
       <c r="CH13" s="42"/>
@@ -5083,10 +5077,10 @@
       <c r="CN13" s="43"/>
       <c r="CO13" s="42"/>
       <c r="CP13" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="CQ13" s="38"/>
-      <c r="CR13" s="58"/>
+      <c r="CR13" s="59"/>
       <c r="CS13" s="43"/>
       <c r="CT13" s="51"/>
       <c r="CU13" s="51"/>
@@ -5119,16 +5113,16 @@
       <c r="B14" s="53"/>
       <c r="C14" s="54"/>
       <c r="D14" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="61" t="s">
         <v>185</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="G14" s="60" t="s">
-        <v>187</v>
       </c>
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
@@ -5141,7 +5135,7 @@
       <c r="P14" s="42"/>
       <c r="Q14" s="42"/>
       <c r="R14" s="42"/>
-      <c r="S14" s="61"/>
+      <c r="S14" s="62"/>
       <c r="T14" s="42"/>
       <c r="U14" s="42"/>
       <c r="V14" s="42"/>
@@ -5159,10 +5153,10 @@
       <c r="AH14" s="53"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="57" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AK14" s="57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AL14" s="45"/>
       <c r="AM14" s="45"/>
@@ -5174,36 +5168,36 @@
       <c r="AS14" s="42"/>
       <c r="AT14" s="42"/>
       <c r="AU14" s="42"/>
-      <c r="AV14" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="AW14" s="56" t="s">
-        <v>191</v>
-      </c>
-      <c r="AX14" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY14" s="56" t="s">
-        <v>191</v>
-      </c>
-      <c r="AZ14" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="BA14" s="56" t="s">
-        <v>191</v>
-      </c>
-      <c r="BB14" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="BC14" s="56" t="s">
-        <v>191</v>
+      <c r="AV14" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="AW14" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX14" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="AY14" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="AZ14" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA14" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB14" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="BC14" s="40" t="s">
+        <v>189</v>
       </c>
       <c r="BD14" s="42"/>
       <c r="BE14" s="42"/>
       <c r="BF14" s="42"/>
       <c r="BG14" s="42"/>
       <c r="BH14" s="42" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="BI14" s="42"/>
       <c r="BJ14" s="42"/>
@@ -5219,7 +5213,7 @@
       <c r="BT14" s="43"/>
       <c r="BU14" s="42"/>
       <c r="BV14" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="BW14" s="38"/>
       <c r="BX14" s="38"/>
@@ -5229,7 +5223,7 @@
       <c r="CB14" s="38"/>
       <c r="CC14" s="38"/>
       <c r="CD14" s="38"/>
-      <c r="CE14" s="61"/>
+      <c r="CE14" s="62"/>
       <c r="CF14" s="42"/>
       <c r="CG14" s="42"/>
       <c r="CH14" s="42"/>
@@ -5241,10 +5235,10 @@
       <c r="CN14" s="43"/>
       <c r="CO14" s="42"/>
       <c r="CP14" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="CQ14" s="38"/>
-      <c r="CR14" s="58"/>
+      <c r="CR14" s="59"/>
       <c r="CS14" s="51"/>
       <c r="CT14" s="51"/>
       <c r="CU14" s="51"/>
@@ -5272,21 +5266,21 @@
       <c r="DQ14" s="51"/>
       <c r="DR14" s="51"/>
     </row>
-    <row r="15" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35"/>
       <c r="B15" s="53"/>
       <c r="C15" s="54"/>
       <c r="D15" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="G15" s="61" t="s">
         <v>195</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G15" s="60" t="s">
-        <v>197</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
@@ -5299,7 +5293,7 @@
       <c r="P15" s="42"/>
       <c r="Q15" s="42"/>
       <c r="R15" s="42"/>
-      <c r="S15" s="61"/>
+      <c r="S15" s="62"/>
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
       <c r="V15" s="42"/>
@@ -5317,10 +5311,10 @@
       <c r="AH15" s="53"/>
       <c r="AI15" s="54"/>
       <c r="AJ15" s="57" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK15" s="57" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AL15" s="45"/>
       <c r="AM15" s="45"/>
@@ -5333,35 +5327,35 @@
       <c r="AT15" s="42"/>
       <c r="AU15" s="42"/>
       <c r="AV15" s="56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AW15" s="56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AX15" s="56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AY15" s="56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AZ15" s="56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BA15" s="56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BB15" s="56" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BC15" s="56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BD15" s="42"/>
       <c r="BE15" s="42"/>
       <c r="BF15" s="42"/>
       <c r="BG15" s="42"/>
       <c r="BH15" s="42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BI15" s="42"/>
       <c r="BJ15" s="42"/>
@@ -5387,7 +5381,7 @@
       <c r="CB15" s="38"/>
       <c r="CC15" s="38"/>
       <c r="CD15" s="38"/>
-      <c r="CE15" s="61"/>
+      <c r="CE15" s="62"/>
       <c r="CF15" s="42"/>
       <c r="CG15" s="42"/>
       <c r="CH15" s="42"/>
@@ -5399,10 +5393,10 @@
       <c r="CN15" s="43"/>
       <c r="CO15" s="42"/>
       <c r="CP15" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="CQ15" s="38"/>
-      <c r="CR15" s="58"/>
+      <c r="CR15" s="59"/>
       <c r="CS15" s="51"/>
       <c r="CT15" s="51"/>
       <c r="CU15" s="51"/>
@@ -5435,16 +5429,16 @@
       <c r="B16" s="53"/>
       <c r="C16" s="54"/>
       <c r="D16" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="G16" s="58" t="s">
         <v>204</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="F16" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>206</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
@@ -5457,7 +5451,7 @@
       <c r="P16" s="42"/>
       <c r="Q16" s="42"/>
       <c r="R16" s="42"/>
-      <c r="S16" s="61"/>
+      <c r="S16" s="62"/>
       <c r="T16" s="42"/>
       <c r="U16" s="42"/>
       <c r="V16" s="42"/>
@@ -5487,28 +5481,28 @@
       <c r="AT16" s="42"/>
       <c r="AU16" s="42"/>
       <c r="AV16" s="56" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="AW16" s="56" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="AX16" s="56" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="AY16" s="56" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="AZ16" s="56" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="BA16" s="56" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="BB16" s="56" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="BC16" s="56" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="BD16" s="42"/>
       <c r="BE16" s="42"/>
@@ -5529,7 +5523,7 @@
       <c r="BT16" s="43"/>
       <c r="BU16" s="42"/>
       <c r="BV16" s="38" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="BW16" s="38"/>
       <c r="BX16" s="38"/>
@@ -5539,7 +5533,7 @@
       <c r="CB16" s="38"/>
       <c r="CC16" s="38"/>
       <c r="CD16" s="38"/>
-      <c r="CE16" s="61"/>
+      <c r="CE16" s="62"/>
       <c r="CF16" s="42"/>
       <c r="CG16" s="42"/>
       <c r="CH16" s="42"/>
@@ -5551,10 +5545,10 @@
       <c r="CN16" s="43"/>
       <c r="CO16" s="42"/>
       <c r="CP16" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="CQ16" s="38"/>
-      <c r="CR16" s="58"/>
+      <c r="CR16" s="59"/>
       <c r="CS16" s="51"/>
       <c r="CT16" s="51"/>
       <c r="CU16" s="51"/>
@@ -5587,15 +5581,15 @@
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
       <c r="D17" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="E17" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="F17" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="65" t="s">
+      <c r="G17" s="58" t="s">
         <v>83</v>
       </c>
       <c r="H17" s="38"/>
@@ -5609,7 +5603,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="42"/>
       <c r="R17" s="42"/>
-      <c r="S17" s="61"/>
+      <c r="S17" s="62"/>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
       <c r="V17" s="42"/>
@@ -5639,28 +5633,28 @@
       <c r="AT17" s="42"/>
       <c r="AU17" s="42"/>
       <c r="AV17" s="56" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="AW17" s="56" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="AX17" s="56" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="AY17" s="56" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="AZ17" s="56" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="BA17" s="56" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="BB17" s="56" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="BC17" s="56" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="BD17" s="42"/>
       <c r="BE17" s="42"/>
@@ -5681,7 +5675,7 @@
       <c r="BT17" s="43"/>
       <c r="BU17" s="42"/>
       <c r="BV17" s="38" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="BW17" s="38"/>
       <c r="BX17" s="38"/>
@@ -5691,7 +5685,7 @@
       <c r="CB17" s="38"/>
       <c r="CC17" s="38"/>
       <c r="CD17" s="38"/>
-      <c r="CE17" s="61"/>
+      <c r="CE17" s="62"/>
       <c r="CF17" s="42"/>
       <c r="CG17" s="42"/>
       <c r="CH17" s="42"/>
@@ -5704,7 +5698,7 @@
       <c r="CO17" s="42"/>
       <c r="CP17" s="45"/>
       <c r="CQ17" s="38"/>
-      <c r="CR17" s="58"/>
+      <c r="CR17" s="59"/>
       <c r="CS17" s="51"/>
       <c r="CT17" s="51"/>
       <c r="CU17" s="51"/>
@@ -5737,15 +5731,15 @@
       <c r="B18" s="53"/>
       <c r="C18" s="54"/>
       <c r="D18" s="38" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="F18" s="59" t="s">
-        <v>217</v>
-      </c>
-      <c r="G18" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="G18" s="61" t="s">
         <v>103</v>
       </c>
       <c r="H18" s="38"/>
@@ -5759,7 +5753,7 @@
       <c r="P18" s="42"/>
       <c r="Q18" s="42"/>
       <c r="R18" s="42"/>
-      <c r="S18" s="61"/>
+      <c r="S18" s="62"/>
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
       <c r="V18" s="42"/>
@@ -5789,28 +5783,28 @@
       <c r="AT18" s="42"/>
       <c r="AU18" s="42"/>
       <c r="AV18" s="56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AW18" s="56" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="AX18" s="56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AY18" s="56" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="AZ18" s="56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="BA18" s="56" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="BB18" s="56" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="BC18" s="56" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="BD18" s="42"/>
       <c r="BE18" s="42"/>
@@ -5831,7 +5825,7 @@
       <c r="BT18" s="43"/>
       <c r="BU18" s="42"/>
       <c r="BV18" s="38" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BW18" s="38"/>
       <c r="BX18" s="38"/>
@@ -5841,7 +5835,7 @@
       <c r="CB18" s="38"/>
       <c r="CC18" s="38"/>
       <c r="CD18" s="38"/>
-      <c r="CE18" s="61"/>
+      <c r="CE18" s="62"/>
       <c r="CF18" s="42"/>
       <c r="CG18" s="42"/>
       <c r="CH18" s="42"/>
@@ -5854,7 +5848,7 @@
       <c r="CO18" s="42"/>
       <c r="CP18" s="38"/>
       <c r="CQ18" s="38"/>
-      <c r="CR18" s="58"/>
+      <c r="CR18" s="59"/>
       <c r="CS18" s="51"/>
       <c r="CT18" s="51"/>
       <c r="CU18" s="51"/>
@@ -5887,16 +5881,16 @@
       <c r="B19" s="53"/>
       <c r="C19" s="54"/>
       <c r="D19" s="38" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>220</v>
-      </c>
-      <c r="F19" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G19" s="60" t="s">
-        <v>222</v>
+        <v>217</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>219</v>
       </c>
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
@@ -5909,7 +5903,7 @@
       <c r="P19" s="42"/>
       <c r="Q19" s="42"/>
       <c r="R19" s="42"/>
-      <c r="S19" s="61"/>
+      <c r="S19" s="62"/>
       <c r="T19" s="42"/>
       <c r="U19" s="42"/>
       <c r="V19" s="42"/>
@@ -5939,28 +5933,28 @@
       <c r="AT19" s="42"/>
       <c r="AU19" s="42"/>
       <c r="AV19" s="56" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="AW19" s="56" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="AX19" s="56" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="AY19" s="56" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="AZ19" s="56" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="BA19" s="56" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="BB19" s="56" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="BC19" s="56" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
       <c r="BD19" s="42"/>
       <c r="BE19" s="42"/>
@@ -5981,7 +5975,7 @@
       <c r="BT19" s="43"/>
       <c r="BU19" s="42"/>
       <c r="BV19" s="38" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="BW19" s="38"/>
       <c r="BX19" s="38"/>
@@ -5991,7 +5985,7 @@
       <c r="CB19" s="38"/>
       <c r="CC19" s="38"/>
       <c r="CD19" s="38"/>
-      <c r="CE19" s="61"/>
+      <c r="CE19" s="62"/>
       <c r="CF19" s="42"/>
       <c r="CG19" s="42"/>
       <c r="CH19" s="42"/>
@@ -6004,7 +5998,7 @@
       <c r="CO19" s="42"/>
       <c r="CP19" s="38"/>
       <c r="CQ19" s="38"/>
-      <c r="CR19" s="58"/>
+      <c r="CR19" s="59"/>
       <c r="CS19" s="51"/>
       <c r="CT19" s="51"/>
       <c r="CU19" s="51"/>
@@ -6037,16 +6031,16 @@
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
       <c r="D20" s="38" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F20" s="59" t="s">
-        <v>227</v>
-      </c>
-      <c r="G20" s="60" t="s">
-        <v>228</v>
+        <v>221</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="G20" s="61" t="s">
+        <v>223</v>
       </c>
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
@@ -6059,7 +6053,7 @@
       <c r="P20" s="42"/>
       <c r="Q20" s="42"/>
       <c r="R20" s="42"/>
-      <c r="S20" s="61"/>
+      <c r="S20" s="62"/>
       <c r="T20" s="42"/>
       <c r="U20" s="42"/>
       <c r="V20" s="42"/>
@@ -6089,28 +6083,28 @@
       <c r="AT20" s="42"/>
       <c r="AU20" s="42"/>
       <c r="AV20" s="56" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="AW20" s="56" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AX20" s="56" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="AY20" s="56" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AZ20" s="56" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="BA20" s="56" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="BB20" s="56" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="BC20" s="56" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="BD20" s="42"/>
       <c r="BE20" s="42"/>
@@ -6131,7 +6125,7 @@
       <c r="BT20" s="43"/>
       <c r="BU20" s="42"/>
       <c r="BV20" s="38" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="BW20" s="38"/>
       <c r="BX20" s="38"/>
@@ -6141,7 +6135,7 @@
       <c r="CB20" s="38"/>
       <c r="CC20" s="38"/>
       <c r="CD20" s="38"/>
-      <c r="CE20" s="61"/>
+      <c r="CE20" s="62"/>
       <c r="CF20" s="42"/>
       <c r="CG20" s="42"/>
       <c r="CH20" s="42"/>
@@ -6154,7 +6148,7 @@
       <c r="CO20" s="42"/>
       <c r="CP20" s="38"/>
       <c r="CQ20" s="38"/>
-      <c r="CR20" s="58"/>
+      <c r="CR20" s="59"/>
       <c r="CS20" s="51"/>
       <c r="CT20" s="51"/>
       <c r="CU20" s="51"/>
@@ -6205,7 +6199,7 @@
       <c r="P21" s="42"/>
       <c r="Q21" s="42"/>
       <c r="R21" s="42"/>
-      <c r="S21" s="61"/>
+      <c r="S21" s="62"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="42"/>
@@ -6234,14 +6228,30 @@
       <c r="AS21" s="42"/>
       <c r="AT21" s="42"/>
       <c r="AU21" s="42"/>
-      <c r="AV21" s="0"/>
-      <c r="AW21" s="0"/>
-      <c r="AX21" s="49"/>
-      <c r="AY21" s="49"/>
-      <c r="AZ21" s="49"/>
-      <c r="BA21" s="49"/>
-      <c r="BB21" s="49"/>
-      <c r="BC21" s="49"/>
+      <c r="AV21" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="AW21" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="AX21" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY21" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="AZ21" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="BA21" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="BB21" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="BC21" s="56" t="s">
+        <v>227</v>
+      </c>
       <c r="BD21" s="42"/>
       <c r="BE21" s="42"/>
       <c r="BF21" s="42"/>
@@ -6261,7 +6271,7 @@
       <c r="BT21" s="43"/>
       <c r="BU21" s="42"/>
       <c r="BV21" s="38" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="BW21" s="38"/>
       <c r="BX21" s="38"/>
@@ -6271,7 +6281,7 @@
       <c r="CB21" s="38"/>
       <c r="CC21" s="38"/>
       <c r="CD21" s="38"/>
-      <c r="CE21" s="61"/>
+      <c r="CE21" s="62"/>
       <c r="CF21" s="42"/>
       <c r="CG21" s="42"/>
       <c r="CH21" s="42"/>
@@ -6284,7 +6294,7 @@
       <c r="CO21" s="42"/>
       <c r="CP21" s="45"/>
       <c r="CQ21" s="38"/>
-      <c r="CR21" s="58"/>
+      <c r="CR21" s="59"/>
       <c r="CS21" s="51"/>
       <c r="CT21" s="51"/>
       <c r="CU21" s="51"/>
@@ -6317,10 +6327,10 @@
       <c r="B22" s="53"/>
       <c r="C22" s="54"/>
       <c r="D22" s="38" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="54"/>
@@ -6335,7 +6345,7 @@
       <c r="P22" s="42"/>
       <c r="Q22" s="42"/>
       <c r="R22" s="42"/>
-      <c r="S22" s="61"/>
+      <c r="S22" s="62"/>
       <c r="T22" s="42"/>
       <c r="U22" s="42"/>
       <c r="V22" s="42"/>
@@ -6364,7 +6374,7 @@
       <c r="AS22" s="42"/>
       <c r="AT22" s="42"/>
       <c r="AU22" s="42"/>
-      <c r="AV22" s="49"/>
+      <c r="AV22" s="0"/>
       <c r="AW22" s="0"/>
       <c r="AX22" s="42"/>
       <c r="AY22" s="42"/>
@@ -6391,7 +6401,7 @@
       <c r="BT22" s="43"/>
       <c r="BU22" s="42"/>
       <c r="BV22" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="BW22" s="38"/>
       <c r="BX22" s="38"/>
@@ -6401,7 +6411,7 @@
       <c r="CB22" s="38"/>
       <c r="CC22" s="38"/>
       <c r="CD22" s="38"/>
-      <c r="CE22" s="61"/>
+      <c r="CE22" s="62"/>
       <c r="CF22" s="42"/>
       <c r="CG22" s="42"/>
       <c r="CH22" s="42"/>
@@ -6414,7 +6424,7 @@
       <c r="CO22" s="42"/>
       <c r="CP22" s="45"/>
       <c r="CQ22" s="38"/>
-      <c r="CR22" s="58"/>
+      <c r="CR22" s="59"/>
       <c r="CS22" s="51"/>
       <c r="CT22" s="51"/>
       <c r="CU22" s="51"/>
@@ -6447,10 +6457,10 @@
       <c r="B23" s="53"/>
       <c r="C23" s="54"/>
       <c r="D23" s="38" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="54"/>
@@ -6465,7 +6475,7 @@
       <c r="P23" s="42"/>
       <c r="Q23" s="42"/>
       <c r="R23" s="42"/>
-      <c r="S23" s="61"/>
+      <c r="S23" s="62"/>
       <c r="T23" s="42"/>
       <c r="U23" s="42"/>
       <c r="V23" s="42"/>
@@ -6494,8 +6504,8 @@
       <c r="AS23" s="42"/>
       <c r="AT23" s="42"/>
       <c r="AU23" s="42"/>
-      <c r="AV23" s="42"/>
-      <c r="AW23" s="42"/>
+      <c r="AV23" s="49"/>
+      <c r="AW23" s="0"/>
       <c r="AX23" s="42"/>
       <c r="AY23" s="42"/>
       <c r="AZ23" s="42"/>
@@ -6521,7 +6531,7 @@
       <c r="BT23" s="43"/>
       <c r="BU23" s="42"/>
       <c r="BV23" s="38" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="BW23" s="38"/>
       <c r="BX23" s="38"/>
@@ -6531,7 +6541,7 @@
       <c r="CB23" s="38"/>
       <c r="CC23" s="38"/>
       <c r="CD23" s="38"/>
-      <c r="CE23" s="61"/>
+      <c r="CE23" s="62"/>
       <c r="CF23" s="42"/>
       <c r="CG23" s="42"/>
       <c r="CH23" s="42"/>
@@ -6544,7 +6554,7 @@
       <c r="CO23" s="42"/>
       <c r="CP23" s="45"/>
       <c r="CQ23" s="38"/>
-      <c r="CR23" s="58"/>
+      <c r="CR23" s="59"/>
       <c r="CS23" s="51"/>
       <c r="CT23" s="51"/>
       <c r="CU23" s="51"/>
@@ -6577,10 +6587,10 @@
       <c r="B24" s="53"/>
       <c r="C24" s="54"/>
       <c r="D24" s="38" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="54"/>
@@ -6595,7 +6605,7 @@
       <c r="P24" s="42"/>
       <c r="Q24" s="42"/>
       <c r="R24" s="42"/>
-      <c r="S24" s="61"/>
+      <c r="S24" s="62"/>
       <c r="T24" s="42"/>
       <c r="U24" s="42"/>
       <c r="V24" s="42"/>
@@ -6651,7 +6661,7 @@
       <c r="BT24" s="43"/>
       <c r="BU24" s="42"/>
       <c r="BV24" s="38" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="BW24" s="38"/>
       <c r="BX24" s="38"/>
@@ -6661,7 +6671,7 @@
       <c r="CB24" s="38"/>
       <c r="CC24" s="38"/>
       <c r="CD24" s="38"/>
-      <c r="CE24" s="61"/>
+      <c r="CE24" s="62"/>
       <c r="CF24" s="42"/>
       <c r="CG24" s="42"/>
       <c r="CH24" s="42"/>
@@ -6674,7 +6684,7 @@
       <c r="CO24" s="42"/>
       <c r="CP24" s="38"/>
       <c r="CQ24" s="38"/>
-      <c r="CR24" s="58"/>
+      <c r="CR24" s="59"/>
       <c r="CS24" s="51"/>
       <c r="CT24" s="51"/>
       <c r="CU24" s="51"/>
@@ -6707,10 +6717,10 @@
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
       <c r="D25" s="38" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F25" s="53"/>
       <c r="G25" s="54"/>
@@ -6725,7 +6735,7 @@
       <c r="P25" s="42"/>
       <c r="Q25" s="42"/>
       <c r="R25" s="42"/>
-      <c r="S25" s="61"/>
+      <c r="S25" s="62"/>
       <c r="T25" s="42"/>
       <c r="U25" s="42"/>
       <c r="V25" s="42"/>
@@ -6789,7 +6799,7 @@
       <c r="CB25" s="38"/>
       <c r="CC25" s="38"/>
       <c r="CD25" s="38"/>
-      <c r="CE25" s="61"/>
+      <c r="CE25" s="62"/>
       <c r="CF25" s="42"/>
       <c r="CG25" s="42"/>
       <c r="CH25" s="42"/>
@@ -6802,7 +6812,7 @@
       <c r="CO25" s="42"/>
       <c r="CP25" s="38"/>
       <c r="CQ25" s="38"/>
-      <c r="CR25" s="58"/>
+      <c r="CR25" s="59"/>
       <c r="CS25" s="51"/>
       <c r="CT25" s="51"/>
       <c r="CU25" s="51"/>
@@ -6853,7 +6863,7 @@
       <c r="P26" s="42"/>
       <c r="Q26" s="42"/>
       <c r="R26" s="42"/>
-      <c r="S26" s="61"/>
+      <c r="S26" s="62"/>
       <c r="T26" s="42"/>
       <c r="U26" s="42"/>
       <c r="V26" s="42"/>
@@ -6917,7 +6927,7 @@
       <c r="CB26" s="38"/>
       <c r="CC26" s="38"/>
       <c r="CD26" s="38"/>
-      <c r="CE26" s="61"/>
+      <c r="CE26" s="62"/>
       <c r="CF26" s="42"/>
       <c r="CG26" s="42"/>
       <c r="CH26" s="42"/>
@@ -6930,7 +6940,7 @@
       <c r="CO26" s="42"/>
       <c r="CP26" s="38"/>
       <c r="CQ26" s="38"/>
-      <c r="CR26" s="58"/>
+      <c r="CR26" s="59"/>
       <c r="CS26" s="51"/>
       <c r="CT26" s="51"/>
       <c r="CU26" s="51"/>
@@ -6963,10 +6973,10 @@
       <c r="B27" s="53"/>
       <c r="C27" s="54"/>
       <c r="D27" s="42" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F27" s="53"/>
       <c r="G27" s="54"/>
@@ -6981,7 +6991,7 @@
       <c r="P27" s="42"/>
       <c r="Q27" s="42"/>
       <c r="R27" s="42"/>
-      <c r="S27" s="61"/>
+      <c r="S27" s="62"/>
       <c r="T27" s="42"/>
       <c r="U27" s="42"/>
       <c r="V27" s="42"/>
@@ -7045,7 +7055,7 @@
       <c r="CB27" s="38"/>
       <c r="CC27" s="38"/>
       <c r="CD27" s="38"/>
-      <c r="CE27" s="61"/>
+      <c r="CE27" s="62"/>
       <c r="CF27" s="42"/>
       <c r="CG27" s="42"/>
       <c r="CH27" s="42"/>
@@ -7058,7 +7068,7 @@
       <c r="CO27" s="42"/>
       <c r="CP27" s="38"/>
       <c r="CQ27" s="38"/>
-      <c r="CR27" s="58"/>
+      <c r="CR27" s="59"/>
       <c r="CS27" s="51"/>
       <c r="CT27" s="51"/>
       <c r="CU27" s="51"/>
@@ -7091,7 +7101,7 @@
       <c r="B28" s="53"/>
       <c r="C28" s="54"/>
       <c r="D28" s="42" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E28" s="42" t="s">
         <v>161</v>
@@ -7109,7 +7119,7 @@
       <c r="P28" s="42"/>
       <c r="Q28" s="42"/>
       <c r="R28" s="42"/>
-      <c r="S28" s="61"/>
+      <c r="S28" s="62"/>
       <c r="T28" s="42"/>
       <c r="U28" s="42"/>
       <c r="V28" s="42"/>
@@ -7173,7 +7183,7 @@
       <c r="CB28" s="38"/>
       <c r="CC28" s="38"/>
       <c r="CD28" s="38"/>
-      <c r="CE28" s="61"/>
+      <c r="CE28" s="62"/>
       <c r="CF28" s="42"/>
       <c r="CG28" s="42"/>
       <c r="CH28" s="42"/>
@@ -7186,7 +7196,7 @@
       <c r="CO28" s="42"/>
       <c r="CP28" s="38"/>
       <c r="CQ28" s="38"/>
-      <c r="CR28" s="58"/>
+      <c r="CR28" s="59"/>
       <c r="CS28" s="51"/>
       <c r="CT28" s="51"/>
       <c r="CU28" s="51"/>
@@ -7219,10 +7229,10 @@
       <c r="B29" s="53"/>
       <c r="C29" s="54"/>
       <c r="D29" s="42" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="54"/>
@@ -7237,7 +7247,7 @@
       <c r="P29" s="42"/>
       <c r="Q29" s="42"/>
       <c r="R29" s="42"/>
-      <c r="S29" s="61"/>
+      <c r="S29" s="62"/>
       <c r="T29" s="42"/>
       <c r="U29" s="42"/>
       <c r="V29" s="42"/>
@@ -7301,7 +7311,7 @@
       <c r="CB29" s="38"/>
       <c r="CC29" s="38"/>
       <c r="CD29" s="38"/>
-      <c r="CE29" s="61"/>
+      <c r="CE29" s="62"/>
       <c r="CF29" s="42"/>
       <c r="CG29" s="42"/>
       <c r="CH29" s="42"/>
@@ -7314,7 +7324,7 @@
       <c r="CO29" s="42"/>
       <c r="CP29" s="38"/>
       <c r="CQ29" s="38"/>
-      <c r="CR29" s="58"/>
+      <c r="CR29" s="59"/>
       <c r="CS29" s="51"/>
       <c r="CT29" s="51"/>
       <c r="CU29" s="51"/>
@@ -7347,10 +7357,10 @@
       <c r="B30" s="53"/>
       <c r="C30" s="54"/>
       <c r="D30" s="38" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F30" s="53"/>
       <c r="G30" s="54"/>
@@ -7365,7 +7375,7 @@
       <c r="P30" s="42"/>
       <c r="Q30" s="42"/>
       <c r="R30" s="42"/>
-      <c r="S30" s="61"/>
+      <c r="S30" s="62"/>
       <c r="T30" s="42"/>
       <c r="U30" s="42"/>
       <c r="V30" s="42"/>
@@ -7429,7 +7439,7 @@
       <c r="CB30" s="38"/>
       <c r="CC30" s="38"/>
       <c r="CD30" s="38"/>
-      <c r="CE30" s="61"/>
+      <c r="CE30" s="62"/>
       <c r="CF30" s="42"/>
       <c r="CG30" s="42"/>
       <c r="CH30" s="42"/>
@@ -7442,7 +7452,7 @@
       <c r="CO30" s="42"/>
       <c r="CP30" s="38"/>
       <c r="CQ30" s="38"/>
-      <c r="CR30" s="58"/>
+      <c r="CR30" s="59"/>
       <c r="CS30" s="51"/>
       <c r="CT30" s="51"/>
       <c r="CU30" s="51"/>
@@ -7493,7 +7503,7 @@
       <c r="P31" s="42"/>
       <c r="Q31" s="42"/>
       <c r="R31" s="42"/>
-      <c r="S31" s="61"/>
+      <c r="S31" s="62"/>
       <c r="T31" s="42"/>
       <c r="U31" s="42"/>
       <c r="V31" s="42"/>
@@ -7557,7 +7567,7 @@
       <c r="CB31" s="38"/>
       <c r="CC31" s="38"/>
       <c r="CD31" s="38"/>
-      <c r="CE31" s="61"/>
+      <c r="CE31" s="62"/>
       <c r="CF31" s="42"/>
       <c r="CG31" s="42"/>
       <c r="CH31" s="42"/>
@@ -7570,7 +7580,7 @@
       <c r="CO31" s="42"/>
       <c r="CP31" s="38"/>
       <c r="CQ31" s="38"/>
-      <c r="CR31" s="58"/>
+      <c r="CR31" s="59"/>
       <c r="CS31" s="51"/>
       <c r="CT31" s="51"/>
       <c r="CU31" s="51"/>
@@ -7603,10 +7613,10 @@
       <c r="B32" s="53"/>
       <c r="C32" s="54"/>
       <c r="D32" s="38" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="54"/>
@@ -7621,7 +7631,7 @@
       <c r="P32" s="42"/>
       <c r="Q32" s="42"/>
       <c r="R32" s="42"/>
-      <c r="S32" s="61"/>
+      <c r="S32" s="62"/>
       <c r="T32" s="42"/>
       <c r="U32" s="42"/>
       <c r="V32" s="42"/>
@@ -7685,7 +7695,7 @@
       <c r="CB32" s="38"/>
       <c r="CC32" s="38"/>
       <c r="CD32" s="38"/>
-      <c r="CE32" s="61"/>
+      <c r="CE32" s="62"/>
       <c r="CF32" s="42"/>
       <c r="CG32" s="42"/>
       <c r="CH32" s="42"/>
@@ -7698,7 +7708,7 @@
       <c r="CO32" s="42"/>
       <c r="CP32" s="38"/>
       <c r="CQ32" s="38"/>
-      <c r="CR32" s="58"/>
+      <c r="CR32" s="59"/>
       <c r="CS32" s="51"/>
       <c r="CT32" s="51"/>
       <c r="CU32" s="51"/>
@@ -7731,10 +7741,10 @@
       <c r="B33" s="53"/>
       <c r="C33" s="54"/>
       <c r="D33" s="38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F33" s="53"/>
       <c r="G33" s="54"/>
@@ -7749,7 +7759,7 @@
       <c r="P33" s="42"/>
       <c r="Q33" s="42"/>
       <c r="R33" s="42"/>
-      <c r="S33" s="61"/>
+      <c r="S33" s="62"/>
       <c r="T33" s="42"/>
       <c r="U33" s="42"/>
       <c r="V33" s="42"/>
@@ -7813,7 +7823,7 @@
       <c r="CB33" s="38"/>
       <c r="CC33" s="38"/>
       <c r="CD33" s="38"/>
-      <c r="CE33" s="61"/>
+      <c r="CE33" s="62"/>
       <c r="CF33" s="42"/>
       <c r="CG33" s="42"/>
       <c r="CH33" s="42"/>
@@ -7826,7 +7836,7 @@
       <c r="CO33" s="42"/>
       <c r="CP33" s="38"/>
       <c r="CQ33" s="38"/>
-      <c r="CR33" s="58"/>
+      <c r="CR33" s="59"/>
       <c r="CS33" s="51"/>
       <c r="CT33" s="51"/>
       <c r="CU33" s="51"/>
@@ -7877,7 +7887,7 @@
       <c r="P34" s="42"/>
       <c r="Q34" s="42"/>
       <c r="R34" s="42"/>
-      <c r="S34" s="61"/>
+      <c r="S34" s="62"/>
       <c r="T34" s="42"/>
       <c r="U34" s="42"/>
       <c r="V34" s="42"/>
@@ -7941,7 +7951,7 @@
       <c r="CB34" s="38"/>
       <c r="CC34" s="38"/>
       <c r="CD34" s="38"/>
-      <c r="CE34" s="61"/>
+      <c r="CE34" s="62"/>
       <c r="CF34" s="42"/>
       <c r="CG34" s="42"/>
       <c r="CH34" s="42"/>
@@ -7954,7 +7964,7 @@
       <c r="CO34" s="42"/>
       <c r="CP34" s="38"/>
       <c r="CQ34" s="38"/>
-      <c r="CR34" s="58"/>
+      <c r="CR34" s="59"/>
       <c r="CS34" s="51"/>
       <c r="CT34" s="51"/>
       <c r="CU34" s="51"/>
@@ -7987,10 +7997,10 @@
       <c r="B35" s="53"/>
       <c r="C35" s="54"/>
       <c r="D35" s="38" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F35" s="53"/>
       <c r="G35" s="54"/>
@@ -8005,7 +8015,7 @@
       <c r="P35" s="42"/>
       <c r="Q35" s="42"/>
       <c r="R35" s="42"/>
-      <c r="S35" s="61"/>
+      <c r="S35" s="62"/>
       <c r="T35" s="42"/>
       <c r="U35" s="42"/>
       <c r="V35" s="42"/>
@@ -8069,7 +8079,7 @@
       <c r="CB35" s="38"/>
       <c r="CC35" s="38"/>
       <c r="CD35" s="38"/>
-      <c r="CE35" s="61"/>
+      <c r="CE35" s="62"/>
       <c r="CF35" s="42"/>
       <c r="CG35" s="42"/>
       <c r="CH35" s="42"/>
@@ -8082,7 +8092,7 @@
       <c r="CO35" s="42"/>
       <c r="CP35" s="38"/>
       <c r="CQ35" s="38"/>
-      <c r="CR35" s="58"/>
+      <c r="CR35" s="59"/>
       <c r="CS35" s="51"/>
       <c r="CT35" s="51"/>
       <c r="CU35" s="51"/>
@@ -8115,10 +8125,10 @@
       <c r="B36" s="53"/>
       <c r="C36" s="54"/>
       <c r="D36" s="38" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E36" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F36" s="53"/>
       <c r="G36" s="54"/>
@@ -8133,7 +8143,7 @@
       <c r="P36" s="42"/>
       <c r="Q36" s="42"/>
       <c r="R36" s="42"/>
-      <c r="S36" s="61"/>
+      <c r="S36" s="62"/>
       <c r="T36" s="42"/>
       <c r="U36" s="42"/>
       <c r="V36" s="42"/>
@@ -8197,7 +8207,7 @@
       <c r="CB36" s="38"/>
       <c r="CC36" s="38"/>
       <c r="CD36" s="38"/>
-      <c r="CE36" s="61"/>
+      <c r="CE36" s="62"/>
       <c r="CF36" s="42"/>
       <c r="CG36" s="42"/>
       <c r="CH36" s="42"/>
@@ -8210,7 +8220,7 @@
       <c r="CO36" s="42"/>
       <c r="CP36" s="38"/>
       <c r="CQ36" s="38"/>
-      <c r="CR36" s="58"/>
+      <c r="CR36" s="59"/>
       <c r="CS36" s="51"/>
       <c r="CT36" s="51"/>
       <c r="CU36" s="51"/>
@@ -8243,10 +8253,10 @@
       <c r="B37" s="53"/>
       <c r="C37" s="54"/>
       <c r="D37" s="42" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F37" s="53"/>
       <c r="G37" s="54"/>
@@ -8261,7 +8271,7 @@
       <c r="P37" s="42"/>
       <c r="Q37" s="42"/>
       <c r="R37" s="42"/>
-      <c r="S37" s="61"/>
+      <c r="S37" s="62"/>
       <c r="T37" s="42"/>
       <c r="U37" s="42"/>
       <c r="V37" s="42"/>
@@ -8325,7 +8335,7 @@
       <c r="CB37" s="38"/>
       <c r="CC37" s="38"/>
       <c r="CD37" s="38"/>
-      <c r="CE37" s="61"/>
+      <c r="CE37" s="62"/>
       <c r="CF37" s="42"/>
       <c r="CG37" s="42"/>
       <c r="CH37" s="42"/>
@@ -8338,7 +8348,7 @@
       <c r="CO37" s="42"/>
       <c r="CP37" s="38"/>
       <c r="CQ37" s="38"/>
-      <c r="CR37" s="58"/>
+      <c r="CR37" s="59"/>
       <c r="CS37" s="51"/>
       <c r="CT37" s="51"/>
       <c r="CU37" s="51"/>
@@ -8371,10 +8381,10 @@
       <c r="B38" s="53"/>
       <c r="C38" s="54"/>
       <c r="D38" s="42" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F38" s="53"/>
       <c r="G38" s="54"/>
@@ -8389,7 +8399,7 @@
       <c r="P38" s="42"/>
       <c r="Q38" s="42"/>
       <c r="R38" s="42"/>
-      <c r="S38" s="61"/>
+      <c r="S38" s="62"/>
       <c r="T38" s="42"/>
       <c r="U38" s="42"/>
       <c r="V38" s="42"/>
@@ -8453,7 +8463,7 @@
       <c r="CB38" s="38"/>
       <c r="CC38" s="38"/>
       <c r="CD38" s="38"/>
-      <c r="CE38" s="61"/>
+      <c r="CE38" s="62"/>
       <c r="CF38" s="42"/>
       <c r="CG38" s="42"/>
       <c r="CH38" s="42"/>
@@ -8466,7 +8476,7 @@
       <c r="CO38" s="42"/>
       <c r="CP38" s="38"/>
       <c r="CQ38" s="38"/>
-      <c r="CR38" s="58"/>
+      <c r="CR38" s="59"/>
       <c r="CS38" s="51"/>
       <c r="CT38" s="51"/>
       <c r="CU38" s="51"/>
@@ -8499,10 +8509,10 @@
       <c r="B39" s="53"/>
       <c r="C39" s="54"/>
       <c r="D39" s="42" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E39" s="42" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F39" s="53"/>
       <c r="G39" s="54"/>
@@ -8517,7 +8527,7 @@
       <c r="P39" s="42"/>
       <c r="Q39" s="42"/>
       <c r="R39" s="42"/>
-      <c r="S39" s="61"/>
+      <c r="S39" s="62"/>
       <c r="T39" s="42"/>
       <c r="U39" s="42"/>
       <c r="V39" s="42"/>
@@ -8581,7 +8591,7 @@
       <c r="CB39" s="38"/>
       <c r="CC39" s="38"/>
       <c r="CD39" s="38"/>
-      <c r="CE39" s="61"/>
+      <c r="CE39" s="62"/>
       <c r="CF39" s="42"/>
       <c r="CG39" s="42"/>
       <c r="CH39" s="42"/>
@@ -8594,7 +8604,7 @@
       <c r="CO39" s="42"/>
       <c r="CP39" s="38"/>
       <c r="CQ39" s="38"/>
-      <c r="CR39" s="58"/>
+      <c r="CR39" s="59"/>
       <c r="CS39" s="51"/>
       <c r="CT39" s="51"/>
       <c r="CU39" s="51"/>
@@ -8627,10 +8637,10 @@
       <c r="B40" s="53"/>
       <c r="C40" s="54"/>
       <c r="D40" s="38" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F40" s="53"/>
       <c r="G40" s="54"/>
@@ -8645,7 +8655,7 @@
       <c r="P40" s="42"/>
       <c r="Q40" s="42"/>
       <c r="R40" s="42"/>
-      <c r="S40" s="61"/>
+      <c r="S40" s="62"/>
       <c r="T40" s="42"/>
       <c r="U40" s="42"/>
       <c r="V40" s="42"/>
@@ -8709,7 +8719,7 @@
       <c r="CB40" s="38"/>
       <c r="CC40" s="38"/>
       <c r="CD40" s="38"/>
-      <c r="CE40" s="61"/>
+      <c r="CE40" s="62"/>
       <c r="CF40" s="42"/>
       <c r="CG40" s="42"/>
       <c r="CH40" s="42"/>
@@ -8722,7 +8732,7 @@
       <c r="CO40" s="42"/>
       <c r="CP40" s="38"/>
       <c r="CQ40" s="38"/>
-      <c r="CR40" s="58"/>
+      <c r="CR40" s="59"/>
       <c r="CS40" s="51"/>
       <c r="CT40" s="51"/>
       <c r="CU40" s="51"/>
@@ -8755,10 +8765,10 @@
       <c r="B41" s="43"/>
       <c r="C41" s="42"/>
       <c r="D41" s="38" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F41" s="53"/>
       <c r="G41" s="54"/>
@@ -8773,7 +8783,7 @@
       <c r="P41" s="42"/>
       <c r="Q41" s="42"/>
       <c r="R41" s="42"/>
-      <c r="S41" s="61"/>
+      <c r="S41" s="62"/>
       <c r="T41" s="42"/>
       <c r="U41" s="42"/>
       <c r="V41" s="42"/>
@@ -8837,7 +8847,7 @@
       <c r="CB41" s="38"/>
       <c r="CC41" s="38"/>
       <c r="CD41" s="38"/>
-      <c r="CE41" s="61"/>
+      <c r="CE41" s="62"/>
       <c r="CF41" s="42"/>
       <c r="CG41" s="42"/>
       <c r="CH41" s="42"/>
@@ -8850,7 +8860,7 @@
       <c r="CO41" s="42"/>
       <c r="CP41" s="38"/>
       <c r="CQ41" s="38"/>
-      <c r="CR41" s="58"/>
+      <c r="CR41" s="59"/>
       <c r="CS41" s="51"/>
       <c r="CT41" s="51"/>
       <c r="CU41" s="51"/>
@@ -8883,10 +8893,10 @@
       <c r="B42" s="43"/>
       <c r="C42" s="42"/>
       <c r="D42" s="38" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F42" s="53"/>
       <c r="G42" s="54"/>
@@ -8901,7 +8911,7 @@
       <c r="P42" s="42"/>
       <c r="Q42" s="42"/>
       <c r="R42" s="42"/>
-      <c r="S42" s="61"/>
+      <c r="S42" s="62"/>
       <c r="T42" s="42"/>
       <c r="U42" s="42"/>
       <c r="V42" s="42"/>
@@ -8965,7 +8975,7 @@
       <c r="CB42" s="38"/>
       <c r="CC42" s="38"/>
       <c r="CD42" s="38"/>
-      <c r="CE42" s="61"/>
+      <c r="CE42" s="62"/>
       <c r="CF42" s="42"/>
       <c r="CG42" s="42"/>
       <c r="CH42" s="42"/>
@@ -8978,7 +8988,7 @@
       <c r="CO42" s="42"/>
       <c r="CP42" s="38"/>
       <c r="CQ42" s="38"/>
-      <c r="CR42" s="58"/>
+      <c r="CR42" s="59"/>
       <c r="CS42" s="51"/>
       <c r="CT42" s="51"/>
       <c r="CU42" s="51"/>
@@ -9011,10 +9021,10 @@
       <c r="B43" s="43"/>
       <c r="C43" s="42"/>
       <c r="D43" s="38" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F43" s="53"/>
       <c r="G43" s="54"/>
@@ -9029,7 +9039,7 @@
       <c r="P43" s="42"/>
       <c r="Q43" s="42"/>
       <c r="R43" s="42"/>
-      <c r="S43" s="61"/>
+      <c r="S43" s="62"/>
       <c r="T43" s="42"/>
       <c r="U43" s="42"/>
       <c r="V43" s="42"/>
@@ -9093,7 +9103,7 @@
       <c r="CB43" s="38"/>
       <c r="CC43" s="38"/>
       <c r="CD43" s="38"/>
-      <c r="CE43" s="61"/>
+      <c r="CE43" s="62"/>
       <c r="CF43" s="42"/>
       <c r="CG43" s="42"/>
       <c r="CH43" s="42"/>
@@ -9106,7 +9116,7 @@
       <c r="CO43" s="42"/>
       <c r="CP43" s="38"/>
       <c r="CQ43" s="38"/>
-      <c r="CR43" s="58"/>
+      <c r="CR43" s="59"/>
       <c r="CS43" s="51"/>
       <c r="CT43" s="51"/>
       <c r="CU43" s="51"/>
@@ -9139,10 +9149,10 @@
       <c r="B44" s="43"/>
       <c r="C44" s="42"/>
       <c r="D44" s="38" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F44" s="43"/>
       <c r="G44" s="42"/>
@@ -9157,7 +9167,7 @@
       <c r="P44" s="42"/>
       <c r="Q44" s="42"/>
       <c r="R44" s="42"/>
-      <c r="S44" s="61"/>
+      <c r="S44" s="62"/>
       <c r="T44" s="42"/>
       <c r="U44" s="42"/>
       <c r="V44" s="42"/>
@@ -9221,7 +9231,7 @@
       <c r="CB44" s="38"/>
       <c r="CC44" s="38"/>
       <c r="CD44" s="38"/>
-      <c r="CE44" s="61"/>
+      <c r="CE44" s="62"/>
       <c r="CF44" s="42"/>
       <c r="CG44" s="42"/>
       <c r="CH44" s="42"/>
@@ -9234,7 +9244,7 @@
       <c r="CO44" s="42"/>
       <c r="CP44" s="38"/>
       <c r="CQ44" s="38"/>
-      <c r="CR44" s="58"/>
+      <c r="CR44" s="59"/>
       <c r="CS44" s="51"/>
       <c r="CT44" s="51"/>
       <c r="CU44" s="51"/>
@@ -9266,10 +9276,10 @@
       <c r="B45" s="43"/>
       <c r="C45" s="42"/>
       <c r="D45" s="38" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F45" s="43"/>
       <c r="G45" s="42"/>
@@ -9284,7 +9294,7 @@
       <c r="P45" s="42"/>
       <c r="Q45" s="42"/>
       <c r="R45" s="42"/>
-      <c r="S45" s="61"/>
+      <c r="S45" s="62"/>
       <c r="T45" s="42"/>
       <c r="U45" s="42"/>
       <c r="V45" s="42"/>
@@ -9348,7 +9358,7 @@
       <c r="CB45" s="38"/>
       <c r="CC45" s="38"/>
       <c r="CD45" s="38"/>
-      <c r="CE45" s="61"/>
+      <c r="CE45" s="62"/>
       <c r="CF45" s="42"/>
       <c r="CG45" s="42"/>
       <c r="CH45" s="42"/>
@@ -9361,7 +9371,7 @@
       <c r="CO45" s="42"/>
       <c r="CP45" s="38"/>
       <c r="CQ45" s="38"/>
-      <c r="CR45" s="58"/>
+      <c r="CR45" s="59"/>
       <c r="CS45" s="51"/>
       <c r="CT45" s="51"/>
       <c r="CU45" s="51"/>
@@ -9393,10 +9403,10 @@
       <c r="B46" s="43"/>
       <c r="C46" s="42"/>
       <c r="D46" s="38" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E46" s="38" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="42"/>
@@ -9411,7 +9421,7 @@
       <c r="P46" s="42"/>
       <c r="Q46" s="42"/>
       <c r="R46" s="42"/>
-      <c r="S46" s="61"/>
+      <c r="S46" s="62"/>
       <c r="T46" s="42"/>
       <c r="U46" s="42"/>
       <c r="V46" s="42"/>
@@ -9475,7 +9485,7 @@
       <c r="CB46" s="38"/>
       <c r="CC46" s="38"/>
       <c r="CD46" s="38"/>
-      <c r="CE46" s="61"/>
+      <c r="CE46" s="62"/>
       <c r="CF46" s="42"/>
       <c r="CG46" s="42"/>
       <c r="CH46" s="42"/>
@@ -9488,7 +9498,7 @@
       <c r="CO46" s="42"/>
       <c r="CP46" s="38"/>
       <c r="CQ46" s="38"/>
-      <c r="CR46" s="58"/>
+      <c r="CR46" s="59"/>
       <c r="CS46" s="51"/>
       <c r="CT46" s="51"/>
       <c r="CU46" s="51"/>
@@ -9520,10 +9530,10 @@
       <c r="B47" s="43"/>
       <c r="C47" s="42"/>
       <c r="D47" s="38" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="42"/>
@@ -9538,7 +9548,7 @@
       <c r="P47" s="42"/>
       <c r="Q47" s="42"/>
       <c r="R47" s="42"/>
-      <c r="S47" s="61"/>
+      <c r="S47" s="62"/>
       <c r="T47" s="42"/>
       <c r="U47" s="42"/>
       <c r="V47" s="42"/>
@@ -9602,7 +9612,7 @@
       <c r="CB47" s="38"/>
       <c r="CC47" s="38"/>
       <c r="CD47" s="38"/>
-      <c r="CE47" s="61"/>
+      <c r="CE47" s="62"/>
       <c r="CF47" s="42"/>
       <c r="CG47" s="42"/>
       <c r="CH47" s="42"/>
@@ -9615,7 +9625,7 @@
       <c r="CO47" s="42"/>
       <c r="CP47" s="38"/>
       <c r="CQ47" s="38"/>
-      <c r="CR47" s="58"/>
+      <c r="CR47" s="59"/>
       <c r="CS47" s="51"/>
       <c r="CT47" s="51"/>
       <c r="CU47" s="51"/>
@@ -9661,7 +9671,7 @@
       <c r="P48" s="42"/>
       <c r="Q48" s="42"/>
       <c r="R48" s="42"/>
-      <c r="S48" s="61"/>
+      <c r="S48" s="62"/>
       <c r="T48" s="42"/>
       <c r="U48" s="42"/>
       <c r="V48" s="42"/>
@@ -9725,7 +9735,7 @@
       <c r="CB48" s="38"/>
       <c r="CC48" s="38"/>
       <c r="CD48" s="38"/>
-      <c r="CE48" s="61"/>
+      <c r="CE48" s="62"/>
       <c r="CF48" s="42"/>
       <c r="CG48" s="42"/>
       <c r="CH48" s="42"/>
@@ -9738,7 +9748,7 @@
       <c r="CO48" s="42"/>
       <c r="CP48" s="38"/>
       <c r="CQ48" s="38"/>
-      <c r="CR48" s="58"/>
+      <c r="CR48" s="59"/>
       <c r="CS48" s="51"/>
       <c r="CT48" s="51"/>
       <c r="CU48" s="51"/>
@@ -9784,7 +9794,7 @@
       <c r="P49" s="42"/>
       <c r="Q49" s="42"/>
       <c r="R49" s="42"/>
-      <c r="S49" s="61"/>
+      <c r="S49" s="62"/>
       <c r="T49" s="42"/>
       <c r="U49" s="42"/>
       <c r="V49" s="42"/>
@@ -9848,7 +9858,7 @@
       <c r="CB49" s="38"/>
       <c r="CC49" s="38"/>
       <c r="CD49" s="38"/>
-      <c r="CE49" s="61"/>
+      <c r="CE49" s="62"/>
       <c r="CF49" s="42"/>
       <c r="CG49" s="42"/>
       <c r="CH49" s="42"/>
@@ -9861,7 +9871,7 @@
       <c r="CO49" s="42"/>
       <c r="CP49" s="38"/>
       <c r="CQ49" s="38"/>
-      <c r="CR49" s="58"/>
+      <c r="CR49" s="59"/>
       <c r="CS49" s="51"/>
       <c r="CT49" s="51"/>
       <c r="CU49" s="51"/>
@@ -9911,7 +9921,7 @@
       <c r="CN50" s="6"/>
       <c r="CO50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -9920,6 +9930,8 @@
       <c r="U51" s="5"/>
       <c r="AI51" s="5"/>
       <c r="AS51" s="5"/>
+      <c r="AV51" s="42"/>
+      <c r="AW51" s="42"/>
       <c r="BU51" s="5"/>
       <c r="CA51" s="5"/>
       <c r="CF51" s="5"/>
@@ -10631,11 +10643,11 @@
     <mergeCell ref="A4:A44"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B83 D1:D3 F1:F5 H1:H83 J1:J83 L1:L83 N1:N83 P1:P83 R1:R83 T1:T83 V1:V83 X1:X83 Z1:Z83 AB1:AB83 AD1:AD83 AF1:AF83 AH1:AH83 AJ1:AJ83 AL1:AL83 AN1:AN83 AP1:AP83 AR1:AR83 AT1:AT83 AV1:AV20 AX1:AX83 AZ1:AZ83 BB1:BB83 BD1:BD83 BF1:BF3 BH1:BH3 BJ1:BJ3 BL1:BL83 BN1:BN83 BP1:BP3 BR1:BR83 BT1:BT83 BV1:BV83 BX1:BX83 BZ1:BZ83 CB1:CB83 CD1:CD83 CF1:CF83 CH1:CH83 CJ1:CJ83 CL1:CL83 CN1:CN83 CP1:AMJ83 E4:P5 AI4:AL4 CA4:CF6 AI5:AJ6 BH5:BH83 E6:E47 G6:H20 BF6:BF83 BJ6:BJ83 BP8:BP83 F21:F83 AV22:AV83 D50:D83" type="none">
+    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:B83 D1:D3 F1:F5 H1:H83 J1:J83 L1:L83 N1:N83 P1:P83 R1:R83 T1:T83 V1:V83 X1:X83 Z1:Z83 AB1:AB83 AD1:AD83 AF1:AF83 AH1:AH83 AJ1:AJ83 AL1:AL83 AN1:AN83 AP1:AP83 AR1:AR83 AT1:AT83 AV1:AV21 AX1:AX83 AZ1:AZ83 BB1:BB83 BD1:BD83 BF1:BF3 BH1:BH3 BJ1:BJ3 BL1:BL83 BN1:BN83 BP1:BP3 BR1:BR3 BT1:BT83 BV1:BV83 BX1:BX83 BZ1:BZ83 CB1:CB83 CD1:CD83 CF1:CF83 CH1:CH83 CJ1:CJ83 CL1:CL83 CN1:CN83 CP1:AMJ83 E4:P5 AI4:AL4 CA4:CF6 AI5:AJ6 BH5:BH83 BR5:BR83 E6:E47 G6:H20 BF6:BF83 BJ6:BJ83 BP8:BP83 F21:F83 AV23:AV83 D50:D83" type="none">
       <formula1>20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C83 E1:E3 G1:G3 I1:I3 K1:K3 M1:M3 O1:O3 Q1:Q83 S1:S83 U1:U83 W1:W83 Y1:Y83 AA1:AA83 AC1:AC83 AE1:AE83 AG1:AG83 AI1:AI3 AK1:AK3 AM1:AM83 AO1:AO83 AQ1:AQ83 AS1:AS83 AU1:AU83 AW1:AW20 AY1:AY83 BA1:BA83 BC1:BC83 BE1:BE83 BG1:BG83 BI1:BI83 BK1:BK83 BM1:BM83 BO1:BO83 BQ1:BQ83 BS1:BS83 BU1:BU83 BW1:BW83 BY1:BY83 CA1:CA3 CC1:CC3 CE1:CE3 CG1:CG83 CI1:CI83 CK1:CK83 CM1:CM83 CO1:CO83 AK5:AK83 I6:I83 K6:K83 M6:M83 O6:O83 AI7:AI83 CA7:CA83 CC7:CC83 CE7:CE83 G21:G83 AW23:AW83 E50:E83" type="textLength">
+    <dataValidation allowBlank="true" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C83 E1:E3 G1:G3 I1:I3 K1:K3 M1:M3 O1:O3 Q1:Q83 S1:S83 U1:U83 W1:W83 Y1:Y83 AA1:AA83 AC1:AC83 AE1:AE83 AG1:AG83 AI1:AI3 AK1:AK3 AM1:AM83 AO1:AO83 AQ1:AQ83 AS1:AS83 AU1:AU83 AW1:AW21 AY1:AY83 BA1:BA83 BC1:BC83 BE1:BE83 BG1:BG83 BI1:BI83 BK1:BK83 BM1:BM83 BO1:BO83 BQ1:BQ83 BS1:BS3 BU1:BU83 BW1:BW83 BY1:BY83 CA1:CA3 CC1:CC3 CE1:CE3 CG1:CG83 CI1:CI83 CK1:CK83 CM1:CM83 CO1:CO83 AK5:AK83 BS5:BS83 I6:I83 K6:K83 M6:M83 O6:O83 AI7:AI83 CA7:CA83 CC7:CC83 CE7:CE83 G21:G83 AW24:AW83 E50:E83" type="textLength">
       <formula1>20</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>